<commit_message>
added the form for aeps in xml format odk
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="521">
   <si>
     <t>type</t>
   </si>
@@ -1534,6 +1534,57 @@
   </si>
   <si>
     <t>(regex(., '[a-zA-Z0-9._%-]+@[a-zA-Z0-9.-]+\.[a-zA-Z]{2,4}'))</t>
+  </si>
+  <si>
+    <t>pulldata('people','name', 'document_key', ${assistant_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','last_name', 'document_key', ${assistant_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','cellphone', 'document_key', ${assistant_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','sex', 'document_key', ${assistant_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','country', 'document_key', ${assistant_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','address', 'document_key', ${assistant_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','email', 'document_key', ${assistant_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','name', 'document_key', ${farmer_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','last_name', 'document_key', ${farmer_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','cellphone', 'document_key', ${farmer_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','sex', 'document_key', ${farmer_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','country', 'document_key', ${farmer_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','address', 'document_key', ${farmer_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('people','email', 'document_key', ${farmer_document_number})</t>
+  </si>
+  <si>
+    <t>pulldata('farm','name', 'farm_key', ${farm_id})</t>
+  </si>
+  <si>
+    <t>pulldata('farm','comments', 'farm_key', ${farm_id})</t>
+  </si>
+  <si>
+    <t>int(pulldata('farm','owner', 'farm_key', ${farm_id}))</t>
   </si>
 </sst>
 </file>
@@ -1942,8 +1993,8 @@
   <dimension ref="A1:L201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2074,6 +2125,9 @@
       <c r="H6" t="s">
         <v>26</v>
       </c>
+      <c r="J6" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2094,6 +2148,9 @@
       <c r="H7" t="s">
         <v>29</v>
       </c>
+      <c r="J7" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2114,6 +2171,9 @@
       <c r="H8" t="s">
         <v>32</v>
       </c>
+      <c r="J8" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2128,6 +2188,9 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
+      <c r="J9" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2145,8 +2208,8 @@
       <c r="F10" t="s">
         <v>37</v>
       </c>
-      <c r="K10" t="s">
-        <v>17</v>
+      <c r="J10" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -2202,6 +2265,9 @@
       <c r="E13" t="s">
         <v>14</v>
       </c>
+      <c r="J13" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2222,6 +2288,9 @@
       <c r="H14" t="s">
         <v>44</v>
       </c>
+      <c r="J14" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2292,6 +2361,9 @@
       <c r="H20" t="s">
         <v>26</v>
       </c>
+      <c r="J20" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -2312,6 +2384,9 @@
       <c r="H21" t="s">
         <v>29</v>
       </c>
+      <c r="J21" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -2332,6 +2407,9 @@
       <c r="H22" t="s">
         <v>32</v>
       </c>
+      <c r="J22" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -2349,6 +2427,9 @@
       <c r="F23" t="s">
         <v>18</v>
       </c>
+      <c r="J23" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -2366,8 +2447,8 @@
       <c r="F24" t="s">
         <v>37</v>
       </c>
-      <c r="K24" t="s">
-        <v>17</v>
+      <c r="J24" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -2423,6 +2504,9 @@
       <c r="E27" t="s">
         <v>14</v>
       </c>
+      <c r="J27" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -2443,6 +2527,9 @@
       <c r="H28" t="s">
         <v>44</v>
       </c>
+      <c r="J28" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -2484,6 +2571,9 @@
       <c r="E33" t="s">
         <v>14</v>
       </c>
+      <c r="J33" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -2512,6 +2602,9 @@
       <c r="C35" t="s">
         <v>69</v>
       </c>
+      <c r="J35" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -2529,6 +2622,9 @@
       <c r="F36" t="s">
         <v>18</v>
       </c>
+      <c r="J36" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -4584,6 +4680,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed the constrains in the dates fields in odk
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -17,12 +17,15 @@
     <sheet name="warnings" sheetId="4" r:id="rId3"/>
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$201</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="524">
   <si>
     <t>type</t>
   </si>
@@ -1585,6 +1588,15 @@
   </si>
   <si>
     <t>int(pulldata('farm','owner', 'farm_key', ${farm_id}))</t>
+  </si>
+  <si>
+    <t>(decimal-date-time(.) &gt; decimal-date-time(${planting_date}))</t>
+  </si>
+  <si>
+    <t>(decimal-date-time(.) &gt; decimal-date-time(${emergency_date}))</t>
+  </si>
+  <si>
+    <t>(decimal-date-time(.) &gt; decimal-date-time(${transfer_date}))</t>
   </si>
 </sst>
 </file>
@@ -1993,8 +2005,8 @@
   <dimension ref="A1:L201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2969,9 +2981,6 @@
       <c r="C60" t="s">
         <v>120</v>
       </c>
-      <c r="D60" t="s">
-        <v>17</v>
-      </c>
       <c r="E60" t="s">
         <v>14</v>
       </c>
@@ -3080,6 +3089,9 @@
       <c r="E70" t="s">
         <v>14</v>
       </c>
+      <c r="G70" t="s">
+        <v>521</v>
+      </c>
       <c r="H70" t="s">
         <v>134</v>
       </c>
@@ -3156,6 +3168,9 @@
       <c r="E75" t="s">
         <v>14</v>
       </c>
+      <c r="G75" t="s">
+        <v>521</v>
+      </c>
       <c r="H75" t="s">
         <v>144</v>
       </c>
@@ -3173,6 +3188,9 @@
       <c r="E76" t="s">
         <v>14</v>
       </c>
+      <c r="G76" t="s">
+        <v>522</v>
+      </c>
       <c r="H76" t="s">
         <v>147</v>
       </c>
@@ -3393,6 +3411,9 @@
       <c r="E95" t="s">
         <v>14</v>
       </c>
+      <c r="G95" t="s">
+        <v>521</v>
+      </c>
       <c r="H95" t="s">
         <v>176</v>
       </c>
@@ -3638,6 +3659,9 @@
       <c r="E115" t="s">
         <v>14</v>
       </c>
+      <c r="G115" t="s">
+        <v>521</v>
+      </c>
       <c r="H115" t="s">
         <v>176</v>
       </c>
@@ -3814,6 +3838,9 @@
       <c r="E129" t="s">
         <v>14</v>
       </c>
+      <c r="G129" t="s">
+        <v>521</v>
+      </c>
       <c r="H129" t="s">
         <v>176</v>
       </c>
@@ -3970,6 +3997,9 @@
       <c r="E142" t="s">
         <v>14</v>
       </c>
+      <c r="G142" t="s">
+        <v>521</v>
+      </c>
       <c r="H142" t="s">
         <v>176</v>
       </c>
@@ -4126,6 +4156,9 @@
       <c r="E155" t="s">
         <v>14</v>
       </c>
+      <c r="G155" t="s">
+        <v>521</v>
+      </c>
       <c r="H155" t="s">
         <v>176</v>
       </c>
@@ -4252,6 +4285,9 @@
       <c r="E169" t="s">
         <v>14</v>
       </c>
+      <c r="G169" t="s">
+        <v>521</v>
+      </c>
       <c r="H169" t="s">
         <v>266</v>
       </c>
@@ -4617,6 +4653,9 @@
       </c>
       <c r="E194" t="s">
         <v>14</v>
+      </c>
+      <c r="G194" t="s">
+        <v>523</v>
       </c>
       <c r="H194" t="s">
         <v>311</v>

</xml_diff>

<commit_message>
chenged the way how the form reads data for the farm in odk
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$201</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$202</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="532">
   <si>
     <t>type</t>
   </si>
@@ -222,12 +222,6 @@
     <t>geopoint</t>
   </si>
   <si>
-    <t>farm_location</t>
-  </si>
-  <si>
-    <t>Ubicación de la finca</t>
-  </si>
-  <si>
     <t>placement-map</t>
   </si>
   <si>
@@ -1597,6 +1591,36 @@
   </si>
   <si>
     <t>(decimal-date-time(.) &gt; decimal-date-time(${transfer_date}))</t>
+  </si>
+  <si>
+    <t>farm_location_lat</t>
+  </si>
+  <si>
+    <t>farm_location_lon</t>
+  </si>
+  <si>
+    <t>Latitud de la finca</t>
+  </si>
+  <si>
+    <t>Longitud de la finca</t>
+  </si>
+  <si>
+    <t>number(pulldata('farm','lat', 'farm_key', ${farm_id}))</t>
+  </si>
+  <si>
+    <t>number(pulldata('farm','lon', 'farm_key', ${farm_id}))</t>
+  </si>
+  <si>
+    <t>(. &gt;= -90) and (. &lt;= 90)</t>
+  </si>
+  <si>
+    <t>(. &gt;= -180) and (. &lt;= 180)</t>
+  </si>
+  <si>
+    <t>La latitud debe ser un campo numérico entre -90 y 90</t>
+  </si>
+  <si>
+    <t>La longitud debe ser un campo numérico entre -180 y 180</t>
   </si>
 </sst>
 </file>
@@ -2002,11 +2026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L201"/>
+  <dimension ref="A1:L202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2023,10 +2047,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2038,7 +2062,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2066,7 +2090,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2080,7 +2104,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2132,13 +2156,13 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2155,13 +2179,13 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H7" t="s">
         <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2178,18 +2202,18 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -2201,12 +2225,12 @@
         <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
@@ -2221,15 +2245,15 @@
         <v>37</v>
       </c>
       <c r="J10" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B11" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -2241,15 +2265,15 @@
         <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
@@ -2261,7 +2285,7 @@
         <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2278,7 +2302,7 @@
         <v>14</v>
       </c>
       <c r="J13" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2295,13 +2319,13 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H14" t="s">
         <v>44</v>
       </c>
       <c r="J14" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2322,7 +2346,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
@@ -2368,13 +2392,13 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2391,13 +2415,13 @@
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H21" t="s">
         <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2414,18 +2438,18 @@
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
       </c>
       <c r="J22" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
@@ -2440,12 +2464,12 @@
         <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -2460,15 +2484,15 @@
         <v>37</v>
       </c>
       <c r="J24" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -2480,15 +2504,15 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B26" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
@@ -2500,7 +2524,7 @@
         <v>18</v>
       </c>
       <c r="K26" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -2517,7 +2541,7 @@
         <v>14</v>
       </c>
       <c r="J27" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -2534,13 +2558,13 @@
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H28" t="s">
         <v>44</v>
       </c>
       <c r="J28" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -2584,119 +2608,128 @@
         <v>14</v>
       </c>
       <c r="J33" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>522</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>524</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
       </c>
-      <c r="L34" t="s">
-        <v>67</v>
+      <c r="G34" t="s">
+        <v>528</v>
+      </c>
+      <c r="H34" t="s">
+        <v>530</v>
+      </c>
+      <c r="J34" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>523</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>525</v>
+      </c>
+      <c r="E35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>529</v>
+      </c>
+      <c r="H35" t="s">
+        <v>531</v>
       </c>
       <c r="J35" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>423</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
-      </c>
-      <c r="E36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="J36" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>421</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="E41" t="s">
         <v>14</v>
-      </c>
-      <c r="L41" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
@@ -2704,200 +2737,200 @@
       <c r="E42" t="s">
         <v>14</v>
       </c>
-      <c r="G42" t="s">
-        <v>425</v>
-      </c>
-      <c r="H42" t="s">
-        <v>80</v>
+      <c r="L42" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" t="s">
+        <v>423</v>
+      </c>
+      <c r="H43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>462</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>460</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
       </c>
-      <c r="I47" t="s">
-        <v>480</v>
+      <c r="F47" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>463</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
       </c>
-      <c r="F48" t="s">
-        <v>85</v>
+      <c r="I48" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
+      </c>
+      <c r="F49" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>462</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
-      </c>
-      <c r="I50" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>430</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
       </c>
-      <c r="F51" t="s">
-        <v>96</v>
+      <c r="I51" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>428</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E52" t="s">
         <v>14</v>
       </c>
-      <c r="G52" t="s">
-        <v>431</v>
-      </c>
-      <c r="H52" t="s">
-        <v>99</v>
+      <c r="F52" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>430</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E53" t="s">
         <v>14</v>
       </c>
-      <c r="F53" t="s">
-        <v>102</v>
+      <c r="G53" t="s">
+        <v>429</v>
+      </c>
+      <c r="H53" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>428</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C54" t="s">
-        <v>104</v>
-      </c>
-      <c r="I54" t="s">
-        <v>479</v>
+        <v>99</v>
+      </c>
+      <c r="E54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>106</v>
-      </c>
-      <c r="E55" t="s">
-        <v>14</v>
-      </c>
-      <c r="G55" t="s">
-        <v>431</v>
-      </c>
-      <c r="H55" t="s">
-        <v>107</v>
+        <v>102</v>
+      </c>
+      <c r="I55" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2905,19 +2938,19 @@
         <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
       </c>
       <c r="G56" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H56" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -2925,75 +2958,90 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H57" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>430</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E58" t="s">
         <v>14</v>
       </c>
-      <c r="F58" t="s">
-        <v>102</v>
+      <c r="G58" t="s">
+        <v>429</v>
+      </c>
+      <c r="H58" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>428</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
-      </c>
-      <c r="I59" t="s">
-        <v>482</v>
+        <v>113</v>
+      </c>
+      <c r="E59" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C60" t="s">
-        <v>120</v>
-      </c>
-      <c r="E60" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" t="s">
-        <v>432</v>
-      </c>
-      <c r="H60" t="s">
-        <v>433</v>
+        <v>115</v>
+      </c>
+      <c r="I60" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>116</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="s">
+        <v>430</v>
+      </c>
+      <c r="H61" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -3006,263 +3054,263 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>9</v>
-      </c>
-      <c r="B65" t="s">
-        <v>121</v>
-      </c>
-      <c r="C65" t="s">
-        <v>122</v>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C66" t="s">
-        <v>125</v>
-      </c>
-      <c r="E66" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>465</v>
+        <v>121</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C67" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E67" t="s">
         <v>14</v>
-      </c>
-      <c r="F67" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>463</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
-      </c>
-      <c r="I68" t="s">
-        <v>483</v>
+        <v>125</v>
+      </c>
+      <c r="E68" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>466</v>
+        <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C69" t="s">
-        <v>131</v>
-      </c>
-      <c r="E69" t="s">
-        <v>14</v>
+        <v>127</v>
+      </c>
+      <c r="I69" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>123</v>
+        <v>464</v>
       </c>
       <c r="B70" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C70" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E70" t="s">
         <v>14</v>
-      </c>
-      <c r="G70" t="s">
-        <v>521</v>
-      </c>
-      <c r="H70" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>45</v>
+        <v>121</v>
+      </c>
+      <c r="B71" t="s">
+        <v>130</v>
+      </c>
+      <c r="C71" t="s">
+        <v>131</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" t="s">
+        <v>519</v>
+      </c>
+      <c r="H71" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" t="s">
-        <v>135</v>
-      </c>
-      <c r="C72" t="s">
-        <v>136</v>
-      </c>
-      <c r="D72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E72" t="s">
-        <v>14</v>
-      </c>
-      <c r="G72" t="s">
-        <v>431</v>
-      </c>
-      <c r="H72" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>430</v>
+        <v>59</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C73" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+      <c r="D73" t="s">
+        <v>17</v>
       </c>
       <c r="E73" t="s">
         <v>14</v>
       </c>
-      <c r="F73" t="s">
-        <v>102</v>
+      <c r="G73" t="s">
+        <v>429</v>
+      </c>
+      <c r="H73" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>428</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C74" t="s">
-        <v>141</v>
-      </c>
-      <c r="I74" t="s">
-        <v>484</v>
+        <v>137</v>
+      </c>
+      <c r="E74" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C75" t="s">
-        <v>143</v>
-      </c>
-      <c r="E75" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" t="s">
-        <v>521</v>
-      </c>
-      <c r="H75" t="s">
-        <v>144</v>
+        <v>139</v>
+      </c>
+      <c r="I75" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C76" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
       </c>
       <c r="G76" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H76" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B77" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C77" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E77" t="s">
         <v>14</v>
+      </c>
+      <c r="G77" t="s">
+        <v>520</v>
+      </c>
+      <c r="H77" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>430</v>
+        <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C78" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E78" t="s">
         <v>14</v>
-      </c>
-      <c r="F78" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>428</v>
       </c>
       <c r="B79" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C79" t="s">
-        <v>153</v>
-      </c>
-      <c r="I79" t="s">
-        <v>485</v>
+        <v>149</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C80" t="s">
-        <v>155</v>
-      </c>
-      <c r="E80" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" t="s">
-        <v>432</v>
-      </c>
-      <c r="H80" t="s">
-        <v>156</v>
+        <v>151</v>
+      </c>
+      <c r="I80" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>45</v>
+        <v>116</v>
+      </c>
+      <c r="B81" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" t="s">
+        <v>153</v>
+      </c>
+      <c r="E81" t="s">
+        <v>14</v>
+      </c>
+      <c r="G81" t="s">
+        <v>430</v>
+      </c>
+      <c r="H81" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -3275,186 +3323,177 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>9</v>
       </c>
-      <c r="B85" t="s">
-        <v>157</v>
-      </c>
-      <c r="C85" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>437</v>
-      </c>
-      <c r="B87" t="s">
-        <v>159</v>
-      </c>
-      <c r="C87" t="s">
-        <v>160</v>
-      </c>
-      <c r="E87" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" t="s">
-        <v>18</v>
+      <c r="B86" t="s">
+        <v>155</v>
+      </c>
+      <c r="C86" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>435</v>
       </c>
       <c r="B88" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C88" t="s">
-        <v>163</v>
+        <v>158</v>
+      </c>
+      <c r="E88" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>439</v>
+        <v>159</v>
       </c>
       <c r="B89" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C89" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>437</v>
       </c>
       <c r="B90" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C90" t="s">
-        <v>167</v>
-      </c>
-      <c r="I90" t="s">
-        <v>486</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C91" t="s">
-        <v>169</v>
-      </c>
-      <c r="E91" t="s">
-        <v>14</v>
-      </c>
-      <c r="G91" t="s">
-        <v>431</v>
-      </c>
-      <c r="H91" t="s">
-        <v>170</v>
+        <v>165</v>
+      </c>
+      <c r="I91" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="B92" t="s">
+        <v>166</v>
+      </c>
+      <c r="C92" t="s">
+        <v>167</v>
+      </c>
+      <c r="E92" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" t="s">
+        <v>429</v>
+      </c>
+      <c r="H92" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>9</v>
-      </c>
-      <c r="B93" t="s">
-        <v>171</v>
-      </c>
-      <c r="C93" t="s">
-        <v>172</v>
-      </c>
-      <c r="I93" t="s">
-        <v>487</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C94" t="s">
-        <v>169</v>
-      </c>
-      <c r="E94" t="s">
-        <v>14</v>
-      </c>
-      <c r="G94" t="s">
-        <v>431</v>
-      </c>
-      <c r="H94" t="s">
         <v>170</v>
+      </c>
+      <c r="I94" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B95" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C95" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E95" t="s">
         <v>14</v>
       </c>
       <c r="G95" t="s">
-        <v>521</v>
+        <v>429</v>
       </c>
       <c r="H95" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="B96" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C96" t="s">
-        <v>178</v>
-      </c>
-      <c r="I96" t="s">
-        <v>486</v>
+        <v>173</v>
+      </c>
+      <c r="E96" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" t="s">
+        <v>519</v>
+      </c>
+      <c r="H96" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C97" t="s">
-        <v>180</v>
-      </c>
-      <c r="E97" t="s">
-        <v>14</v>
+        <v>176</v>
+      </c>
+      <c r="I97" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B98" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C98" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -3465,10 +3504,10 @@
         <v>59</v>
       </c>
       <c r="B99" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C99" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
@@ -3479,10 +3518,10 @@
         <v>59</v>
       </c>
       <c r="B100" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C100" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E100" t="s">
         <v>14</v>
@@ -3490,1010 +3529,1004 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="B101" t="s">
+        <v>183</v>
+      </c>
+      <c r="C101" t="s">
+        <v>184</v>
+      </c>
+      <c r="E101" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>467</v>
-      </c>
-      <c r="B102" t="s">
-        <v>187</v>
-      </c>
-      <c r="C102" t="s">
-        <v>188</v>
-      </c>
-      <c r="E102" t="s">
-        <v>14</v>
-      </c>
-      <c r="F102" t="s">
-        <v>18</v>
-      </c>
-      <c r="I102" t="s">
-        <v>487</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>19</v>
+        <v>465</v>
       </c>
       <c r="B103" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C103" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="E103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" t="s">
+        <v>18</v>
+      </c>
+      <c r="I103" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="B104" t="s">
+        <v>187</v>
+      </c>
+      <c r="C104" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>437</v>
-      </c>
-      <c r="B107" t="s">
-        <v>192</v>
-      </c>
-      <c r="C107" t="s">
-        <v>193</v>
-      </c>
-      <c r="E107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F107" t="s">
-        <v>18</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>161</v>
+        <v>435</v>
       </c>
       <c r="B108" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C108" t="s">
-        <v>195</v>
+        <v>191</v>
+      </c>
+      <c r="E108" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>441</v>
+        <v>159</v>
       </c>
       <c r="B109" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C109" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>9</v>
+        <v>439</v>
       </c>
       <c r="B110" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C110" t="s">
-        <v>199</v>
-      </c>
-      <c r="I110" t="s">
-        <v>488</v>
+        <v>195</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B111" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C111" t="s">
-        <v>201</v>
-      </c>
-      <c r="E111" t="s">
-        <v>14</v>
-      </c>
-      <c r="G111" t="s">
-        <v>431</v>
-      </c>
-      <c r="H111" t="s">
-        <v>170</v>
+        <v>197</v>
+      </c>
+      <c r="I111" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="B112" t="s">
+        <v>198</v>
+      </c>
+      <c r="C112" t="s">
+        <v>199</v>
+      </c>
+      <c r="E112" t="s">
+        <v>14</v>
+      </c>
+      <c r="G112" t="s">
+        <v>429</v>
+      </c>
+      <c r="H112" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>9</v>
-      </c>
-      <c r="B113" t="s">
-        <v>202</v>
-      </c>
-      <c r="C113" t="s">
-        <v>203</v>
-      </c>
-      <c r="I113" t="s">
-        <v>489</v>
+        <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B114" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C114" t="s">
         <v>201</v>
       </c>
-      <c r="E114" t="s">
-        <v>14</v>
-      </c>
-      <c r="G114" t="s">
-        <v>431</v>
-      </c>
-      <c r="H114" t="s">
-        <v>170</v>
+      <c r="I114" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B115" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C115" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="E115" t="s">
         <v>14</v>
       </c>
       <c r="G115" t="s">
-        <v>521</v>
+        <v>429</v>
       </c>
       <c r="H115" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>444</v>
+        <v>121</v>
       </c>
       <c r="B116" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C116" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="E116" t="s">
         <v>14</v>
       </c>
-      <c r="F116" t="s">
-        <v>18</v>
-      </c>
-      <c r="I116" t="s">
-        <v>490</v>
+      <c r="G116" t="s">
+        <v>519</v>
+      </c>
+      <c r="H116" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>19</v>
+        <v>442</v>
       </c>
       <c r="B117" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C117" t="s">
-        <v>190</v>
+        <v>205</v>
+      </c>
+      <c r="E117" t="s">
+        <v>14</v>
+      </c>
+      <c r="F117" t="s">
+        <v>18</v>
+      </c>
+      <c r="I117" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="B118" t="s">
+        <v>206</v>
+      </c>
+      <c r="C118" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>437</v>
-      </c>
-      <c r="B121" t="s">
-        <v>209</v>
-      </c>
-      <c r="C121" t="s">
-        <v>210</v>
-      </c>
-      <c r="E121" t="s">
-        <v>14</v>
-      </c>
-      <c r="F121" t="s">
-        <v>18</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>161</v>
+        <v>435</v>
       </c>
       <c r="B122" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C122" t="s">
-        <v>212</v>
+        <v>208</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
+      </c>
+      <c r="F122" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>446</v>
+        <v>159</v>
       </c>
       <c r="B123" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C123" t="s">
-        <v>214</v>
-      </c>
-      <c r="E123" t="s">
-        <v>14</v>
-      </c>
-      <c r="F123" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>9</v>
+        <v>444</v>
       </c>
       <c r="B124" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C124" t="s">
-        <v>216</v>
-      </c>
-      <c r="I124" t="s">
-        <v>491</v>
+        <v>212</v>
+      </c>
+      <c r="E124" t="s">
+        <v>14</v>
+      </c>
+      <c r="F124" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C125" t="s">
-        <v>218</v>
-      </c>
-      <c r="E125" t="s">
-        <v>14</v>
-      </c>
-      <c r="G125" t="s">
-        <v>431</v>
-      </c>
-      <c r="H125" t="s">
-        <v>170</v>
+        <v>214</v>
+      </c>
+      <c r="I125" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="B126" t="s">
+        <v>215</v>
+      </c>
+      <c r="C126" t="s">
+        <v>216</v>
+      </c>
+      <c r="E126" t="s">
+        <v>14</v>
+      </c>
+      <c r="G126" t="s">
+        <v>429</v>
+      </c>
+      <c r="H126" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>9</v>
-      </c>
-      <c r="B127" t="s">
-        <v>219</v>
-      </c>
-      <c r="C127" t="s">
-        <v>220</v>
-      </c>
-      <c r="I127" t="s">
-        <v>492</v>
+        <v>45</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B128" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C128" t="s">
         <v>218</v>
       </c>
-      <c r="E128" t="s">
-        <v>14</v>
-      </c>
-      <c r="G128" t="s">
-        <v>431</v>
-      </c>
-      <c r="H128" t="s">
-        <v>170</v>
+      <c r="I128" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B129" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C129" t="s">
-        <v>175</v>
+        <v>216</v>
       </c>
       <c r="E129" t="s">
         <v>14</v>
       </c>
       <c r="G129" t="s">
-        <v>521</v>
+        <v>429</v>
       </c>
       <c r="H129" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B130" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C130" t="s">
-        <v>190</v>
+        <v>173</v>
+      </c>
+      <c r="E130" t="s">
+        <v>14</v>
+      </c>
+      <c r="G130" t="s">
+        <v>519</v>
+      </c>
+      <c r="H130" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="B131" t="s">
+        <v>221</v>
+      </c>
+      <c r="C131" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>437</v>
-      </c>
-      <c r="B134" t="s">
-        <v>224</v>
-      </c>
-      <c r="C134" t="s">
-        <v>225</v>
-      </c>
-      <c r="E134" t="s">
-        <v>14</v>
-      </c>
-      <c r="F134" t="s">
-        <v>18</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>161</v>
+        <v>435</v>
       </c>
       <c r="B135" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C135" t="s">
-        <v>227</v>
+        <v>223</v>
+      </c>
+      <c r="E135" t="s">
+        <v>14</v>
+      </c>
+      <c r="F135" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>448</v>
+        <v>159</v>
       </c>
       <c r="B136" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C136" t="s">
-        <v>229</v>
-      </c>
-      <c r="E136" t="s">
-        <v>14</v>
-      </c>
-      <c r="F136" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>9</v>
+        <v>446</v>
       </c>
       <c r="B137" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C137" t="s">
-        <v>231</v>
-      </c>
-      <c r="I137" t="s">
-        <v>493</v>
+        <v>227</v>
+      </c>
+      <c r="E137" t="s">
+        <v>14</v>
+      </c>
+      <c r="F137" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B138" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C138" t="s">
-        <v>233</v>
-      </c>
-      <c r="E138" t="s">
-        <v>14</v>
-      </c>
-      <c r="G138" t="s">
-        <v>431</v>
-      </c>
-      <c r="H138" t="s">
-        <v>170</v>
+        <v>229</v>
+      </c>
+      <c r="I138" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="B139" t="s">
+        <v>230</v>
+      </c>
+      <c r="C139" t="s">
+        <v>231</v>
+      </c>
+      <c r="E139" t="s">
+        <v>14</v>
+      </c>
+      <c r="G139" t="s">
+        <v>429</v>
+      </c>
+      <c r="H139" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>9</v>
-      </c>
-      <c r="B140" t="s">
-        <v>234</v>
-      </c>
-      <c r="C140" t="s">
-        <v>235</v>
-      </c>
-      <c r="I140" t="s">
-        <v>494</v>
+        <v>45</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B141" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C141" t="s">
         <v>233</v>
       </c>
-      <c r="E141" t="s">
-        <v>14</v>
-      </c>
-      <c r="G141" t="s">
-        <v>431</v>
-      </c>
-      <c r="H141" t="s">
-        <v>170</v>
+      <c r="I141" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B142" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C142" t="s">
-        <v>175</v>
+        <v>231</v>
       </c>
       <c r="E142" t="s">
         <v>14</v>
       </c>
       <c r="G142" t="s">
-        <v>521</v>
+        <v>429</v>
       </c>
       <c r="H142" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B143" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C143" t="s">
-        <v>190</v>
+        <v>173</v>
+      </c>
+      <c r="E143" t="s">
+        <v>14</v>
+      </c>
+      <c r="G143" t="s">
+        <v>519</v>
+      </c>
+      <c r="H143" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="B144" t="s">
+        <v>236</v>
+      </c>
+      <c r="C144" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>437</v>
-      </c>
-      <c r="B147" t="s">
-        <v>239</v>
-      </c>
-      <c r="C147" t="s">
-        <v>240</v>
-      </c>
-      <c r="E147" t="s">
-        <v>14</v>
-      </c>
-      <c r="F147" t="s">
-        <v>18</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>161</v>
+        <v>435</v>
       </c>
       <c r="B148" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C148" t="s">
-        <v>242</v>
+        <v>238</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>448</v>
+        <v>159</v>
       </c>
       <c r="B149" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C149" t="s">
-        <v>244</v>
-      </c>
-      <c r="E149" t="s">
-        <v>14</v>
-      </c>
-      <c r="F149" t="s">
-        <v>18</v>
+        <v>240</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>9</v>
+        <v>446</v>
       </c>
       <c r="B150" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C150" t="s">
-        <v>246</v>
-      </c>
-      <c r="I150" t="s">
-        <v>495</v>
+        <v>242</v>
+      </c>
+      <c r="E150" t="s">
+        <v>14</v>
+      </c>
+      <c r="F150" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B151" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C151" t="s">
-        <v>248</v>
-      </c>
-      <c r="E151" t="s">
-        <v>14</v>
-      </c>
-      <c r="G151" t="s">
-        <v>431</v>
-      </c>
-      <c r="H151" t="s">
-        <v>170</v>
+        <v>244</v>
+      </c>
+      <c r="I151" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="B152" t="s">
+        <v>245</v>
+      </c>
+      <c r="C152" t="s">
+        <v>246</v>
+      </c>
+      <c r="E152" t="s">
+        <v>14</v>
+      </c>
+      <c r="G152" t="s">
+        <v>429</v>
+      </c>
+      <c r="H152" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>9</v>
-      </c>
-      <c r="B153" t="s">
-        <v>249</v>
-      </c>
-      <c r="C153" t="s">
-        <v>250</v>
-      </c>
-      <c r="I153" t="s">
-        <v>496</v>
+        <v>45</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B154" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C154" t="s">
         <v>248</v>
       </c>
-      <c r="E154" t="s">
-        <v>14</v>
-      </c>
-      <c r="G154" t="s">
-        <v>431</v>
-      </c>
-      <c r="H154" t="s">
-        <v>170</v>
+      <c r="I154" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B155" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C155" t="s">
-        <v>175</v>
+        <v>246</v>
       </c>
       <c r="E155" t="s">
         <v>14</v>
       </c>
       <c r="G155" t="s">
-        <v>521</v>
+        <v>429</v>
       </c>
       <c r="H155" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="B156" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C156" t="s">
-        <v>254</v>
+        <v>173</v>
+      </c>
+      <c r="E156" t="s">
+        <v>14</v>
+      </c>
+      <c r="G156" t="s">
+        <v>519</v>
+      </c>
+      <c r="H156" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>468</v>
+        <v>9</v>
       </c>
       <c r="B157" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C157" t="s">
-        <v>256</v>
-      </c>
-      <c r="E157" t="s">
-        <v>14</v>
-      </c>
-      <c r="F157" t="s">
-        <v>18</v>
-      </c>
-      <c r="I157" t="s">
-        <v>497</v>
+        <v>252</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>45</v>
+        <v>466</v>
+      </c>
+      <c r="B158" t="s">
+        <v>253</v>
+      </c>
+      <c r="C158" t="s">
+        <v>254</v>
+      </c>
+      <c r="E158" t="s">
+        <v>14</v>
+      </c>
+      <c r="F158" t="s">
+        <v>18</v>
+      </c>
+      <c r="I158" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>9</v>
-      </c>
-      <c r="B159" t="s">
-        <v>257</v>
-      </c>
-      <c r="C159" t="s">
-        <v>258</v>
-      </c>
-      <c r="I159" t="s">
-        <v>498</v>
+        <v>45</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>9</v>
+      </c>
+      <c r="B160" t="s">
+        <v>255</v>
+      </c>
+      <c r="C160" t="s">
+        <v>256</v>
+      </c>
+      <c r="I160" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>450</v>
+      </c>
+      <c r="B161" t="s">
+        <v>257</v>
+      </c>
+      <c r="C161" t="s">
+        <v>258</v>
+      </c>
+      <c r="E161" t="s">
+        <v>14</v>
+      </c>
+      <c r="F161" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>19</v>
+      </c>
+      <c r="B163" t="s">
+        <v>259</v>
+      </c>
+      <c r="C163" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>9</v>
+      </c>
+      <c r="B169" t="s">
+        <v>260</v>
+      </c>
+      <c r="C169" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>121</v>
+      </c>
+      <c r="B170" t="s">
+        <v>262</v>
+      </c>
+      <c r="C170" t="s">
+        <v>263</v>
+      </c>
+      <c r="E170" t="s">
+        <v>14</v>
+      </c>
+      <c r="G170" t="s">
+        <v>519</v>
+      </c>
+      <c r="H170" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
         <v>452</v>
       </c>
-      <c r="B160" t="s">
-        <v>259</v>
-      </c>
-      <c r="C160" t="s">
-        <v>260</v>
-      </c>
-      <c r="E160" t="s">
-        <v>14</v>
-      </c>
-      <c r="F160" t="s">
+      <c r="B171" t="s">
+        <v>265</v>
+      </c>
+      <c r="C171" t="s">
+        <v>266</v>
+      </c>
+      <c r="E171" t="s">
+        <v>14</v>
+      </c>
+      <c r="F171" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>19</v>
-      </c>
-      <c r="B162" t="s">
-        <v>261</v>
-      </c>
-      <c r="C162" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
-        <v>9</v>
-      </c>
-      <c r="B168" t="s">
-        <v>262</v>
-      </c>
-      <c r="C168" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
-        <v>123</v>
-      </c>
-      <c r="B169" t="s">
-        <v>264</v>
-      </c>
-      <c r="C169" t="s">
-        <v>265</v>
-      </c>
-      <c r="E169" t="s">
-        <v>14</v>
-      </c>
-      <c r="G169" t="s">
-        <v>521</v>
-      </c>
-      <c r="H169" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
-        <v>454</v>
-      </c>
-      <c r="B170" t="s">
-        <v>267</v>
-      </c>
-      <c r="C170" t="s">
-        <v>268</v>
-      </c>
-      <c r="E170" t="s">
-        <v>14</v>
-      </c>
-      <c r="F170" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
-        <v>59</v>
-      </c>
-      <c r="B171" t="s">
-        <v>269</v>
-      </c>
-      <c r="C171" t="s">
-        <v>270</v>
-      </c>
-      <c r="E171" t="s">
-        <v>14</v>
-      </c>
-      <c r="G171" t="s">
-        <v>431</v>
-      </c>
-      <c r="H171" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>59</v>
       </c>
       <c r="B172" t="s">
+        <v>267</v>
+      </c>
+      <c r="C172" t="s">
+        <v>268</v>
+      </c>
+      <c r="E172" t="s">
+        <v>14</v>
+      </c>
+      <c r="G172" t="s">
+        <v>429</v>
+      </c>
+      <c r="H172" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>59</v>
+      </c>
+      <c r="B173" t="s">
+        <v>270</v>
+      </c>
+      <c r="C173" t="s">
+        <v>271</v>
+      </c>
+      <c r="E173" t="s">
+        <v>14</v>
+      </c>
+      <c r="G173" t="s">
+        <v>429</v>
+      </c>
+      <c r="H173" t="s">
         <v>272</v>
       </c>
-      <c r="C172" t="s">
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>467</v>
+      </c>
+      <c r="B174" t="s">
         <v>273</v>
       </c>
-      <c r="E172" t="s">
-        <v>14</v>
-      </c>
-      <c r="G172" t="s">
-        <v>431</v>
-      </c>
-      <c r="H172" t="s">
+      <c r="C174" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
-        <v>469</v>
-      </c>
-      <c r="B173" t="s">
+      <c r="E174" t="s">
+        <v>14</v>
+      </c>
+      <c r="F174" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>59</v>
+      </c>
+      <c r="B175" t="s">
         <v>275</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C175" t="s">
         <v>276</v>
       </c>
-      <c r="E173" t="s">
-        <v>14</v>
-      </c>
-      <c r="F173" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
-        <v>59</v>
-      </c>
-      <c r="B174" t="s">
+      <c r="E175" t="s">
+        <v>14</v>
+      </c>
+      <c r="G175" t="s">
+        <v>429</v>
+      </c>
+      <c r="H175" t="s">
         <v>277</v>
       </c>
-      <c r="C174" t="s">
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>428</v>
+      </c>
+      <c r="B176" t="s">
         <v>278</v>
       </c>
-      <c r="E174" t="s">
-        <v>14</v>
-      </c>
-      <c r="G174" t="s">
-        <v>431</v>
-      </c>
-      <c r="H174" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
-        <v>430</v>
-      </c>
-      <c r="B175" t="s">
-        <v>280</v>
-      </c>
-      <c r="C175" t="s">
-        <v>101</v>
-      </c>
-      <c r="E175" t="s">
-        <v>14</v>
-      </c>
-      <c r="F175" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
-        <v>9</v>
-      </c>
-      <c r="B176" t="s">
-        <v>281</v>
-      </c>
       <c r="C176" t="s">
-        <v>282</v>
-      </c>
-      <c r="I176" t="s">
-        <v>499</v>
+        <v>99</v>
+      </c>
+      <c r="E176" t="s">
+        <v>14</v>
+      </c>
+      <c r="F176" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>458</v>
+        <v>9</v>
       </c>
       <c r="B177" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C177" t="s">
-        <v>284</v>
-      </c>
-      <c r="E177" t="s">
-        <v>14</v>
+        <v>280</v>
+      </c>
+      <c r="I177" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>430</v>
+        <v>456</v>
       </c>
       <c r="B178" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C178" t="s">
-        <v>115</v>
+        <v>282</v>
       </c>
       <c r="E178" t="s">
         <v>14</v>
-      </c>
-      <c r="F178" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>161</v>
+        <v>428</v>
       </c>
       <c r="B179" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C179" t="s">
-        <v>287</v>
-      </c>
-      <c r="I179" t="s">
-        <v>500</v>
+        <v>113</v>
+      </c>
+      <c r="E179" t="s">
+        <v>14</v>
+      </c>
+      <c r="F179" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>470</v>
+        <v>159</v>
       </c>
       <c r="B180" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C180" t="s">
-        <v>289</v>
-      </c>
-      <c r="E180" t="s">
-        <v>14</v>
+        <v>285</v>
+      </c>
+      <c r="I180" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>59</v>
+        <v>468</v>
       </c>
       <c r="B181" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C181" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E181" t="s">
         <v>14</v>
-      </c>
-      <c r="G181" t="s">
-        <v>431</v>
-      </c>
-      <c r="H181" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
@@ -4501,29 +4534,44 @@
         <v>59</v>
       </c>
       <c r="B182" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C182" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E182" t="s">
         <v>14</v>
       </c>
       <c r="G182" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H182" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>191</v>
+        <v>59</v>
+      </c>
+      <c r="B183" t="s">
+        <v>291</v>
+      </c>
+      <c r="C183" t="s">
+        <v>292</v>
+      </c>
+      <c r="E183" t="s">
+        <v>14</v>
+      </c>
+      <c r="G183" t="s">
+        <v>429</v>
+      </c>
+      <c r="H183" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
@@ -4531,180 +4579,180 @@
         <v>45</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
-        <v>9</v>
-      </c>
-      <c r="B187" t="s">
-        <v>296</v>
-      </c>
-      <c r="C187" t="s">
-        <v>297</v>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>430</v>
+        <v>9</v>
       </c>
       <c r="B188" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C188" t="s">
-        <v>299</v>
-      </c>
-      <c r="E188" t="s">
-        <v>14</v>
-      </c>
-      <c r="F188" t="s">
-        <v>96</v>
+        <v>295</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B189" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C189" t="s">
-        <v>101</v>
+        <v>297</v>
       </c>
       <c r="E189" t="s">
         <v>14</v>
       </c>
       <c r="F189" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>9</v>
+        <v>428</v>
       </c>
       <c r="B190" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C190" t="s">
-        <v>302</v>
-      </c>
-      <c r="I190" t="s">
-        <v>501</v>
+        <v>99</v>
+      </c>
+      <c r="E190" t="s">
+        <v>14</v>
+      </c>
+      <c r="F190" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B191" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C191" t="s">
-        <v>304</v>
-      </c>
-      <c r="E191" t="s">
-        <v>14</v>
-      </c>
-      <c r="G191" t="s">
-        <v>431</v>
-      </c>
-      <c r="H191" t="s">
-        <v>305</v>
+        <v>300</v>
+      </c>
+      <c r="I191" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>430</v>
+        <v>59</v>
       </c>
       <c r="B192" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C192" t="s">
-        <v>115</v>
+        <v>302</v>
       </c>
       <c r="E192" t="s">
         <v>14</v>
       </c>
-      <c r="F192" t="s">
-        <v>102</v>
+      <c r="G192" t="s">
+        <v>429</v>
+      </c>
+      <c r="H192" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>9</v>
+        <v>428</v>
       </c>
       <c r="B193" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C193" t="s">
-        <v>308</v>
-      </c>
-      <c r="I193" t="s">
-        <v>502</v>
+        <v>113</v>
+      </c>
+      <c r="E193" t="s">
+        <v>14</v>
+      </c>
+      <c r="F193" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="B194" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C194" t="s">
-        <v>310</v>
-      </c>
-      <c r="E194" t="s">
-        <v>14</v>
-      </c>
-      <c r="G194" t="s">
-        <v>523</v>
-      </c>
-      <c r="H194" t="s">
-        <v>311</v>
+        <v>306</v>
+      </c>
+      <c r="I194" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="B195" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C195" t="s">
-        <v>313</v>
+        <v>308</v>
+      </c>
+      <c r="E195" t="s">
+        <v>14</v>
+      </c>
+      <c r="G195" t="s">
+        <v>521</v>
+      </c>
+      <c r="H195" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="B196" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C196" t="s">
-        <v>315</v>
-      </c>
-      <c r="E196" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B197" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C197" t="s">
-        <v>317</v>
+        <v>313</v>
+      </c>
+      <c r="E197" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>191</v>
+        <v>19</v>
+      </c>
+      <c r="B198" t="s">
+        <v>314</v>
+      </c>
+      <c r="C198" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
@@ -4714,6 +4762,11 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4729,7 +4782,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4739,635 +4792,635 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C14" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C17" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C18" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C19" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B22" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C22" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B23" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C23" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B24" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C24" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C27" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C28" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B29" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C29" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B32" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B33" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C33" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B34" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C34" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B35" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C35" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B36" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C36" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B37" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C37" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B40" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C40" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B41" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C41" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B42" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C42" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B43" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C43" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B44" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C44" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B45" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C45" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B48" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C48" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B49" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C49" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B50" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C50" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C52" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B53" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C53" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B56" t="s">
         <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D57" t="s">
         <v>37</v>
@@ -5375,7 +5428,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -5392,354 +5445,354 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C60" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B61" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C61" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B63" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C63" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
       </c>
       <c r="C64" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B66" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C66" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B67" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C67" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B68" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C68" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B69" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C69" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B70" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C70" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B71" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C71" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B72" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C72" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B73" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C73" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B74" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C74" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B77" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C77" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B78" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C78" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B80" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C80" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C82" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B83" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C83" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B84" t="s">
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B86" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C86" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B87" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C87" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B88" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C88" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B89" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C89" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B90" t="s">
         <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -5757,7 +5810,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -5771,7 +5824,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5781,30 +5834,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1" t="s">
         <v>397</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>398</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>399</v>
       </c>
-      <c r="D1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E1" t="s">
-        <v>401</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B2" t="s">
         <v>402</v>
-      </c>
-      <c r="B2" t="s">
-        <v>404</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -5813,7 +5866,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F2" s="1">
         <v>201807</v>

</xml_diff>

<commit_message>
deleted the field amount in advanced in  agronomy practice
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$202</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$201</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="531">
   <si>
     <t>type</t>
   </si>
@@ -538,9 +538,6 @@
   </si>
   <si>
     <t>Información avanzada de fertilización</t>
-  </si>
-  <si>
-    <t>fertilization_type_count_advanced</t>
   </si>
   <si>
     <t>fertilization_date_advanced</t>
@@ -2026,11 +2023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L202"/>
+  <dimension ref="A1:L201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2047,10 +2044,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D1" t="s">
         <v>405</v>
-      </c>
-      <c r="D1" t="s">
-        <v>406</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2062,7 +2059,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2090,7 +2087,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2104,7 +2101,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2156,13 +2153,13 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2179,13 +2176,13 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H7" t="s">
         <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2202,18 +2199,18 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -2225,12 +2222,12 @@
         <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
@@ -2245,15 +2242,15 @@
         <v>37</v>
       </c>
       <c r="J10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -2265,15 +2262,15 @@
         <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
@@ -2285,7 +2282,7 @@
         <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2302,7 +2299,7 @@
         <v>14</v>
       </c>
       <c r="J13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2319,13 +2316,13 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H14" t="s">
         <v>44</v>
       </c>
       <c r="J14" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2346,7 +2343,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
@@ -2392,13 +2389,13 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2415,13 +2412,13 @@
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H21" t="s">
         <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2438,18 +2435,18 @@
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
       </c>
       <c r="J22" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
@@ -2464,12 +2461,12 @@
         <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -2484,15 +2481,15 @@
         <v>37</v>
       </c>
       <c r="J24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -2504,15 +2501,15 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B26" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
@@ -2524,7 +2521,7 @@
         <v>18</v>
       </c>
       <c r="K26" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -2541,7 +2538,7 @@
         <v>14</v>
       </c>
       <c r="J27" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -2558,13 +2555,13 @@
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H28" t="s">
         <v>44</v>
       </c>
       <c r="J28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -2608,7 +2605,7 @@
         <v>14</v>
       </c>
       <c r="J33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2616,22 +2613,22 @@
         <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C34" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
       </c>
       <c r="G34" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H34" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J34" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2639,22 +2636,22 @@
         <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C35" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E35" t="s">
         <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H35" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J35" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2668,12 +2665,12 @@
         <v>67</v>
       </c>
       <c r="J36" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B37" t="s">
         <v>68</v>
@@ -2688,7 +2685,7 @@
         <v>18</v>
       </c>
       <c r="J37" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2758,7 +2755,7 @@
         <v>14</v>
       </c>
       <c r="G43" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H43" t="s">
         <v>78</v>
@@ -2782,7 +2779,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B47" t="s">
         <v>81</v>
@@ -2814,12 +2811,12 @@
         <v>14</v>
       </c>
       <c r="I48" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B49" t="s">
         <v>86</v>
@@ -2836,7 +2833,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B50" t="s">
         <v>88</v>
@@ -2862,12 +2859,12 @@
         <v>14</v>
       </c>
       <c r="I51" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B52" t="s">
         <v>92</v>
@@ -2896,7 +2893,7 @@
         <v>14</v>
       </c>
       <c r="G53" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H53" t="s">
         <v>97</v>
@@ -2904,7 +2901,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B54" t="s">
         <v>98</v>
@@ -2930,7 +2927,7 @@
         <v>102</v>
       </c>
       <c r="I55" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2947,7 +2944,7 @@
         <v>14</v>
       </c>
       <c r="G56" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H56" t="s">
         <v>105</v>
@@ -2967,7 +2964,7 @@
         <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H57" t="s">
         <v>108</v>
@@ -2987,7 +2984,7 @@
         <v>14</v>
       </c>
       <c r="G58" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H58" t="s">
         <v>111</v>
@@ -2995,7 +2992,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B59" t="s">
         <v>112</v>
@@ -3021,7 +3018,7 @@
         <v>115</v>
       </c>
       <c r="I60" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -3038,10 +3035,10 @@
         <v>14</v>
       </c>
       <c r="G61" t="s">
+        <v>429</v>
+      </c>
+      <c r="H61" t="s">
         <v>430</v>
-      </c>
-      <c r="H61" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -3086,7 +3083,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B68" t="s">
         <v>124</v>
@@ -3112,12 +3109,12 @@
         <v>127</v>
       </c>
       <c r="I69" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B70" t="s">
         <v>128</v>
@@ -3143,7 +3140,7 @@
         <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H71" t="s">
         <v>132</v>
@@ -3171,7 +3168,7 @@
         <v>14</v>
       </c>
       <c r="G73" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H73" t="s">
         <v>135</v>
@@ -3179,7 +3176,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B74" t="s">
         <v>136</v>
@@ -3205,7 +3202,7 @@
         <v>139</v>
       </c>
       <c r="I75" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -3222,7 +3219,7 @@
         <v>14</v>
       </c>
       <c r="G76" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H76" t="s">
         <v>142</v>
@@ -3242,7 +3239,7 @@
         <v>14</v>
       </c>
       <c r="G77" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H77" t="s">
         <v>145</v>
@@ -3264,7 +3261,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B79" t="s">
         <v>148</v>
@@ -3290,7 +3287,7 @@
         <v>151</v>
       </c>
       <c r="I80" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3307,7 +3304,7 @@
         <v>14</v>
       </c>
       <c r="G81" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H81" t="s">
         <v>154</v>
@@ -3341,7 +3338,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B88" t="s">
         <v>157</v>
@@ -3369,7 +3366,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B90" t="s">
         <v>162</v>
@@ -3389,7 +3386,7 @@
         <v>165</v>
       </c>
       <c r="I91" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -3406,7 +3403,7 @@
         <v>14</v>
       </c>
       <c r="G92" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H92" t="s">
         <v>168</v>
@@ -3428,72 +3425,66 @@
         <v>170</v>
       </c>
       <c r="I94" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B95" t="s">
         <v>171</v>
       </c>
       <c r="C95" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E95" t="s">
         <v>14</v>
       </c>
       <c r="G95" t="s">
-        <v>429</v>
+        <v>518</v>
       </c>
       <c r="H95" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C96" t="s">
-        <v>173</v>
-      </c>
-      <c r="E96" t="s">
-        <v>14</v>
-      </c>
-      <c r="G96" t="s">
-        <v>519</v>
-      </c>
-      <c r="H96" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="I96" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B97" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C97" t="s">
-        <v>176</v>
-      </c>
-      <c r="I97" t="s">
-        <v>484</v>
+        <v>177</v>
+      </c>
+      <c r="E97" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B98" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C98" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -3504,10 +3495,10 @@
         <v>59</v>
       </c>
       <c r="B99" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C99" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
@@ -3518,10 +3509,10 @@
         <v>59</v>
       </c>
       <c r="B100" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C100" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E100" t="s">
         <v>14</v>
@@ -3529,1004 +3520,1010 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>59</v>
-      </c>
-      <c r="B101" t="s">
-        <v>183</v>
-      </c>
-      <c r="C101" t="s">
-        <v>184</v>
-      </c>
-      <c r="E101" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>45</v>
+        <v>464</v>
+      </c>
+      <c r="B102" t="s">
+        <v>184</v>
+      </c>
+      <c r="C102" t="s">
+        <v>185</v>
+      </c>
+      <c r="E102" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" t="s">
+        <v>18</v>
+      </c>
+      <c r="I102" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>465</v>
+        <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C103" t="s">
-        <v>186</v>
-      </c>
-      <c r="E103" t="s">
-        <v>14</v>
-      </c>
-      <c r="F103" t="s">
-        <v>18</v>
-      </c>
-      <c r="I103" t="s">
-        <v>485</v>
+        <v>187</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>19</v>
-      </c>
-      <c r="B104" t="s">
-        <v>187</v>
-      </c>
-      <c r="C104" t="s">
-        <v>188</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>434</v>
+      </c>
+      <c r="B107" t="s">
         <v>189</v>
+      </c>
+      <c r="C107" t="s">
+        <v>190</v>
+      </c>
+      <c r="E107" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>435</v>
+        <v>159</v>
       </c>
       <c r="B108" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C108" t="s">
-        <v>191</v>
-      </c>
-      <c r="E108" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108" t="s">
-        <v>18</v>
+        <v>192</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>159</v>
+        <v>438</v>
       </c>
       <c r="B109" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C109" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>439</v>
+        <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C110" t="s">
-        <v>195</v>
+        <v>196</v>
+      </c>
+      <c r="I110" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B111" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C111" t="s">
-        <v>197</v>
-      </c>
-      <c r="I111" t="s">
-        <v>486</v>
+        <v>198</v>
+      </c>
+      <c r="E111" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" t="s">
+        <v>428</v>
+      </c>
+      <c r="H111" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>59</v>
-      </c>
-      <c r="B112" t="s">
-        <v>198</v>
-      </c>
-      <c r="C112" t="s">
-        <v>199</v>
-      </c>
-      <c r="E112" t="s">
-        <v>14</v>
-      </c>
-      <c r="G112" t="s">
-        <v>429</v>
-      </c>
-      <c r="H112" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="B113" t="s">
+        <v>199</v>
+      </c>
+      <c r="C113" t="s">
+        <v>200</v>
+      </c>
+      <c r="I113" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B114" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C114" t="s">
-        <v>201</v>
-      </c>
-      <c r="I114" t="s">
-        <v>487</v>
+        <v>198</v>
+      </c>
+      <c r="E114" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" t="s">
+        <v>428</v>
+      </c>
+      <c r="H114" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B115" t="s">
         <v>202</v>
       </c>
       <c r="C115" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="E115" t="s">
         <v>14</v>
       </c>
       <c r="G115" t="s">
-        <v>429</v>
+        <v>518</v>
       </c>
       <c r="H115" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>441</v>
       </c>
       <c r="B116" t="s">
         <v>203</v>
       </c>
       <c r="C116" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="E116" t="s">
         <v>14</v>
       </c>
-      <c r="G116" t="s">
-        <v>519</v>
-      </c>
-      <c r="H116" t="s">
-        <v>174</v>
+      <c r="F116" t="s">
+        <v>18</v>
+      </c>
+      <c r="I116" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>442</v>
+        <v>19</v>
       </c>
       <c r="B117" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C117" t="s">
-        <v>205</v>
-      </c>
-      <c r="E117" t="s">
-        <v>14</v>
-      </c>
-      <c r="F117" t="s">
-        <v>18</v>
-      </c>
-      <c r="I117" t="s">
-        <v>488</v>
+        <v>187</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>19</v>
-      </c>
-      <c r="B118" t="s">
-        <v>206</v>
-      </c>
-      <c r="C118" t="s">
-        <v>188</v>
+        <v>45</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>434</v>
+      </c>
+      <c r="B121" t="s">
+        <v>206</v>
+      </c>
+      <c r="C121" t="s">
+        <v>207</v>
+      </c>
+      <c r="E121" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>435</v>
+        <v>159</v>
       </c>
       <c r="B122" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C122" t="s">
-        <v>208</v>
-      </c>
-      <c r="E122" t="s">
-        <v>14</v>
-      </c>
-      <c r="F122" t="s">
-        <v>18</v>
+        <v>209</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>159</v>
+        <v>443</v>
       </c>
       <c r="B123" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C123" t="s">
-        <v>210</v>
+        <v>211</v>
+      </c>
+      <c r="E123" t="s">
+        <v>14</v>
+      </c>
+      <c r="F123" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>444</v>
+        <v>9</v>
       </c>
       <c r="B124" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C124" t="s">
-        <v>212</v>
-      </c>
-      <c r="E124" t="s">
-        <v>14</v>
-      </c>
-      <c r="F124" t="s">
-        <v>18</v>
+        <v>213</v>
+      </c>
+      <c r="I124" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B125" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C125" t="s">
-        <v>214</v>
-      </c>
-      <c r="I125" t="s">
-        <v>489</v>
+        <v>215</v>
+      </c>
+      <c r="E125" t="s">
+        <v>14</v>
+      </c>
+      <c r="G125" t="s">
+        <v>428</v>
+      </c>
+      <c r="H125" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>59</v>
-      </c>
-      <c r="B126" t="s">
-        <v>215</v>
-      </c>
-      <c r="C126" t="s">
-        <v>216</v>
-      </c>
-      <c r="E126" t="s">
-        <v>14</v>
-      </c>
-      <c r="G126" t="s">
-        <v>429</v>
-      </c>
-      <c r="H126" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="B127" t="s">
+        <v>216</v>
+      </c>
+      <c r="C127" t="s">
+        <v>217</v>
+      </c>
+      <c r="I127" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B128" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C128" t="s">
-        <v>218</v>
-      </c>
-      <c r="I128" t="s">
-        <v>490</v>
+        <v>215</v>
+      </c>
+      <c r="E128" t="s">
+        <v>14</v>
+      </c>
+      <c r="G128" t="s">
+        <v>428</v>
+      </c>
+      <c r="H128" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B129" t="s">
         <v>219</v>
       </c>
       <c r="C129" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="E129" t="s">
         <v>14</v>
       </c>
       <c r="G129" t="s">
-        <v>429</v>
+        <v>518</v>
       </c>
       <c r="H129" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
       <c r="B130" t="s">
         <v>220</v>
       </c>
       <c r="C130" t="s">
-        <v>173</v>
-      </c>
-      <c r="E130" t="s">
-        <v>14</v>
-      </c>
-      <c r="G130" t="s">
-        <v>519</v>
-      </c>
-      <c r="H130" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>19</v>
-      </c>
-      <c r="B131" t="s">
-        <v>221</v>
-      </c>
-      <c r="C131" t="s">
-        <v>188</v>
+        <v>45</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>434</v>
+      </c>
+      <c r="B134" t="s">
+        <v>221</v>
+      </c>
+      <c r="C134" t="s">
+        <v>222</v>
+      </c>
+      <c r="E134" t="s">
+        <v>14</v>
+      </c>
+      <c r="F134" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>435</v>
+        <v>159</v>
       </c>
       <c r="B135" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C135" t="s">
-        <v>223</v>
-      </c>
-      <c r="E135" t="s">
-        <v>14</v>
-      </c>
-      <c r="F135" t="s">
-        <v>18</v>
+        <v>224</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>159</v>
+        <v>445</v>
       </c>
       <c r="B136" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C136" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="E136" t="s">
+        <v>14</v>
+      </c>
+      <c r="F136" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>446</v>
+        <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C137" t="s">
-        <v>227</v>
-      </c>
-      <c r="E137" t="s">
-        <v>14</v>
-      </c>
-      <c r="F137" t="s">
-        <v>18</v>
+        <v>228</v>
+      </c>
+      <c r="I137" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B138" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C138" t="s">
-        <v>229</v>
-      </c>
-      <c r="I138" t="s">
-        <v>491</v>
+        <v>230</v>
+      </c>
+      <c r="E138" t="s">
+        <v>14</v>
+      </c>
+      <c r="G138" t="s">
+        <v>428</v>
+      </c>
+      <c r="H138" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>59</v>
-      </c>
-      <c r="B139" t="s">
-        <v>230</v>
-      </c>
-      <c r="C139" t="s">
-        <v>231</v>
-      </c>
-      <c r="E139" t="s">
-        <v>14</v>
-      </c>
-      <c r="G139" t="s">
-        <v>429</v>
-      </c>
-      <c r="H139" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>231</v>
+      </c>
+      <c r="C140" t="s">
+        <v>232</v>
+      </c>
+      <c r="I140" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B141" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C141" t="s">
-        <v>233</v>
-      </c>
-      <c r="I141" t="s">
-        <v>492</v>
+        <v>230</v>
+      </c>
+      <c r="E141" t="s">
+        <v>14</v>
+      </c>
+      <c r="G141" t="s">
+        <v>428</v>
+      </c>
+      <c r="H141" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B142" t="s">
         <v>234</v>
       </c>
       <c r="C142" t="s">
-        <v>231</v>
+        <v>172</v>
       </c>
       <c r="E142" t="s">
         <v>14</v>
       </c>
       <c r="G142" t="s">
-        <v>429</v>
+        <v>518</v>
       </c>
       <c r="H142" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
       <c r="B143" t="s">
         <v>235</v>
       </c>
       <c r="C143" t="s">
-        <v>173</v>
-      </c>
-      <c r="E143" t="s">
-        <v>14</v>
-      </c>
-      <c r="G143" t="s">
-        <v>519</v>
-      </c>
-      <c r="H143" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>19</v>
-      </c>
-      <c r="B144" t="s">
-        <v>236</v>
-      </c>
-      <c r="C144" t="s">
-        <v>188</v>
+        <v>45</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>434</v>
+      </c>
+      <c r="B147" t="s">
+        <v>236</v>
+      </c>
+      <c r="C147" t="s">
+        <v>237</v>
+      </c>
+      <c r="E147" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>435</v>
+        <v>159</v>
       </c>
       <c r="B148" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C148" t="s">
-        <v>238</v>
-      </c>
-      <c r="E148" t="s">
-        <v>14</v>
-      </c>
-      <c r="F148" t="s">
-        <v>18</v>
+        <v>239</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>159</v>
+        <v>445</v>
       </c>
       <c r="B149" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C149" t="s">
-        <v>240</v>
+        <v>241</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
+      </c>
+      <c r="F149" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>446</v>
+        <v>9</v>
       </c>
       <c r="B150" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C150" t="s">
-        <v>242</v>
-      </c>
-      <c r="E150" t="s">
-        <v>14</v>
-      </c>
-      <c r="F150" t="s">
-        <v>18</v>
+        <v>243</v>
+      </c>
+      <c r="I150" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B151" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C151" t="s">
-        <v>244</v>
-      </c>
-      <c r="I151" t="s">
-        <v>493</v>
+        <v>245</v>
+      </c>
+      <c r="E151" t="s">
+        <v>14</v>
+      </c>
+      <c r="G151" t="s">
+        <v>428</v>
+      </c>
+      <c r="H151" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>59</v>
-      </c>
-      <c r="B152" t="s">
-        <v>245</v>
-      </c>
-      <c r="C152" t="s">
-        <v>246</v>
-      </c>
-      <c r="E152" t="s">
-        <v>14</v>
-      </c>
-      <c r="G152" t="s">
-        <v>429</v>
-      </c>
-      <c r="H152" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="B153" t="s">
+        <v>246</v>
+      </c>
+      <c r="C153" t="s">
+        <v>247</v>
+      </c>
+      <c r="I153" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B154" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C154" t="s">
-        <v>248</v>
-      </c>
-      <c r="I154" t="s">
-        <v>494</v>
+        <v>245</v>
+      </c>
+      <c r="E154" t="s">
+        <v>14</v>
+      </c>
+      <c r="G154" t="s">
+        <v>428</v>
+      </c>
+      <c r="H154" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B155" t="s">
         <v>249</v>
       </c>
       <c r="C155" t="s">
-        <v>246</v>
+        <v>172</v>
       </c>
       <c r="E155" t="s">
         <v>14</v>
       </c>
       <c r="G155" t="s">
-        <v>429</v>
+        <v>518</v>
       </c>
       <c r="H155" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="B156" t="s">
         <v>250</v>
       </c>
       <c r="C156" t="s">
-        <v>173</v>
-      </c>
-      <c r="E156" t="s">
-        <v>14</v>
-      </c>
-      <c r="G156" t="s">
-        <v>519</v>
-      </c>
-      <c r="H156" t="s">
-        <v>174</v>
+        <v>251</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>9</v>
+        <v>465</v>
       </c>
       <c r="B157" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C157" t="s">
-        <v>252</v>
+        <v>253</v>
+      </c>
+      <c r="E157" t="s">
+        <v>14</v>
+      </c>
+      <c r="F157" t="s">
+        <v>18</v>
+      </c>
+      <c r="I157" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>466</v>
-      </c>
-      <c r="B158" t="s">
-        <v>253</v>
-      </c>
-      <c r="C158" t="s">
-        <v>254</v>
-      </c>
-      <c r="E158" t="s">
-        <v>14</v>
-      </c>
-      <c r="F158" t="s">
-        <v>18</v>
-      </c>
-      <c r="I158" t="s">
-        <v>495</v>
+        <v>45</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="B159" t="s">
+        <v>254</v>
+      </c>
+      <c r="C159" t="s">
+        <v>255</v>
+      </c>
+      <c r="I159" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>449</v>
+      </c>
+      <c r="B160" t="s">
+        <v>256</v>
+      </c>
+      <c r="C160" t="s">
+        <v>257</v>
+      </c>
+      <c r="E160" t="s">
+        <v>14</v>
+      </c>
+      <c r="F160" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>19</v>
+      </c>
+      <c r="B162" t="s">
+        <v>258</v>
+      </c>
+      <c r="C162" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
         <v>9</v>
       </c>
-      <c r="B160" t="s">
-        <v>255</v>
-      </c>
-      <c r="C160" t="s">
-        <v>256</v>
-      </c>
-      <c r="I160" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>450</v>
-      </c>
-      <c r="B161" t="s">
-        <v>257</v>
-      </c>
-      <c r="C161" t="s">
-        <v>258</v>
-      </c>
-      <c r="E161" t="s">
-        <v>14</v>
-      </c>
-      <c r="F161" t="s">
+      <c r="B168" t="s">
+        <v>259</v>
+      </c>
+      <c r="C168" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>121</v>
+      </c>
+      <c r="B169" t="s">
+        <v>261</v>
+      </c>
+      <c r="C169" t="s">
+        <v>262</v>
+      </c>
+      <c r="E169" t="s">
+        <v>14</v>
+      </c>
+      <c r="G169" t="s">
+        <v>518</v>
+      </c>
+      <c r="H169" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>451</v>
+      </c>
+      <c r="B170" t="s">
+        <v>264</v>
+      </c>
+      <c r="C170" t="s">
+        <v>265</v>
+      </c>
+      <c r="E170" t="s">
+        <v>14</v>
+      </c>
+      <c r="F170" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>19</v>
-      </c>
-      <c r="B163" t="s">
-        <v>259</v>
-      </c>
-      <c r="C163" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
-        <v>9</v>
-      </c>
-      <c r="B169" t="s">
-        <v>260</v>
-      </c>
-      <c r="C169" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
-        <v>121</v>
-      </c>
-      <c r="B170" t="s">
-        <v>262</v>
-      </c>
-      <c r="C170" t="s">
-        <v>263</v>
-      </c>
-      <c r="E170" t="s">
-        <v>14</v>
-      </c>
-      <c r="G170" t="s">
-        <v>519</v>
-      </c>
-      <c r="H170" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>452</v>
+        <v>59</v>
       </c>
       <c r="B171" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C171" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E171" t="s">
         <v>14</v>
       </c>
-      <c r="F171" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G171" t="s">
+        <v>428</v>
+      </c>
+      <c r="H171" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>59</v>
       </c>
       <c r="B172" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C172" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E172" t="s">
         <v>14</v>
       </c>
       <c r="G172" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H172" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
+        <v>466</v>
+      </c>
+      <c r="B173" t="s">
+        <v>272</v>
+      </c>
+      <c r="C173" t="s">
+        <v>273</v>
+      </c>
+      <c r="E173" t="s">
+        <v>14</v>
+      </c>
+      <c r="F173" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
         <v>59</v>
       </c>
-      <c r="B173" t="s">
-        <v>270</v>
-      </c>
-      <c r="C173" t="s">
-        <v>271</v>
-      </c>
-      <c r="E173" t="s">
-        <v>14</v>
-      </c>
-      <c r="G173" t="s">
-        <v>429</v>
-      </c>
-      <c r="H173" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
-        <v>467</v>
-      </c>
       <c r="B174" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C174" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E174" t="s">
         <v>14</v>
       </c>
-      <c r="F174" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G174" t="s">
+        <v>428</v>
+      </c>
+      <c r="H174" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>59</v>
+        <v>427</v>
       </c>
       <c r="B175" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C175" t="s">
-        <v>276</v>
+        <v>99</v>
       </c>
       <c r="E175" t="s">
         <v>14</v>
       </c>
-      <c r="G175" t="s">
-        <v>429</v>
-      </c>
-      <c r="H175" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F175" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>428</v>
+        <v>9</v>
       </c>
       <c r="B176" t="s">
         <v>278</v>
       </c>
       <c r="C176" t="s">
-        <v>99</v>
-      </c>
-      <c r="E176" t="s">
-        <v>14</v>
-      </c>
-      <c r="F176" t="s">
-        <v>100</v>
+        <v>279</v>
+      </c>
+      <c r="I176" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>9</v>
+        <v>455</v>
       </c>
       <c r="B177" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C177" t="s">
-        <v>280</v>
-      </c>
-      <c r="I177" t="s">
-        <v>497</v>
+        <v>281</v>
+      </c>
+      <c r="E177" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>456</v>
+        <v>427</v>
       </c>
       <c r="B178" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C178" t="s">
-        <v>282</v>
+        <v>113</v>
       </c>
       <c r="E178" t="s">
         <v>14</v>
+      </c>
+      <c r="F178" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>428</v>
+        <v>159</v>
       </c>
       <c r="B179" t="s">
         <v>283</v>
       </c>
       <c r="C179" t="s">
-        <v>113</v>
-      </c>
-      <c r="E179" t="s">
-        <v>14</v>
-      </c>
-      <c r="F179" t="s">
-        <v>100</v>
+        <v>284</v>
+      </c>
+      <c r="I179" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>159</v>
+        <v>467</v>
       </c>
       <c r="B180" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C180" t="s">
-        <v>285</v>
-      </c>
-      <c r="I180" t="s">
-        <v>498</v>
+        <v>286</v>
+      </c>
+      <c r="E180" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>468</v>
+        <v>59</v>
       </c>
       <c r="B181" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C181" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E181" t="s">
         <v>14</v>
+      </c>
+      <c r="G181" t="s">
+        <v>428</v>
+      </c>
+      <c r="H181" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
@@ -4534,44 +4531,29 @@
         <v>59</v>
       </c>
       <c r="B182" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C182" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E182" t="s">
         <v>14</v>
       </c>
       <c r="G182" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H182" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>59</v>
-      </c>
-      <c r="B183" t="s">
-        <v>291</v>
-      </c>
-      <c r="C183" t="s">
-        <v>292</v>
-      </c>
-      <c r="E183" t="s">
-        <v>14</v>
-      </c>
-      <c r="G183" t="s">
-        <v>429</v>
-      </c>
-      <c r="H183" t="s">
-        <v>293</v>
+        <v>188</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>189</v>
+        <v>45</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
@@ -4579,180 +4561,180 @@
         <v>45</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
-        <v>45</v>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>9</v>
+      </c>
+      <c r="B187" t="s">
+        <v>293</v>
+      </c>
+      <c r="C187" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>9</v>
+        <v>427</v>
       </c>
       <c r="B188" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C188" t="s">
-        <v>295</v>
+        <v>296</v>
+      </c>
+      <c r="E188" t="s">
+        <v>14</v>
+      </c>
+      <c r="F188" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B189" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C189" t="s">
-        <v>297</v>
+        <v>99</v>
       </c>
       <c r="E189" t="s">
         <v>14</v>
       </c>
       <c r="F189" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>428</v>
+        <v>9</v>
       </c>
       <c r="B190" t="s">
         <v>298</v>
       </c>
       <c r="C190" t="s">
-        <v>99</v>
-      </c>
-      <c r="E190" t="s">
-        <v>14</v>
-      </c>
-      <c r="F190" t="s">
-        <v>100</v>
+        <v>299</v>
+      </c>
+      <c r="I190" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B191" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C191" t="s">
-        <v>300</v>
-      </c>
-      <c r="I191" t="s">
-        <v>499</v>
+        <v>301</v>
+      </c>
+      <c r="E191" t="s">
+        <v>14</v>
+      </c>
+      <c r="G191" t="s">
+        <v>428</v>
+      </c>
+      <c r="H191" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>59</v>
+        <v>427</v>
       </c>
       <c r="B192" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C192" t="s">
-        <v>302</v>
+        <v>113</v>
       </c>
       <c r="E192" t="s">
         <v>14</v>
       </c>
-      <c r="G192" t="s">
-        <v>429</v>
-      </c>
-      <c r="H192" t="s">
-        <v>303</v>
+      <c r="F192" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>428</v>
+        <v>9</v>
       </c>
       <c r="B193" t="s">
         <v>304</v>
       </c>
       <c r="C193" t="s">
-        <v>113</v>
-      </c>
-      <c r="E193" t="s">
-        <v>14</v>
-      </c>
-      <c r="F193" t="s">
-        <v>100</v>
+        <v>305</v>
+      </c>
+      <c r="I193" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="B194" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C194" t="s">
-        <v>306</v>
-      </c>
-      <c r="I194" t="s">
-        <v>500</v>
+        <v>307</v>
+      </c>
+      <c r="E194" t="s">
+        <v>14</v>
+      </c>
+      <c r="G194" t="s">
+        <v>520</v>
+      </c>
+      <c r="H194" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="B195" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C195" t="s">
-        <v>308</v>
-      </c>
-      <c r="E195" t="s">
-        <v>14</v>
-      </c>
-      <c r="G195" t="s">
-        <v>521</v>
-      </c>
-      <c r="H195" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="B196" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C196" t="s">
-        <v>311</v>
+        <v>312</v>
+      </c>
+      <c r="E196" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B197" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C197" t="s">
-        <v>313</v>
-      </c>
-      <c r="E197" t="s">
-        <v>14</v>
+        <v>314</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>19</v>
-      </c>
-      <c r="B198" t="s">
-        <v>314</v>
-      </c>
-      <c r="C198" t="s">
-        <v>315</v>
+        <v>188</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>189</v>
+        <v>45</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
@@ -4762,11 +4744,6 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4781,8 +4758,8 @@
   <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4792,277 +4769,277 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E1" t="s">
         <v>469</v>
-      </c>
-      <c r="E1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B4" t="s">
+        <v>320</v>
+      </c>
+      <c r="C4" t="s">
         <v>321</v>
-      </c>
-      <c r="C4" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C5" t="s">
         <v>323</v>
-      </c>
-      <c r="C5" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8" t="s">
         <v>329</v>
-      </c>
-      <c r="C8" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" t="s">
         <v>331</v>
-      </c>
-      <c r="C9" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B10" t="s">
         <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B11" t="s">
         <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B16" t="s">
         <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B21" t="s">
         <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -5073,354 +5050,354 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B26" t="s">
         <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C28" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C29" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B31" t="s">
         <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C32" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C34" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B35" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C36" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B37" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C37" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B39" t="s">
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B40" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C40" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B41" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C41" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B42" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C42" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B43" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C43" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B44" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C44" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B45" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C45" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B47" t="s">
         <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B49" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B52" t="s">
         <v>83</v>
       </c>
       <c r="C52" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B53" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C53" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B55" t="s">
         <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B56" t="s">
         <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D57" t="s">
         <v>37</v>
@@ -5428,7 +5405,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -5445,354 +5422,354 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B60" t="s">
         <v>83</v>
       </c>
       <c r="C60" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B61" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C61" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B62" t="s">
         <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B63" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
       </c>
       <c r="C64" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B65" t="s">
         <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B66" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C66" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B67" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C67" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B68" t="s">
+        <v>337</v>
+      </c>
+      <c r="C68" t="s">
         <v>338</v>
-      </c>
-      <c r="C68" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B69" t="s">
+        <v>339</v>
+      </c>
+      <c r="C69" t="s">
         <v>340</v>
-      </c>
-      <c r="C69" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B70" t="s">
+        <v>341</v>
+      </c>
+      <c r="C70" t="s">
         <v>342</v>
-      </c>
-      <c r="C70" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B71" t="s">
+        <v>343</v>
+      </c>
+      <c r="C71" t="s">
         <v>344</v>
-      </c>
-      <c r="C71" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B72" t="s">
+        <v>345</v>
+      </c>
+      <c r="C72" t="s">
         <v>346</v>
-      </c>
-      <c r="C72" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B73" t="s">
+        <v>347</v>
+      </c>
+      <c r="C73" t="s">
         <v>348</v>
-      </c>
-      <c r="C73" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B74" t="s">
+        <v>349</v>
+      </c>
+      <c r="C74" t="s">
         <v>350</v>
-      </c>
-      <c r="C74" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B76" t="s">
         <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B77" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C77" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B78" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C78" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B80" t="s">
         <v>83</v>
       </c>
       <c r="C80" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B82" t="s">
         <v>83</v>
       </c>
       <c r="C82" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B83" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C83" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B84" t="s">
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B86" t="s">
+        <v>386</v>
+      </c>
+      <c r="C86" t="s">
         <v>387</v>
-      </c>
-      <c r="C86" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B87" t="s">
+        <v>388</v>
+      </c>
+      <c r="C87" t="s">
         <v>389</v>
-      </c>
-      <c r="C87" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B88" t="s">
+        <v>390</v>
+      </c>
+      <c r="C88" t="s">
         <v>391</v>
-      </c>
-      <c r="C88" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B89" t="s">
+        <v>392</v>
+      </c>
+      <c r="C89" t="s">
         <v>393</v>
-      </c>
-      <c r="C89" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B90" t="s">
         <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -5810,7 +5787,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -5834,30 +5811,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" t="s">
         <v>395</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>396</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>397</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>398</v>
       </c>
-      <c r="E1" t="s">
-        <v>399</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -5866,7 +5843,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F2" s="1">
         <v>201807</v>

</xml_diff>

<commit_message>
updated the guides for implementation in odk
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$201</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$197</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="527">
   <si>
     <t>type</t>
   </si>
@@ -630,9 +630,6 @@
     <t>Información avanzada de monitoreo</t>
   </si>
   <si>
-    <t>monitoring_type_count_advance</t>
-  </si>
-  <si>
     <t>monitoring_date_advanced</t>
   </si>
   <si>
@@ -681,9 +678,6 @@
     <t>Información avanzada de preparación de suelo</t>
   </si>
   <si>
-    <t>prepare_soil_type_count_advanced</t>
-  </si>
-  <si>
     <t>prepare_soil_date_advanced</t>
   </si>
   <si>
@@ -726,9 +720,6 @@
     <t>Información avanzada de rastrojo</t>
   </si>
   <si>
-    <t>stubble_type_count_advanced</t>
-  </si>
-  <si>
     <t>stubble_date_advanced</t>
   </si>
   <si>
@@ -769,9 +760,6 @@
   </si>
   <si>
     <t>Información avanzada de manejo fitosanitario</t>
-  </si>
-  <si>
-    <t>phytosanitary_type_count_advanced</t>
   </si>
   <si>
     <t>phytosanitary_date_advanced</t>
@@ -2023,11 +2011,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L201"/>
+  <dimension ref="A1:L197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2044,10 +2032,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2059,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2087,7 +2075,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2101,7 +2089,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2153,13 +2141,13 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2176,13 +2164,13 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H7" t="s">
         <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2199,18 +2187,18 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -2222,12 +2210,12 @@
         <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
@@ -2242,15 +2230,15 @@
         <v>37</v>
       </c>
       <c r="J10" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B11" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -2262,15 +2250,15 @@
         <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B12" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
@@ -2282,7 +2270,7 @@
         <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2299,7 +2287,7 @@
         <v>14</v>
       </c>
       <c r="J13" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2316,13 +2304,13 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="H14" t="s">
         <v>44</v>
       </c>
       <c r="J14" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2343,7 +2331,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
@@ -2389,13 +2377,13 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2412,13 +2400,13 @@
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H21" t="s">
         <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2435,18 +2423,18 @@
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
       </c>
       <c r="J22" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
@@ -2461,12 +2449,12 @@
         <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -2481,15 +2469,15 @@
         <v>37</v>
       </c>
       <c r="J24" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B25" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -2501,15 +2489,15 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B26" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
@@ -2521,7 +2509,7 @@
         <v>18</v>
       </c>
       <c r="K26" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -2538,7 +2526,7 @@
         <v>14</v>
       </c>
       <c r="J27" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -2555,13 +2543,13 @@
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="H28" t="s">
         <v>44</v>
       </c>
       <c r="J28" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -2605,7 +2593,7 @@
         <v>14</v>
       </c>
       <c r="J33" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2613,22 +2601,22 @@
         <v>116</v>
       </c>
       <c r="B34" t="s">
+        <v>517</v>
+      </c>
+      <c r="C34" t="s">
+        <v>519</v>
+      </c>
+      <c r="E34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
+        <v>523</v>
+      </c>
+      <c r="H34" t="s">
+        <v>525</v>
+      </c>
+      <c r="J34" t="s">
         <v>521</v>
-      </c>
-      <c r="C34" t="s">
-        <v>523</v>
-      </c>
-      <c r="E34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" t="s">
-        <v>527</v>
-      </c>
-      <c r="H34" t="s">
-        <v>529</v>
-      </c>
-      <c r="J34" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2636,22 +2624,22 @@
         <v>116</v>
       </c>
       <c r="B35" t="s">
+        <v>518</v>
+      </c>
+      <c r="C35" t="s">
+        <v>520</v>
+      </c>
+      <c r="E35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>524</v>
+      </c>
+      <c r="H35" t="s">
+        <v>526</v>
+      </c>
+      <c r="J35" t="s">
         <v>522</v>
-      </c>
-      <c r="C35" t="s">
-        <v>524</v>
-      </c>
-      <c r="E35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" t="s">
-        <v>528</v>
-      </c>
-      <c r="H35" t="s">
-        <v>530</v>
-      </c>
-      <c r="J35" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2665,12 +2653,12 @@
         <v>67</v>
       </c>
       <c r="J36" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B37" t="s">
         <v>68</v>
@@ -2685,7 +2673,7 @@
         <v>18</v>
       </c>
       <c r="J37" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2755,7 +2743,7 @@
         <v>14</v>
       </c>
       <c r="G43" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="H43" t="s">
         <v>78</v>
@@ -2779,7 +2767,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B47" t="s">
         <v>81</v>
@@ -2811,12 +2799,12 @@
         <v>14</v>
       </c>
       <c r="I48" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B49" t="s">
         <v>86</v>
@@ -2833,7 +2821,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B50" t="s">
         <v>88</v>
@@ -2859,12 +2847,12 @@
         <v>14</v>
       </c>
       <c r="I51" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B52" t="s">
         <v>92</v>
@@ -2893,7 +2881,7 @@
         <v>14</v>
       </c>
       <c r="G53" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H53" t="s">
         <v>97</v>
@@ -2901,7 +2889,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B54" t="s">
         <v>98</v>
@@ -2927,7 +2915,7 @@
         <v>102</v>
       </c>
       <c r="I55" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2944,7 +2932,7 @@
         <v>14</v>
       </c>
       <c r="G56" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H56" t="s">
         <v>105</v>
@@ -2964,7 +2952,7 @@
         <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H57" t="s">
         <v>108</v>
@@ -2984,7 +2972,7 @@
         <v>14</v>
       </c>
       <c r="G58" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H58" t="s">
         <v>111</v>
@@ -2992,7 +2980,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B59" t="s">
         <v>112</v>
@@ -3018,7 +3006,7 @@
         <v>115</v>
       </c>
       <c r="I60" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -3035,10 +3023,10 @@
         <v>14</v>
       </c>
       <c r="G61" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="H61" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -3083,7 +3071,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B68" t="s">
         <v>124</v>
@@ -3109,12 +3097,12 @@
         <v>127</v>
       </c>
       <c r="I69" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B70" t="s">
         <v>128</v>
@@ -3140,7 +3128,7 @@
         <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="H71" t="s">
         <v>132</v>
@@ -3168,7 +3156,7 @@
         <v>14</v>
       </c>
       <c r="G73" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H73" t="s">
         <v>135</v>
@@ -3176,7 +3164,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B74" t="s">
         <v>136</v>
@@ -3202,7 +3190,7 @@
         <v>139</v>
       </c>
       <c r="I75" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -3219,7 +3207,7 @@
         <v>14</v>
       </c>
       <c r="G76" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="H76" t="s">
         <v>142</v>
@@ -3239,7 +3227,7 @@
         <v>14</v>
       </c>
       <c r="G77" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="H77" t="s">
         <v>145</v>
@@ -3261,7 +3249,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B79" t="s">
         <v>148</v>
@@ -3287,7 +3275,7 @@
         <v>151</v>
       </c>
       <c r="I80" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3304,7 +3292,7 @@
         <v>14</v>
       </c>
       <c r="G81" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="H81" t="s">
         <v>154</v>
@@ -3338,7 +3326,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B88" t="s">
         <v>157</v>
@@ -3366,7 +3354,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B90" t="s">
         <v>162</v>
@@ -3386,7 +3374,7 @@
         <v>165</v>
       </c>
       <c r="I91" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -3403,7 +3391,7 @@
         <v>14</v>
       </c>
       <c r="G92" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H92" t="s">
         <v>168</v>
@@ -3425,7 +3413,7 @@
         <v>170</v>
       </c>
       <c r="I94" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -3442,7 +3430,7 @@
         <v>14</v>
       </c>
       <c r="G95" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="H95" t="s">
         <v>173</v>
@@ -3459,7 +3447,7 @@
         <v>175</v>
       </c>
       <c r="I96" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -3525,7 +3513,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B102" t="s">
         <v>184</v>
@@ -3540,7 +3528,7 @@
         <v>18</v>
       </c>
       <c r="I102" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -3566,7 +3554,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B107" t="s">
         <v>189</v>
@@ -3594,7 +3582,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B109" t="s">
         <v>193</v>
@@ -3614,7 +3602,7 @@
         <v>196</v>
       </c>
       <c r="I110" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -3631,7 +3619,7 @@
         <v>14</v>
       </c>
       <c r="G111" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H111" t="s">
         <v>168</v>
@@ -3653,258 +3641,246 @@
         <v>200</v>
       </c>
       <c r="I113" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B114" t="s">
         <v>201</v>
       </c>
       <c r="C114" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="E114" t="s">
         <v>14</v>
       </c>
       <c r="G114" t="s">
-        <v>428</v>
+        <v>514</v>
       </c>
       <c r="H114" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>121</v>
+        <v>437</v>
       </c>
       <c r="B115" t="s">
         <v>202</v>
       </c>
       <c r="C115" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="E115" t="s">
         <v>14</v>
       </c>
-      <c r="G115" t="s">
-        <v>518</v>
-      </c>
-      <c r="H115" t="s">
-        <v>173</v>
+      <c r="F115" t="s">
+        <v>18</v>
+      </c>
+      <c r="I115" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>441</v>
+        <v>19</v>
       </c>
       <c r="B116" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C116" t="s">
-        <v>204</v>
-      </c>
-      <c r="E116" t="s">
-        <v>14</v>
-      </c>
-      <c r="F116" t="s">
-        <v>18</v>
-      </c>
-      <c r="I116" t="s">
-        <v>487</v>
+        <v>187</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>19</v>
-      </c>
-      <c r="B117" t="s">
-        <v>205</v>
-      </c>
-      <c r="C117" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
         <v>188</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>430</v>
+      </c>
+      <c r="B120" t="s">
+        <v>205</v>
+      </c>
+      <c r="C120" t="s">
+        <v>206</v>
+      </c>
+      <c r="E120" t="s">
+        <v>14</v>
+      </c>
+      <c r="F120" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>434</v>
+        <v>159</v>
       </c>
       <c r="B121" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C121" t="s">
-        <v>207</v>
-      </c>
-      <c r="E121" t="s">
-        <v>14</v>
-      </c>
-      <c r="F121" t="s">
-        <v>18</v>
+        <v>208</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>159</v>
+        <v>439</v>
       </c>
       <c r="B122" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C122" t="s">
-        <v>209</v>
+        <v>210</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
+      </c>
+      <c r="F122" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>443</v>
+        <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C123" t="s">
-        <v>211</v>
-      </c>
-      <c r="E123" t="s">
-        <v>14</v>
-      </c>
-      <c r="F123" t="s">
-        <v>18</v>
+        <v>212</v>
+      </c>
+      <c r="I123" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B124" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C124" t="s">
-        <v>213</v>
-      </c>
-      <c r="I124" t="s">
-        <v>488</v>
+        <v>214</v>
+      </c>
+      <c r="E124" t="s">
+        <v>14</v>
+      </c>
+      <c r="G124" t="s">
+        <v>424</v>
+      </c>
+      <c r="H124" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>59</v>
-      </c>
-      <c r="B125" t="s">
-        <v>214</v>
-      </c>
-      <c r="C125" t="s">
-        <v>215</v>
-      </c>
-      <c r="E125" t="s">
-        <v>14</v>
-      </c>
-      <c r="G125" t="s">
-        <v>428</v>
-      </c>
-      <c r="H125" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="B126" t="s">
+        <v>215</v>
+      </c>
+      <c r="C126" t="s">
+        <v>216</v>
+      </c>
+      <c r="I126" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="B127" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C127" t="s">
-        <v>217</v>
-      </c>
-      <c r="I127" t="s">
-        <v>489</v>
+        <v>172</v>
+      </c>
+      <c r="E127" t="s">
+        <v>14</v>
+      </c>
+      <c r="G127" t="s">
+        <v>514</v>
+      </c>
+      <c r="H127" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B128" t="s">
         <v>218</v>
       </c>
       <c r="C128" t="s">
-        <v>215</v>
-      </c>
-      <c r="E128" t="s">
-        <v>14</v>
-      </c>
-      <c r="G128" t="s">
-        <v>428</v>
-      </c>
-      <c r="H128" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>121</v>
-      </c>
-      <c r="B129" t="s">
-        <v>219</v>
-      </c>
-      <c r="C129" t="s">
-        <v>172</v>
-      </c>
-      <c r="E129" t="s">
-        <v>14</v>
-      </c>
-      <c r="G129" t="s">
-        <v>518</v>
-      </c>
-      <c r="H129" t="s">
-        <v>173</v>
+        <v>45</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>19</v>
-      </c>
-      <c r="B130" t="s">
-        <v>220</v>
-      </c>
-      <c r="C130" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>45</v>
+        <v>188</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>188</v>
+        <v>430</v>
+      </c>
+      <c r="B132" t="s">
+        <v>219</v>
+      </c>
+      <c r="C132" t="s">
+        <v>220</v>
+      </c>
+      <c r="E132" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>159</v>
+      </c>
+      <c r="B133" t="s">
+        <v>221</v>
+      </c>
+      <c r="C133" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="B134" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C134" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E134" t="s">
         <v>14</v>
@@ -3915,49 +3891,46 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>159</v>
+        <v>9</v>
       </c>
       <c r="B135" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C135" t="s">
-        <v>224</v>
+        <v>226</v>
+      </c>
+      <c r="I135" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>445</v>
+        <v>59</v>
       </c>
       <c r="B136" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C136" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E136" t="s">
         <v>14</v>
       </c>
-      <c r="F136" t="s">
-        <v>18</v>
+      <c r="G136" t="s">
+        <v>424</v>
+      </c>
+      <c r="H136" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>9</v>
-      </c>
-      <c r="B137" t="s">
-        <v>227</v>
-      </c>
-      <c r="C137" t="s">
-        <v>228</v>
-      </c>
-      <c r="I137" t="s">
-        <v>490</v>
+        <v>45</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B138" t="s">
         <v>229</v>
@@ -3965,139 +3938,133 @@
       <c r="C138" t="s">
         <v>230</v>
       </c>
-      <c r="E138" t="s">
-        <v>14</v>
-      </c>
-      <c r="G138" t="s">
-        <v>428</v>
-      </c>
-      <c r="H138" t="s">
-        <v>168</v>
+      <c r="I138" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>45</v>
+        <v>121</v>
+      </c>
+      <c r="B139" t="s">
+        <v>231</v>
+      </c>
+      <c r="C139" t="s">
+        <v>172</v>
+      </c>
+      <c r="E139" t="s">
+        <v>14</v>
+      </c>
+      <c r="G139" t="s">
+        <v>514</v>
+      </c>
+      <c r="H139" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C140" t="s">
-        <v>232</v>
-      </c>
-      <c r="I140" t="s">
-        <v>491</v>
+        <v>187</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>59</v>
-      </c>
-      <c r="B141" t="s">
-        <v>233</v>
-      </c>
-      <c r="C141" t="s">
-        <v>230</v>
-      </c>
-      <c r="E141" t="s">
-        <v>14</v>
-      </c>
-      <c r="G141" t="s">
-        <v>428</v>
-      </c>
-      <c r="H141" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>121</v>
-      </c>
-      <c r="B142" t="s">
-        <v>234</v>
-      </c>
-      <c r="C142" t="s">
-        <v>172</v>
-      </c>
-      <c r="E142" t="s">
-        <v>14</v>
-      </c>
-      <c r="G142" t="s">
-        <v>518</v>
-      </c>
-      <c r="H142" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>19</v>
-      </c>
-      <c r="B143" t="s">
-        <v>235</v>
-      </c>
-      <c r="C143" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>45</v>
+        <v>430</v>
+      </c>
+      <c r="B144" t="s">
+        <v>233</v>
+      </c>
+      <c r="C144" t="s">
+        <v>234</v>
+      </c>
+      <c r="E144" t="s">
+        <v>14</v>
+      </c>
+      <c r="F144" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>188</v>
+        <v>159</v>
+      </c>
+      <c r="B145" t="s">
+        <v>235</v>
+      </c>
+      <c r="C145" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>441</v>
+      </c>
+      <c r="B146" t="s">
+        <v>237</v>
+      </c>
+      <c r="C146" t="s">
+        <v>238</v>
+      </c>
+      <c r="E146" t="s">
+        <v>14</v>
+      </c>
+      <c r="F146" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>434</v>
+        <v>9</v>
       </c>
       <c r="B147" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C147" t="s">
-        <v>237</v>
-      </c>
-      <c r="E147" t="s">
-        <v>14</v>
-      </c>
-      <c r="F147" t="s">
-        <v>18</v>
+        <v>240</v>
+      </c>
+      <c r="I147" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="B148" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C148" t="s">
-        <v>239</v>
+        <v>242</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="G148" t="s">
+        <v>424</v>
+      </c>
+      <c r="H148" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>445</v>
-      </c>
-      <c r="B149" t="s">
-        <v>240</v>
-      </c>
-      <c r="C149" t="s">
-        <v>241</v>
-      </c>
-      <c r="E149" t="s">
-        <v>14</v>
-      </c>
-      <c r="F149" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
@@ -4105,645 +4072,586 @@
         <v>9</v>
       </c>
       <c r="B150" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C150" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I150" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B151" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C151" t="s">
-        <v>245</v>
+        <v>172</v>
       </c>
       <c r="E151" t="s">
         <v>14</v>
       </c>
       <c r="G151" t="s">
-        <v>428</v>
+        <v>514</v>
       </c>
       <c r="H151" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="B152" t="s">
+        <v>246</v>
+      </c>
+      <c r="C152" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>9</v>
+        <v>461</v>
       </c>
       <c r="B153" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C153" t="s">
-        <v>247</v>
+        <v>249</v>
+      </c>
+      <c r="E153" t="s">
+        <v>14</v>
+      </c>
+      <c r="F153" t="s">
+        <v>18</v>
       </c>
       <c r="I153" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>59</v>
-      </c>
-      <c r="B154" t="s">
-        <v>248</v>
-      </c>
-      <c r="C154" t="s">
-        <v>245</v>
-      </c>
-      <c r="E154" t="s">
-        <v>14</v>
-      </c>
-      <c r="G154" t="s">
-        <v>428</v>
-      </c>
-      <c r="H154" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="B155" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C155" t="s">
-        <v>172</v>
-      </c>
-      <c r="E155" t="s">
-        <v>14</v>
-      </c>
-      <c r="G155" t="s">
-        <v>518</v>
-      </c>
-      <c r="H155" t="s">
-        <v>173</v>
+        <v>251</v>
+      </c>
+      <c r="I155" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>9</v>
+        <v>445</v>
       </c>
       <c r="B156" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C156" t="s">
-        <v>251</v>
+        <v>253</v>
+      </c>
+      <c r="E156" t="s">
+        <v>14</v>
+      </c>
+      <c r="F156" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>465</v>
-      </c>
-      <c r="B157" t="s">
-        <v>252</v>
-      </c>
-      <c r="C157" t="s">
-        <v>253</v>
-      </c>
-      <c r="E157" t="s">
-        <v>14</v>
-      </c>
-      <c r="F157" t="s">
-        <v>18</v>
-      </c>
-      <c r="I157" t="s">
-        <v>494</v>
+        <v>45</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="B158" t="s">
+        <v>254</v>
+      </c>
+      <c r="C158" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>9</v>
-      </c>
-      <c r="B159" t="s">
-        <v>254</v>
-      </c>
-      <c r="C159" t="s">
-        <v>255</v>
-      </c>
-      <c r="I159" t="s">
-        <v>495</v>
+        <v>45</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>449</v>
-      </c>
-      <c r="B160" t="s">
-        <v>256</v>
-      </c>
-      <c r="C160" t="s">
-        <v>257</v>
-      </c>
-      <c r="E160" t="s">
-        <v>14</v>
-      </c>
-      <c r="F160" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>45</v>
+        <v>188</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>19</v>
-      </c>
-      <c r="B162" t="s">
-        <v>258</v>
-      </c>
-      <c r="C162" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>188</v>
+        <v>9</v>
+      </c>
+      <c r="B164" t="s">
+        <v>255</v>
+      </c>
+      <c r="C164" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>121</v>
+      </c>
+      <c r="B165" t="s">
+        <v>257</v>
+      </c>
+      <c r="C165" t="s">
+        <v>258</v>
+      </c>
+      <c r="E165" t="s">
+        <v>14</v>
+      </c>
+      <c r="G165" t="s">
+        <v>514</v>
+      </c>
+      <c r="H165" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>45</v>
+        <v>447</v>
+      </c>
+      <c r="B166" t="s">
+        <v>260</v>
+      </c>
+      <c r="C166" t="s">
+        <v>261</v>
+      </c>
+      <c r="E166" t="s">
+        <v>14</v>
+      </c>
+      <c r="F166" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>59</v>
+      </c>
+      <c r="B167" t="s">
+        <v>262</v>
+      </c>
+      <c r="C167" t="s">
+        <v>263</v>
+      </c>
+      <c r="E167" t="s">
+        <v>14</v>
+      </c>
+      <c r="G167" t="s">
+        <v>424</v>
+      </c>
+      <c r="H167" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B168" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C168" t="s">
-        <v>260</v>
+        <v>266</v>
+      </c>
+      <c r="E168" t="s">
+        <v>14</v>
+      </c>
+      <c r="G168" t="s">
+        <v>424</v>
+      </c>
+      <c r="H168" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>121</v>
+        <v>462</v>
       </c>
       <c r="B169" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="C169" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="E169" t="s">
         <v>14</v>
       </c>
-      <c r="G169" t="s">
-        <v>518</v>
-      </c>
-      <c r="H169" t="s">
-        <v>263</v>
+      <c r="F169" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>451</v>
+        <v>59</v>
       </c>
       <c r="B170" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C170" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="E170" t="s">
         <v>14</v>
       </c>
-      <c r="F170" t="s">
-        <v>18</v>
+      <c r="G170" t="s">
+        <v>424</v>
+      </c>
+      <c r="H170" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>59</v>
+        <v>423</v>
       </c>
       <c r="B171" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C171" t="s">
-        <v>267</v>
+        <v>99</v>
       </c>
       <c r="E171" t="s">
         <v>14</v>
       </c>
-      <c r="G171" t="s">
-        <v>428</v>
-      </c>
-      <c r="H171" t="s">
-        <v>268</v>
+      <c r="F171" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B172" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C172" t="s">
-        <v>270</v>
-      </c>
-      <c r="E172" t="s">
-        <v>14</v>
-      </c>
-      <c r="G172" t="s">
-        <v>428</v>
-      </c>
-      <c r="H172" t="s">
-        <v>271</v>
+        <v>275</v>
+      </c>
+      <c r="I172" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="B173" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C173" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E173" t="s">
         <v>14</v>
-      </c>
-      <c r="F173" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>59</v>
+        <v>423</v>
       </c>
       <c r="B174" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C174" t="s">
-        <v>275</v>
+        <v>113</v>
       </c>
       <c r="E174" t="s">
         <v>14</v>
       </c>
-      <c r="G174" t="s">
-        <v>428</v>
-      </c>
-      <c r="H174" t="s">
-        <v>276</v>
+      <c r="F174" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>427</v>
+        <v>159</v>
       </c>
       <c r="B175" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C175" t="s">
-        <v>99</v>
-      </c>
-      <c r="E175" t="s">
-        <v>14</v>
-      </c>
-      <c r="F175" t="s">
-        <v>100</v>
+        <v>280</v>
+      </c>
+      <c r="I175" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>9</v>
+        <v>463</v>
       </c>
       <c r="B176" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C176" t="s">
-        <v>279</v>
-      </c>
-      <c r="I176" t="s">
-        <v>496</v>
+        <v>282</v>
+      </c>
+      <c r="E176" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>455</v>
+        <v>59</v>
       </c>
       <c r="B177" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C177" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E177" t="s">
         <v>14</v>
+      </c>
+      <c r="G177" t="s">
+        <v>424</v>
+      </c>
+      <c r="H177" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>427</v>
+        <v>59</v>
       </c>
       <c r="B178" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C178" t="s">
-        <v>113</v>
+        <v>287</v>
       </c>
       <c r="E178" t="s">
         <v>14</v>
       </c>
-      <c r="F178" t="s">
-        <v>100</v>
+      <c r="G178" t="s">
+        <v>424</v>
+      </c>
+      <c r="H178" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>159</v>
-      </c>
-      <c r="B179" t="s">
-        <v>283</v>
-      </c>
-      <c r="C179" t="s">
-        <v>284</v>
-      </c>
-      <c r="I179" t="s">
-        <v>497</v>
+        <v>188</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>467</v>
-      </c>
-      <c r="B180" t="s">
-        <v>285</v>
-      </c>
-      <c r="C180" t="s">
-        <v>286</v>
-      </c>
-      <c r="E180" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>59</v>
-      </c>
-      <c r="B181" t="s">
-        <v>287</v>
-      </c>
-      <c r="C181" t="s">
-        <v>288</v>
-      </c>
-      <c r="E181" t="s">
-        <v>14</v>
-      </c>
-      <c r="G181" t="s">
-        <v>428</v>
-      </c>
-      <c r="H181" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
-        <v>59</v>
-      </c>
-      <c r="B182" t="s">
-        <v>290</v>
-      </c>
-      <c r="C182" t="s">
-        <v>291</v>
-      </c>
-      <c r="E182" t="s">
-        <v>14</v>
-      </c>
-      <c r="G182" t="s">
-        <v>428</v>
-      </c>
-      <c r="H182" t="s">
-        <v>292</v>
+        <v>45</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>188</v>
+        <v>9</v>
+      </c>
+      <c r="B183" t="s">
+        <v>289</v>
+      </c>
+      <c r="C183" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>45</v>
+        <v>423</v>
+      </c>
+      <c r="B184" t="s">
+        <v>291</v>
+      </c>
+      <c r="C184" t="s">
+        <v>292</v>
+      </c>
+      <c r="E184" t="s">
+        <v>14</v>
+      </c>
+      <c r="F184" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>45</v>
+        <v>423</v>
+      </c>
+      <c r="B185" t="s">
+        <v>293</v>
+      </c>
+      <c r="C185" t="s">
+        <v>99</v>
+      </c>
+      <c r="E185" t="s">
+        <v>14</v>
+      </c>
+      <c r="F185" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>9</v>
+      </c>
+      <c r="B186" t="s">
+        <v>294</v>
+      </c>
+      <c r="C186" t="s">
+        <v>295</v>
+      </c>
+      <c r="I186" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B187" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C187" t="s">
-        <v>294</v>
+        <v>297</v>
+      </c>
+      <c r="E187" t="s">
+        <v>14</v>
+      </c>
+      <c r="G187" t="s">
+        <v>424</v>
+      </c>
+      <c r="H187" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B188" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C188" t="s">
-        <v>296</v>
+        <v>113</v>
       </c>
       <c r="E188" t="s">
         <v>14</v>
       </c>
       <c r="F188" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>427</v>
+        <v>9</v>
       </c>
       <c r="B189" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C189" t="s">
-        <v>99</v>
-      </c>
-      <c r="E189" t="s">
-        <v>14</v>
-      </c>
-      <c r="F189" t="s">
-        <v>100</v>
+        <v>301</v>
+      </c>
+      <c r="I189" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="B190" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C190" t="s">
-        <v>299</v>
-      </c>
-      <c r="I190" t="s">
-        <v>498</v>
+        <v>303</v>
+      </c>
+      <c r="E190" t="s">
+        <v>14</v>
+      </c>
+      <c r="G190" t="s">
+        <v>516</v>
+      </c>
+      <c r="H190" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="B191" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C191" t="s">
-        <v>301</v>
-      </c>
-      <c r="E191" t="s">
-        <v>14</v>
-      </c>
-      <c r="G191" t="s">
-        <v>428</v>
-      </c>
-      <c r="H191" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>427</v>
+        <v>59</v>
       </c>
       <c r="B192" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C192" t="s">
-        <v>113</v>
+        <v>308</v>
       </c>
       <c r="E192" t="s">
         <v>14</v>
       </c>
-      <c r="F192" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B193" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C193" t="s">
-        <v>305</v>
-      </c>
-      <c r="I193" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>121</v>
-      </c>
-      <c r="B194" t="s">
-        <v>306</v>
-      </c>
-      <c r="C194" t="s">
-        <v>307</v>
-      </c>
-      <c r="E194" t="s">
-        <v>14</v>
-      </c>
-      <c r="G194" t="s">
-        <v>520</v>
-      </c>
-      <c r="H194" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>159</v>
-      </c>
-      <c r="B195" t="s">
-        <v>309</v>
-      </c>
-      <c r="C195" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>59</v>
-      </c>
-      <c r="B196" t="s">
-        <v>311</v>
-      </c>
-      <c r="C196" t="s">
-        <v>312</v>
-      </c>
-      <c r="E196" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>19</v>
-      </c>
-      <c r="B197" t="s">
-        <v>313</v>
-      </c>
-      <c r="C197" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4769,277 +4677,277 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C4" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B8" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B10" t="s">
         <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B11" t="s">
         <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B14" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C14" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B16" t="s">
         <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B17" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C17" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B18" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C18" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B19" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C19" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B21" t="s">
         <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B22" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C22" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B23" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C23" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B24" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C24" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -5050,354 +4958,354 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B26" t="s">
         <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B27" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C27" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B28" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C28" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B29" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C29" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B31" t="s">
         <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B32" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C32" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B33" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C33" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B34" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C34" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B35" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C35" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B36" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C36" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B37" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C37" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B39" t="s">
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B40" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C40" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B41" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C41" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B42" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C42" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B43" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C43" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B44" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C44" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B45" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C45" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B47" t="s">
         <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B48" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C48" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B49" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C49" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B50" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C50" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B52" t="s">
         <v>83</v>
       </c>
       <c r="C52" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B53" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C53" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B55" t="s">
         <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B56" t="s">
         <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D57" t="s">
         <v>37</v>
@@ -5405,7 +5313,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -5422,354 +5330,354 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B60" t="s">
         <v>83</v>
       </c>
       <c r="C60" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B61" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C61" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B62" t="s">
         <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B63" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C63" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
       </c>
       <c r="C64" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B65" t="s">
         <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B66" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C66" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B67" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C67" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B68" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C68" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B69" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C69" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B70" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C70" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B71" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C71" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B72" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C72" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B73" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C73" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B74" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C74" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B76" t="s">
         <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B77" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C77" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B78" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C78" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B80" t="s">
         <v>83</v>
       </c>
       <c r="C80" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B82" t="s">
         <v>83</v>
       </c>
       <c r="C82" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B83" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C83" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B84" t="s">
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B86" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C86" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B87" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C87" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B88" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C88" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B89" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C89" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B90" t="s">
         <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -5787,7 +5695,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -5811,30 +5719,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1" t="s">
         <v>394</v>
       </c>
-      <c r="B1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E1" t="s">
-        <v>398</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -5843,7 +5751,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F2" s="1">
         <v>201807</v>

</xml_diff>

<commit_message>
deleted the field altitude in plot section. Changed the type of field in farm location for geopoint
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$196</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$195</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="515">
   <si>
     <t>type</t>
   </si>
@@ -1557,36 +1557,6 @@
     <t>(decimal-date-time(.) &gt; decimal-date-time(${transfer_date}))</t>
   </si>
   <si>
-    <t>farm_location_lat</t>
-  </si>
-  <si>
-    <t>farm_location_lon</t>
-  </si>
-  <si>
-    <t>Latitud de la finca</t>
-  </si>
-  <si>
-    <t>Longitud de la finca</t>
-  </si>
-  <si>
-    <t>number(pulldata('farm','lat', 'farm_key', ${farm_id}))</t>
-  </si>
-  <si>
-    <t>number(pulldata('farm','lon', 'farm_key', ${farm_id}))</t>
-  </si>
-  <si>
-    <t>(. &gt;= -90) and (. &lt;= 90)</t>
-  </si>
-  <si>
-    <t>(. &gt;= -180) and (. &lt;= 180)</t>
-  </si>
-  <si>
-    <t>La latitud debe ser un campo numérico entre -90 y 90</t>
-  </si>
-  <si>
-    <t>La longitud debe ser un campo numérico entre -180 y 180</t>
-  </si>
-  <si>
     <t>El número de identificación debe ser numérico y no tener espacios en blanco al final</t>
   </si>
   <si>
@@ -1594,6 +1564,12 @@
   </si>
   <si>
     <t>El apellido debe contener solamente texto y no tener espacios en blanco al final</t>
+  </si>
+  <si>
+    <t>farm_location</t>
+  </si>
+  <si>
+    <t>Ubicación de la finca</t>
   </si>
 </sst>
 </file>
@@ -1999,11 +1975,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L196"/>
+  <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2112,7 +2088,7 @@
         <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2132,7 +2108,7 @@
         <v>401</v>
       </c>
       <c r="H6" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="J6" t="s">
         <v>490</v>
@@ -2155,7 +2131,7 @@
         <v>401</v>
       </c>
       <c r="H7" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="J7" t="s">
         <v>491</v>
@@ -2348,7 +2324,7 @@
         <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2368,7 +2344,7 @@
         <v>401</v>
       </c>
       <c r="H20" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="J20" t="s">
         <v>497</v>
@@ -2391,7 +2367,7 @@
         <v>401</v>
       </c>
       <c r="H21" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="J21" t="s">
         <v>498</v>
@@ -2586,301 +2562,295 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="C34" t="s">
-        <v>512</v>
+        <v>514</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
       </c>
-      <c r="G34" t="s">
-        <v>516</v>
-      </c>
-      <c r="H34" t="s">
-        <v>518</v>
-      </c>
-      <c r="J34" t="s">
-        <v>514</v>
+      <c r="L34" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>511</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>513</v>
-      </c>
-      <c r="E35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" t="s">
-        <v>517</v>
-      </c>
-      <c r="H35" t="s">
-        <v>519</v>
+        <v>64</v>
       </c>
       <c r="J35" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>410</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="E36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
       </c>
       <c r="J36" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>410</v>
-      </c>
-      <c r="B37" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" t="s">
-        <v>18</v>
-      </c>
-      <c r="J37" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="E40" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
       </c>
       <c r="E41" t="s">
         <v>14</v>
+      </c>
+      <c r="L41" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" t="s">
-        <v>14</v>
-      </c>
-      <c r="L42" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>448</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="E45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>448</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
       </c>
       <c r="E46" t="s">
         <v>14</v>
       </c>
-      <c r="F46" t="s">
-        <v>77</v>
+      <c r="I46" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>449</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
-      </c>
-      <c r="D47" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
       </c>
-      <c r="I47" t="s">
-        <v>466</v>
+      <c r="F47" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B48" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
-      </c>
-      <c r="F48" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>450</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
+      </c>
+      <c r="I49" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>416</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
       </c>
-      <c r="I50" t="s">
-        <v>467</v>
+      <c r="F50" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>416</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
       </c>
-      <c r="F51" t="s">
-        <v>88</v>
+      <c r="G51" t="s">
+        <v>417</v>
+      </c>
+      <c r="H51" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>416</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E52" t="s">
         <v>14</v>
       </c>
-      <c r="G52" t="s">
-        <v>417</v>
-      </c>
-      <c r="H52" t="s">
-        <v>91</v>
+      <c r="F52" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>416</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
-      </c>
-      <c r="E53" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="I53" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>96</v>
-      </c>
-      <c r="I54" t="s">
-        <v>465</v>
+        <v>98</v>
+      </c>
+      <c r="E54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" t="s">
+        <v>417</v>
+      </c>
+      <c r="H54" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -2888,10 +2858,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2900,7 +2870,7 @@
         <v>417</v>
       </c>
       <c r="H55" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2908,10 +2878,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2920,78 +2890,63 @@
         <v>417</v>
       </c>
       <c r="H56" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>416</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
       </c>
-      <c r="G57" t="s">
-        <v>417</v>
-      </c>
-      <c r="H57" t="s">
-        <v>105</v>
+      <c r="F57" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>416</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
-      </c>
-      <c r="E58" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58" t="s">
-        <v>94</v>
+        <v>109</v>
+      </c>
+      <c r="I58" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
-      </c>
-      <c r="I59" t="s">
-        <v>468</v>
+        <v>112</v>
+      </c>
+      <c r="E59" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" t="s">
+        <v>418</v>
+      </c>
+      <c r="H59" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>110</v>
-      </c>
-      <c r="B60" t="s">
-        <v>111</v>
-      </c>
-      <c r="C60" t="s">
-        <v>112</v>
-      </c>
-      <c r="E60" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" t="s">
-        <v>418</v>
-      </c>
-      <c r="H60" t="s">
-        <v>419</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -3004,158 +2959,173 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>42</v>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C65" t="s">
-        <v>114</v>
+        <v>117</v>
+      </c>
+      <c r="E65" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>451</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C66" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E66" t="s">
         <v>14</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>451</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C67" t="s">
-        <v>119</v>
-      </c>
-      <c r="E67" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" t="s">
-        <v>18</v>
+        <v>121</v>
+      </c>
+      <c r="I67" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="B68" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C68" t="s">
-        <v>121</v>
-      </c>
-      <c r="I68" t="s">
-        <v>469</v>
+        <v>123</v>
+      </c>
+      <c r="E68" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>452</v>
+        <v>115</v>
       </c>
       <c r="B69" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E69" t="s">
         <v>14</v>
+      </c>
+      <c r="G69" t="s">
+        <v>507</v>
+      </c>
+      <c r="H69" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>115</v>
-      </c>
-      <c r="B70" t="s">
-        <v>124</v>
-      </c>
-      <c r="C70" t="s">
-        <v>125</v>
-      </c>
-      <c r="E70" t="s">
-        <v>14</v>
-      </c>
-      <c r="G70" t="s">
-        <v>507</v>
-      </c>
-      <c r="H70" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="B71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" t="s">
+        <v>128</v>
+      </c>
+      <c r="D71" t="s">
+        <v>17</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" t="s">
+        <v>417</v>
+      </c>
+      <c r="H71" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>56</v>
+        <v>416</v>
       </c>
       <c r="B72" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D72" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="E72" t="s">
         <v>14</v>
       </c>
-      <c r="G72" t="s">
-        <v>417</v>
-      </c>
-      <c r="H72" t="s">
-        <v>129</v>
+      <c r="F72" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>416</v>
+        <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C73" t="s">
-        <v>131</v>
-      </c>
-      <c r="E73" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" t="s">
-        <v>94</v>
+        <v>133</v>
+      </c>
+      <c r="I73" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C74" t="s">
-        <v>133</v>
-      </c>
-      <c r="I74" t="s">
-        <v>470</v>
+        <v>135</v>
+      </c>
+      <c r="E74" t="s">
+        <v>14</v>
+      </c>
+      <c r="G74" t="s">
+        <v>507</v>
+      </c>
+      <c r="H74" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -3163,104 +3133,89 @@
         <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C75" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E75" t="s">
         <v>14</v>
       </c>
       <c r="G75" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="H75" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C76" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
-      </c>
-      <c r="G76" t="s">
-        <v>508</v>
-      </c>
-      <c r="H76" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>416</v>
       </c>
       <c r="B77" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E77" t="s">
         <v>14</v>
+      </c>
+      <c r="F77" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>416</v>
+        <v>9</v>
       </c>
       <c r="B78" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C78" t="s">
-        <v>143</v>
-      </c>
-      <c r="E78" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" t="s">
-        <v>94</v>
+        <v>145</v>
+      </c>
+      <c r="I78" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B79" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C79" t="s">
-        <v>145</v>
-      </c>
-      <c r="I79" t="s">
-        <v>471</v>
+        <v>147</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+      <c r="G79" t="s">
+        <v>418</v>
+      </c>
+      <c r="H79" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>110</v>
-      </c>
-      <c r="B80" t="s">
-        <v>146</v>
-      </c>
-      <c r="C80" t="s">
-        <v>147</v>
-      </c>
-      <c r="E80" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" t="s">
-        <v>418</v>
-      </c>
-      <c r="H80" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3273,157 +3228,166 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>9</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B84" t="s">
         <v>149</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C84" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>423</v>
+      </c>
+      <c r="B86" t="s">
+        <v>151</v>
+      </c>
+      <c r="C86" t="s">
+        <v>152</v>
+      </c>
+      <c r="E86" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>423</v>
+        <v>153</v>
       </c>
       <c r="B87" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C87" t="s">
-        <v>152</v>
-      </c>
-      <c r="E87" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>153</v>
+        <v>425</v>
       </c>
       <c r="B88" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C88" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>425</v>
+        <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C89" t="s">
-        <v>157</v>
+        <v>159</v>
+      </c>
+      <c r="I89" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B90" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C90" t="s">
-        <v>159</v>
-      </c>
-      <c r="I90" t="s">
-        <v>472</v>
+        <v>161</v>
+      </c>
+      <c r="E90" t="s">
+        <v>14</v>
+      </c>
+      <c r="G90" t="s">
+        <v>417</v>
+      </c>
+      <c r="H90" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>56</v>
-      </c>
-      <c r="B91" t="s">
-        <v>160</v>
-      </c>
-      <c r="C91" t="s">
-        <v>161</v>
-      </c>
-      <c r="E91" t="s">
-        <v>14</v>
-      </c>
-      <c r="G91" t="s">
-        <v>417</v>
-      </c>
-      <c r="H91" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="B92" t="s">
+        <v>163</v>
+      </c>
+      <c r="C92" t="s">
+        <v>164</v>
+      </c>
+      <c r="I92" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B93" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C93" t="s">
-        <v>164</v>
-      </c>
-      <c r="I93" t="s">
-        <v>473</v>
+        <v>166</v>
+      </c>
+      <c r="E93" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" t="s">
+        <v>507</v>
+      </c>
+      <c r="H93" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C94" t="s">
-        <v>166</v>
-      </c>
-      <c r="E94" t="s">
-        <v>14</v>
-      </c>
-      <c r="G94" t="s">
-        <v>507</v>
-      </c>
-      <c r="H94" t="s">
-        <v>167</v>
+        <v>169</v>
+      </c>
+      <c r="I94" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C95" t="s">
-        <v>169</v>
-      </c>
-      <c r="I95" t="s">
-        <v>472</v>
+        <v>171</v>
+      </c>
+      <c r="E95" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B96" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C96" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
@@ -3434,10 +3398,10 @@
         <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C97" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
@@ -3448,10 +3412,10 @@
         <v>56</v>
       </c>
       <c r="B98" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C98" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -3459,757 +3423,763 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>56</v>
-      </c>
-      <c r="B99" t="s">
-        <v>176</v>
-      </c>
-      <c r="C99" t="s">
-        <v>177</v>
-      </c>
-      <c r="E99" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>453</v>
+      </c>
+      <c r="B100" t="s">
+        <v>178</v>
+      </c>
+      <c r="C100" t="s">
+        <v>179</v>
+      </c>
+      <c r="E100" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" t="s">
+        <v>18</v>
+      </c>
+      <c r="I100" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>453</v>
+        <v>19</v>
       </c>
       <c r="B101" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C101" t="s">
-        <v>179</v>
-      </c>
-      <c r="E101" t="s">
-        <v>14</v>
-      </c>
-      <c r="F101" t="s">
-        <v>18</v>
-      </c>
-      <c r="I101" t="s">
-        <v>473</v>
+        <v>181</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>19</v>
-      </c>
-      <c r="B102" t="s">
-        <v>180</v>
-      </c>
-      <c r="C102" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>423</v>
+      </c>
+      <c r="B105" t="s">
+        <v>183</v>
+      </c>
+      <c r="C105" t="s">
+        <v>184</v>
+      </c>
+      <c r="E105" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>423</v>
+        <v>153</v>
       </c>
       <c r="B106" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C106" t="s">
-        <v>184</v>
-      </c>
-      <c r="E106" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>153</v>
+        <v>427</v>
       </c>
       <c r="B107" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C107" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>427</v>
+        <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C108" t="s">
-        <v>188</v>
+        <v>190</v>
+      </c>
+      <c r="I108" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B109" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C109" t="s">
-        <v>190</v>
-      </c>
-      <c r="I109" t="s">
-        <v>474</v>
+        <v>192</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+      <c r="G109" t="s">
+        <v>417</v>
+      </c>
+      <c r="H109" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>56</v>
-      </c>
-      <c r="B110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C110" t="s">
-        <v>192</v>
-      </c>
-      <c r="E110" t="s">
-        <v>14</v>
-      </c>
-      <c r="G110" t="s">
-        <v>417</v>
-      </c>
-      <c r="H110" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="B111" t="s">
+        <v>193</v>
+      </c>
+      <c r="C111" t="s">
+        <v>194</v>
+      </c>
+      <c r="I111" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B112" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C112" t="s">
-        <v>194</v>
-      </c>
-      <c r="I112" t="s">
-        <v>475</v>
+        <v>166</v>
+      </c>
+      <c r="E112" t="s">
+        <v>14</v>
+      </c>
+      <c r="G112" t="s">
+        <v>507</v>
+      </c>
+      <c r="H112" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>430</v>
       </c>
       <c r="B113" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C113" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
       </c>
-      <c r="G113" t="s">
-        <v>507</v>
-      </c>
-      <c r="H113" t="s">
-        <v>167</v>
+      <c r="F113" t="s">
+        <v>18</v>
+      </c>
+      <c r="I113" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>430</v>
+        <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C114" t="s">
-        <v>197</v>
-      </c>
-      <c r="E114" t="s">
-        <v>14</v>
-      </c>
-      <c r="F114" t="s">
-        <v>18</v>
-      </c>
-      <c r="I114" t="s">
-        <v>476</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>19</v>
-      </c>
-      <c r="B115" t="s">
-        <v>198</v>
-      </c>
-      <c r="C115" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>423</v>
+      </c>
+      <c r="B118" t="s">
+        <v>199</v>
+      </c>
+      <c r="C118" t="s">
+        <v>200</v>
+      </c>
+      <c r="E118" t="s">
+        <v>14</v>
+      </c>
+      <c r="F118" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>423</v>
+        <v>153</v>
       </c>
       <c r="B119" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C119" t="s">
-        <v>200</v>
-      </c>
-      <c r="E119" t="s">
-        <v>14</v>
-      </c>
-      <c r="F119" t="s">
-        <v>18</v>
+        <v>202</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>153</v>
+        <v>432</v>
       </c>
       <c r="B120" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C120" t="s">
-        <v>202</v>
+        <v>204</v>
+      </c>
+      <c r="E120" t="s">
+        <v>14</v>
+      </c>
+      <c r="F120" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>432</v>
+        <v>9</v>
       </c>
       <c r="B121" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C121" t="s">
-        <v>204</v>
-      </c>
-      <c r="E121" t="s">
-        <v>14</v>
-      </c>
-      <c r="F121" t="s">
-        <v>18</v>
+        <v>206</v>
+      </c>
+      <c r="I121" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B122" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C122" t="s">
-        <v>206</v>
-      </c>
-      <c r="I122" t="s">
-        <v>477</v>
+        <v>208</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
+      </c>
+      <c r="G122" t="s">
+        <v>417</v>
+      </c>
+      <c r="H122" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>56</v>
-      </c>
-      <c r="B123" t="s">
-        <v>207</v>
-      </c>
-      <c r="C123" t="s">
-        <v>208</v>
-      </c>
-      <c r="E123" t="s">
-        <v>14</v>
-      </c>
-      <c r="G123" t="s">
-        <v>417</v>
-      </c>
-      <c r="H123" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="B124" t="s">
+        <v>209</v>
+      </c>
+      <c r="C124" t="s">
+        <v>210</v>
+      </c>
+      <c r="I124" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B125" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C125" t="s">
-        <v>210</v>
-      </c>
-      <c r="I125" t="s">
-        <v>478</v>
+        <v>166</v>
+      </c>
+      <c r="E125" t="s">
+        <v>14</v>
+      </c>
+      <c r="G125" t="s">
+        <v>507</v>
+      </c>
+      <c r="H125" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C126" t="s">
-        <v>166</v>
-      </c>
-      <c r="E126" t="s">
-        <v>14</v>
-      </c>
-      <c r="G126" t="s">
-        <v>507</v>
-      </c>
-      <c r="H126" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>19</v>
-      </c>
-      <c r="B127" t="s">
-        <v>212</v>
-      </c>
-      <c r="C127" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>423</v>
+      </c>
+      <c r="B130" t="s">
+        <v>213</v>
+      </c>
+      <c r="C130" t="s">
+        <v>214</v>
+      </c>
+      <c r="E130" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>423</v>
+        <v>153</v>
       </c>
       <c r="B131" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C131" t="s">
-        <v>214</v>
-      </c>
-      <c r="E131" t="s">
-        <v>14</v>
-      </c>
-      <c r="F131" t="s">
-        <v>18</v>
+        <v>216</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>153</v>
+        <v>434</v>
       </c>
       <c r="B132" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C132" t="s">
-        <v>216</v>
+        <v>218</v>
+      </c>
+      <c r="E132" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>434</v>
+        <v>9</v>
       </c>
       <c r="B133" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C133" t="s">
-        <v>218</v>
-      </c>
-      <c r="E133" t="s">
-        <v>14</v>
-      </c>
-      <c r="F133" t="s">
-        <v>18</v>
+        <v>220</v>
+      </c>
+      <c r="I133" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B134" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C134" t="s">
-        <v>220</v>
-      </c>
-      <c r="I134" t="s">
-        <v>479</v>
+        <v>222</v>
+      </c>
+      <c r="E134" t="s">
+        <v>14</v>
+      </c>
+      <c r="G134" t="s">
+        <v>417</v>
+      </c>
+      <c r="H134" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>56</v>
-      </c>
-      <c r="B135" t="s">
-        <v>221</v>
-      </c>
-      <c r="C135" t="s">
-        <v>222</v>
-      </c>
-      <c r="E135" t="s">
-        <v>14</v>
-      </c>
-      <c r="G135" t="s">
-        <v>417</v>
-      </c>
-      <c r="H135" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="B136" t="s">
+        <v>223</v>
+      </c>
+      <c r="C136" t="s">
+        <v>224</v>
+      </c>
+      <c r="I136" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B137" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C137" t="s">
-        <v>224</v>
-      </c>
-      <c r="I137" t="s">
-        <v>480</v>
+        <v>166</v>
+      </c>
+      <c r="E137" t="s">
+        <v>14</v>
+      </c>
+      <c r="G137" t="s">
+        <v>507</v>
+      </c>
+      <c r="H137" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C138" t="s">
-        <v>166</v>
-      </c>
-      <c r="E138" t="s">
-        <v>14</v>
-      </c>
-      <c r="G138" t="s">
-        <v>507</v>
-      </c>
-      <c r="H138" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>19</v>
-      </c>
-      <c r="B139" t="s">
-        <v>226</v>
-      </c>
-      <c r="C139" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>423</v>
+      </c>
+      <c r="B142" t="s">
+        <v>227</v>
+      </c>
+      <c r="C142" t="s">
+        <v>228</v>
+      </c>
+      <c r="E142" t="s">
+        <v>14</v>
+      </c>
+      <c r="F142" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>423</v>
+        <v>153</v>
       </c>
       <c r="B143" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C143" t="s">
-        <v>228</v>
-      </c>
-      <c r="E143" t="s">
-        <v>14</v>
-      </c>
-      <c r="F143" t="s">
-        <v>18</v>
+        <v>230</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>153</v>
+        <v>434</v>
       </c>
       <c r="B144" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C144" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+      <c r="E144" t="s">
+        <v>14</v>
+      </c>
+      <c r="F144" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>434</v>
+        <v>9</v>
       </c>
       <c r="B145" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C145" t="s">
-        <v>232</v>
-      </c>
-      <c r="E145" t="s">
-        <v>14</v>
-      </c>
-      <c r="F145" t="s">
-        <v>18</v>
+        <v>234</v>
+      </c>
+      <c r="I145" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B146" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C146" t="s">
-        <v>234</v>
-      </c>
-      <c r="I146" t="s">
-        <v>481</v>
+        <v>236</v>
+      </c>
+      <c r="E146" t="s">
+        <v>14</v>
+      </c>
+      <c r="G146" t="s">
+        <v>417</v>
+      </c>
+      <c r="H146" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>56</v>
-      </c>
-      <c r="B147" t="s">
-        <v>235</v>
-      </c>
-      <c r="C147" t="s">
-        <v>236</v>
-      </c>
-      <c r="E147" t="s">
-        <v>14</v>
-      </c>
-      <c r="G147" t="s">
-        <v>417</v>
-      </c>
-      <c r="H147" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="B148" t="s">
+        <v>237</v>
+      </c>
+      <c r="C148" t="s">
+        <v>238</v>
+      </c>
+      <c r="I148" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B149" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C149" t="s">
-        <v>238</v>
-      </c>
-      <c r="I149" t="s">
-        <v>482</v>
+        <v>166</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
+      </c>
+      <c r="G149" t="s">
+        <v>507</v>
+      </c>
+      <c r="H149" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B150" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C150" t="s">
-        <v>166</v>
-      </c>
-      <c r="E150" t="s">
-        <v>14</v>
-      </c>
-      <c r="G150" t="s">
-        <v>507</v>
-      </c>
-      <c r="H150" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>9</v>
+        <v>454</v>
       </c>
       <c r="B151" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C151" t="s">
-        <v>241</v>
+        <v>243</v>
+      </c>
+      <c r="E151" t="s">
+        <v>14</v>
+      </c>
+      <c r="F151" t="s">
+        <v>18</v>
+      </c>
+      <c r="I151" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>454</v>
-      </c>
-      <c r="B152" t="s">
-        <v>242</v>
-      </c>
-      <c r="C152" t="s">
-        <v>243</v>
-      </c>
-      <c r="E152" t="s">
-        <v>14</v>
-      </c>
-      <c r="F152" t="s">
-        <v>18</v>
-      </c>
-      <c r="I152" t="s">
-        <v>483</v>
+        <v>42</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="B153" t="s">
+        <v>244</v>
+      </c>
+      <c r="C153" t="s">
+        <v>245</v>
+      </c>
+      <c r="I153" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>9</v>
+        <v>438</v>
       </c>
       <c r="B154" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C154" t="s">
-        <v>245</v>
-      </c>
-      <c r="I154" t="s">
-        <v>484</v>
+        <v>247</v>
+      </c>
+      <c r="E154" t="s">
+        <v>14</v>
+      </c>
+      <c r="F154" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>438</v>
-      </c>
-      <c r="B155" t="s">
-        <v>246</v>
-      </c>
-      <c r="C155" t="s">
-        <v>247</v>
-      </c>
-      <c r="E155" t="s">
-        <v>14</v>
-      </c>
-      <c r="F155" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>42</v>
+        <v>19</v>
+      </c>
+      <c r="B156" t="s">
+        <v>248</v>
+      </c>
+      <c r="C156" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>19</v>
-      </c>
-      <c r="B157" t="s">
-        <v>248</v>
-      </c>
-      <c r="C157" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>42</v>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>9</v>
+      </c>
+      <c r="B162" t="s">
+        <v>249</v>
+      </c>
+      <c r="C162" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B163" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C163" t="s">
-        <v>250</v>
+        <v>252</v>
+      </c>
+      <c r="E163" t="s">
+        <v>14</v>
+      </c>
+      <c r="G163" t="s">
+        <v>507</v>
+      </c>
+      <c r="H163" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>115</v>
+        <v>440</v>
       </c>
       <c r="B164" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C164" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E164" t="s">
         <v>14</v>
       </c>
-      <c r="G164" t="s">
-        <v>507</v>
-      </c>
-      <c r="H164" t="s">
-        <v>253</v>
+      <c r="F164" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>440</v>
+        <v>56</v>
       </c>
       <c r="B165" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C165" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E165" t="s">
         <v>14</v>
       </c>
-      <c r="F165" t="s">
-        <v>18</v>
+      <c r="G165" t="s">
+        <v>417</v>
+      </c>
+      <c r="H165" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
@@ -4217,10 +4187,10 @@
         <v>56</v>
       </c>
       <c r="B166" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C166" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E166" t="s">
         <v>14</v>
@@ -4229,154 +4199,154 @@
         <v>417</v>
       </c>
       <c r="H166" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>56</v>
+        <v>455</v>
       </c>
       <c r="B167" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C167" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E167" t="s">
         <v>14</v>
       </c>
-      <c r="G167" t="s">
-        <v>417</v>
-      </c>
-      <c r="H167" t="s">
-        <v>261</v>
+      <c r="F167" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>455</v>
+        <v>56</v>
       </c>
       <c r="B168" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C168" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E168" t="s">
         <v>14</v>
       </c>
-      <c r="F168" t="s">
-        <v>18</v>
+      <c r="G168" t="s">
+        <v>417</v>
+      </c>
+      <c r="H168" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>56</v>
+        <v>416</v>
       </c>
       <c r="B169" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C169" t="s">
-        <v>265</v>
+        <v>93</v>
       </c>
       <c r="E169" t="s">
         <v>14</v>
       </c>
-      <c r="G169" t="s">
-        <v>417</v>
-      </c>
-      <c r="H169" t="s">
-        <v>266</v>
+      <c r="F169" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>416</v>
+        <v>9</v>
       </c>
       <c r="B170" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C170" t="s">
-        <v>93</v>
-      </c>
-      <c r="E170" t="s">
-        <v>14</v>
-      </c>
-      <c r="F170" t="s">
-        <v>94</v>
+        <v>269</v>
+      </c>
+      <c r="I170" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>9</v>
+        <v>444</v>
       </c>
       <c r="B171" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C171" t="s">
-        <v>269</v>
-      </c>
-      <c r="I171" t="s">
-        <v>485</v>
+        <v>271</v>
+      </c>
+      <c r="E171" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>444</v>
+        <v>416</v>
       </c>
       <c r="B172" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C172" t="s">
-        <v>271</v>
+        <v>107</v>
       </c>
       <c r="E172" t="s">
         <v>14</v>
+      </c>
+      <c r="F172" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>416</v>
+        <v>153</v>
       </c>
       <c r="B173" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C173" t="s">
-        <v>107</v>
-      </c>
-      <c r="E173" t="s">
-        <v>14</v>
-      </c>
-      <c r="F173" t="s">
-        <v>94</v>
+        <v>274</v>
+      </c>
+      <c r="I173" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>153</v>
+        <v>456</v>
       </c>
       <c r="B174" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C174" t="s">
-        <v>274</v>
-      </c>
-      <c r="I174" t="s">
-        <v>486</v>
+        <v>276</v>
+      </c>
+      <c r="E174" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>456</v>
+        <v>56</v>
       </c>
       <c r="B175" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C175" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E175" t="s">
         <v>14</v>
+      </c>
+      <c r="G175" t="s">
+        <v>417</v>
+      </c>
+      <c r="H175" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
@@ -4384,10 +4354,10 @@
         <v>56</v>
       </c>
       <c r="B176" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C176" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E176" t="s">
         <v>14</v>
@@ -4396,32 +4366,17 @@
         <v>417</v>
       </c>
       <c r="H176" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>56</v>
-      </c>
-      <c r="B177" t="s">
-        <v>280</v>
-      </c>
-      <c r="C177" t="s">
-        <v>281</v>
-      </c>
-      <c r="E177" t="s">
-        <v>14</v>
-      </c>
-      <c r="G177" t="s">
-        <v>417</v>
-      </c>
-      <c r="H177" t="s">
-        <v>282</v>
+        <v>182</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>182</v>
+        <v>42</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
@@ -4429,20 +4384,32 @@
         <v>42</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
-        <v>42</v>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>9</v>
+      </c>
+      <c r="B181" t="s">
+        <v>283</v>
+      </c>
+      <c r="C181" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="B182" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C182" t="s">
-        <v>284</v>
+        <v>286</v>
+      </c>
+      <c r="E182" t="s">
+        <v>14</v>
+      </c>
+      <c r="F182" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
@@ -4450,159 +4417,147 @@
         <v>416</v>
       </c>
       <c r="B183" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C183" t="s">
-        <v>286</v>
+        <v>93</v>
       </c>
       <c r="E183" t="s">
         <v>14</v>
       </c>
       <c r="F183" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>416</v>
+        <v>9</v>
       </c>
       <c r="B184" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C184" t="s">
-        <v>93</v>
-      </c>
-      <c r="E184" t="s">
-        <v>14</v>
-      </c>
-      <c r="F184" t="s">
-        <v>94</v>
+        <v>289</v>
+      </c>
+      <c r="I184" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B185" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C185" t="s">
-        <v>289</v>
-      </c>
-      <c r="I185" t="s">
-        <v>487</v>
+        <v>291</v>
+      </c>
+      <c r="E185" t="s">
+        <v>14</v>
+      </c>
+      <c r="G185" t="s">
+        <v>417</v>
+      </c>
+      <c r="H185" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>56</v>
+        <v>416</v>
       </c>
       <c r="B186" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C186" t="s">
-        <v>291</v>
+        <v>107</v>
       </c>
       <c r="E186" t="s">
         <v>14</v>
       </c>
-      <c r="G186" t="s">
-        <v>417</v>
-      </c>
-      <c r="H186" t="s">
-        <v>292</v>
+      <c r="F186" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>416</v>
+        <v>9</v>
       </c>
       <c r="B187" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C187" t="s">
-        <v>107</v>
-      </c>
-      <c r="E187" t="s">
-        <v>14</v>
-      </c>
-      <c r="F187" t="s">
-        <v>94</v>
+        <v>295</v>
+      </c>
+      <c r="I187" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B188" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C188" t="s">
-        <v>295</v>
-      </c>
-      <c r="I188" t="s">
-        <v>488</v>
+        <v>297</v>
+      </c>
+      <c r="E188" t="s">
+        <v>14</v>
+      </c>
+      <c r="G188" t="s">
+        <v>509</v>
+      </c>
+      <c r="H188" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B189" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C189" t="s">
-        <v>297</v>
-      </c>
-      <c r="E189" t="s">
-        <v>14</v>
-      </c>
-      <c r="G189" t="s">
-        <v>509</v>
-      </c>
-      <c r="H189" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>153</v>
+        <v>56</v>
       </c>
       <c r="B190" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C190" t="s">
-        <v>300</v>
+        <v>302</v>
+      </c>
+      <c r="E190" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B191" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C191" t="s">
-        <v>302</v>
-      </c>
-      <c r="E191" t="s">
-        <v>14</v>
+        <v>304</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>19</v>
-      </c>
-      <c r="B192" t="s">
-        <v>303</v>
-      </c>
-      <c r="C192" t="s">
-        <v>304</v>
+        <v>182</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>182</v>
+        <v>42</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
@@ -4612,11 +4567,6 @@
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed the type of field in farm location for latitude and longitude
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$196</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="523">
   <si>
     <t>type</t>
   </si>
@@ -1557,6 +1557,33 @@
     <t>(decimal-date-time(.) &gt; decimal-date-time(${transfer_date}))</t>
   </si>
   <si>
+    <t>farm_location_lon</t>
+  </si>
+  <si>
+    <t>Latitud de la finca</t>
+  </si>
+  <si>
+    <t>Longitud de la finca</t>
+  </si>
+  <si>
+    <t>number(pulldata('farm','lat', 'farm_key', ${farm_id}))</t>
+  </si>
+  <si>
+    <t>number(pulldata('farm','lon', 'farm_key', ${farm_id}))</t>
+  </si>
+  <si>
+    <t>(. &gt;= -90) and (. &lt;= 90)</t>
+  </si>
+  <si>
+    <t>(. &gt;= -180) and (. &lt;= 180)</t>
+  </si>
+  <si>
+    <t>La latitud debe ser un campo numérico entre -90 y 90</t>
+  </si>
+  <si>
+    <t>La longitud debe ser un campo numérico entre -180 y 180</t>
+  </si>
+  <si>
     <t>El número de identificación debe ser numérico y no tener espacios en blanco al final</t>
   </si>
   <si>
@@ -1567,9 +1594,6 @@
   </si>
   <si>
     <t>farm_location</t>
-  </si>
-  <si>
-    <t>Ubicación de la finca</t>
   </si>
 </sst>
 </file>
@@ -1975,11 +1999,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L195"/>
+  <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2088,7 +2112,7 @@
         <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2108,7 +2132,7 @@
         <v>401</v>
       </c>
       <c r="H6" t="s">
-        <v>511</v>
+        <v>520</v>
       </c>
       <c r="J6" t="s">
         <v>490</v>
@@ -2131,7 +2155,7 @@
         <v>401</v>
       </c>
       <c r="H7" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="J7" t="s">
         <v>491</v>
@@ -2324,7 +2348,7 @@
         <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2344,7 +2368,7 @@
         <v>401</v>
       </c>
       <c r="H20" t="s">
-        <v>511</v>
+        <v>520</v>
       </c>
       <c r="J20" t="s">
         <v>497</v>
@@ -2367,7 +2391,7 @@
         <v>401</v>
       </c>
       <c r="H21" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="J21" t="s">
         <v>498</v>
@@ -2565,292 +2589,298 @@
         <v>61</v>
       </c>
       <c r="B34" t="s">
+        <v>522</v>
+      </c>
+      <c r="C34" t="s">
+        <v>511</v>
+      </c>
+      <c r="E34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
+        <v>515</v>
+      </c>
+      <c r="H34" t="s">
+        <v>517</v>
+      </c>
+      <c r="J34" t="s">
         <v>513</v>
-      </c>
-      <c r="C34" t="s">
-        <v>514</v>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" t="s">
-        <v>14</v>
-      </c>
-      <c r="L34" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>510</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>512</v>
+      </c>
+      <c r="E35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>516</v>
+      </c>
+      <c r="H35" t="s">
+        <v>518</v>
       </c>
       <c r="J35" t="s">
-        <v>505</v>
+        <v>514</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>410</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
-      </c>
-      <c r="E36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="J36" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>410</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="E41" t="s">
         <v>14</v>
-      </c>
-      <c r="L41" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="L42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>448</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
-      </c>
-      <c r="E45" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>448</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
         <v>14</v>
       </c>
-      <c r="I46" t="s">
-        <v>466</v>
+      <c r="F46" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>449</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="D47" t="s">
+        <v>17</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
       </c>
-      <c r="F47" t="s">
-        <v>77</v>
+      <c r="I47" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
+      </c>
+      <c r="F48" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>450</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
-      </c>
-      <c r="I49" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>416</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
       </c>
-      <c r="F50" t="s">
-        <v>88</v>
+      <c r="I50" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>416</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
       </c>
-      <c r="G51" t="s">
-        <v>417</v>
-      </c>
-      <c r="H51" t="s">
-        <v>91</v>
+      <c r="F51" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>416</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E52" t="s">
         <v>14</v>
       </c>
-      <c r="F52" t="s">
-        <v>94</v>
+      <c r="G52" t="s">
+        <v>417</v>
+      </c>
+      <c r="H52" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
-      </c>
-      <c r="I53" t="s">
-        <v>465</v>
+        <v>93</v>
+      </c>
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C54" t="s">
-        <v>98</v>
-      </c>
-      <c r="E54" t="s">
-        <v>14</v>
-      </c>
-      <c r="G54" t="s">
-        <v>417</v>
-      </c>
-      <c r="H54" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="I54" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -2858,10 +2888,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -2870,7 +2900,7 @@
         <v>417</v>
       </c>
       <c r="H55" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2878,10 +2908,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -2890,63 +2920,78 @@
         <v>417</v>
       </c>
       <c r="H56" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>416</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
       </c>
-      <c r="F57" t="s">
-        <v>94</v>
+      <c r="G57" t="s">
+        <v>417</v>
+      </c>
+      <c r="H57" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
-      </c>
-      <c r="I58" t="s">
-        <v>468</v>
+        <v>107</v>
+      </c>
+      <c r="E58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C59" t="s">
-        <v>112</v>
-      </c>
-      <c r="E59" t="s">
-        <v>14</v>
-      </c>
-      <c r="G59" t="s">
-        <v>418</v>
-      </c>
-      <c r="H59" t="s">
-        <v>419</v>
+        <v>109</v>
+      </c>
+      <c r="I59" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>110</v>
+      </c>
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" t="s">
+        <v>418</v>
+      </c>
+      <c r="H60" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -2959,173 +3004,158 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>9</v>
-      </c>
-      <c r="B64" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" t="s">
-        <v>114</v>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C65" t="s">
-        <v>117</v>
-      </c>
-      <c r="E65" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>451</v>
+        <v>115</v>
       </c>
       <c r="B66" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C66" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E66" t="s">
         <v>14</v>
-      </c>
-      <c r="F66" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>451</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C67" t="s">
-        <v>121</v>
-      </c>
-      <c r="I67" t="s">
-        <v>469</v>
+        <v>119</v>
+      </c>
+      <c r="E67" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>452</v>
+        <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C68" t="s">
-        <v>123</v>
-      </c>
-      <c r="E68" t="s">
-        <v>14</v>
+        <v>121</v>
+      </c>
+      <c r="I68" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>115</v>
+        <v>452</v>
       </c>
       <c r="B69" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E69" t="s">
         <v>14</v>
-      </c>
-      <c r="G69" t="s">
-        <v>507</v>
-      </c>
-      <c r="H69" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>115</v>
+      </c>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s">
+        <v>125</v>
+      </c>
+      <c r="E70" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" t="s">
+        <v>507</v>
+      </c>
+      <c r="H70" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>56</v>
-      </c>
-      <c r="B71" t="s">
-        <v>127</v>
-      </c>
-      <c r="C71" t="s">
-        <v>128</v>
-      </c>
-      <c r="D71" t="s">
-        <v>17</v>
-      </c>
-      <c r="E71" t="s">
-        <v>14</v>
-      </c>
-      <c r="G71" t="s">
-        <v>417</v>
-      </c>
-      <c r="H71" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>416</v>
+        <v>56</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C72" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="D72" t="s">
+        <v>17</v>
       </c>
       <c r="E72" t="s">
         <v>14</v>
       </c>
-      <c r="F72" t="s">
-        <v>94</v>
+      <c r="G72" t="s">
+        <v>417</v>
+      </c>
+      <c r="H72" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="B73" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C73" t="s">
-        <v>133</v>
-      </c>
-      <c r="I73" t="s">
-        <v>470</v>
+        <v>131</v>
+      </c>
+      <c r="E73" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C74" t="s">
-        <v>135</v>
-      </c>
-      <c r="E74" t="s">
-        <v>14</v>
-      </c>
-      <c r="G74" t="s">
-        <v>507</v>
-      </c>
-      <c r="H74" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="I74" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -3133,89 +3163,104 @@
         <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E75" t="s">
         <v>14</v>
       </c>
       <c r="G75" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H75" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C76" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
+      </c>
+      <c r="G76" t="s">
+        <v>508</v>
+      </c>
+      <c r="H76" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>416</v>
+        <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E77" t="s">
         <v>14</v>
-      </c>
-      <c r="F77" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>145</v>
-      </c>
-      <c r="I78" t="s">
-        <v>471</v>
+        <v>143</v>
+      </c>
+      <c r="E78" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C79" t="s">
-        <v>147</v>
-      </c>
-      <c r="E79" t="s">
-        <v>14</v>
-      </c>
-      <c r="G79" t="s">
-        <v>418</v>
-      </c>
-      <c r="H79" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="I79" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>110</v>
+      </c>
+      <c r="B80" t="s">
+        <v>146</v>
+      </c>
+      <c r="C80" t="s">
+        <v>147</v>
+      </c>
+      <c r="E80" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" t="s">
+        <v>418</v>
+      </c>
+      <c r="H80" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3228,166 +3273,157 @@
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>9</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>149</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>423</v>
-      </c>
-      <c r="B86" t="s">
-        <v>151</v>
-      </c>
-      <c r="C86" t="s">
-        <v>152</v>
-      </c>
-      <c r="E86" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>423</v>
       </c>
       <c r="B87" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C87" t="s">
-        <v>155</v>
+        <v>152</v>
+      </c>
+      <c r="E87" t="s">
+        <v>14</v>
+      </c>
+      <c r="F87" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>425</v>
+        <v>153</v>
       </c>
       <c r="B88" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C88" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>425</v>
       </c>
       <c r="B89" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C89" t="s">
-        <v>159</v>
-      </c>
-      <c r="I89" t="s">
-        <v>472</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C90" t="s">
-        <v>161</v>
-      </c>
-      <c r="E90" t="s">
-        <v>14</v>
-      </c>
-      <c r="G90" t="s">
-        <v>417</v>
-      </c>
-      <c r="H90" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="I90" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="B91" t="s">
+        <v>160</v>
+      </c>
+      <c r="C91" t="s">
+        <v>161</v>
+      </c>
+      <c r="E91" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" t="s">
+        <v>417</v>
+      </c>
+      <c r="H91" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" t="s">
-        <v>163</v>
-      </c>
-      <c r="C92" t="s">
-        <v>164</v>
-      </c>
-      <c r="I92" t="s">
-        <v>473</v>
+        <v>42</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C93" t="s">
-        <v>166</v>
-      </c>
-      <c r="E93" t="s">
-        <v>14</v>
-      </c>
-      <c r="G93" t="s">
-        <v>507</v>
-      </c>
-      <c r="H93" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="I93" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B94" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C94" t="s">
-        <v>169</v>
-      </c>
-      <c r="I94" t="s">
-        <v>472</v>
+        <v>166</v>
+      </c>
+      <c r="E94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" t="s">
+        <v>507</v>
+      </c>
+      <c r="H94" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B95" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C95" t="s">
-        <v>171</v>
-      </c>
-      <c r="E95" t="s">
-        <v>14</v>
+        <v>169</v>
+      </c>
+      <c r="I95" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C96" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
@@ -3398,10 +3434,10 @@
         <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C97" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
@@ -3412,10 +3448,10 @@
         <v>56</v>
       </c>
       <c r="B98" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C98" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -3423,763 +3459,757 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="B99" t="s">
+        <v>176</v>
+      </c>
+      <c r="C99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E99" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>453</v>
-      </c>
-      <c r="B100" t="s">
-        <v>178</v>
-      </c>
-      <c r="C100" t="s">
-        <v>179</v>
-      </c>
-      <c r="E100" t="s">
-        <v>14</v>
-      </c>
-      <c r="F100" t="s">
-        <v>18</v>
-      </c>
-      <c r="I100" t="s">
-        <v>473</v>
+        <v>42</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>19</v>
+        <v>453</v>
       </c>
       <c r="B101" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C101" t="s">
-        <v>181</v>
+        <v>179</v>
+      </c>
+      <c r="E101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F101" t="s">
+        <v>18</v>
+      </c>
+      <c r="I101" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>42</v>
+        <v>19</v>
+      </c>
+      <c r="B102" t="s">
+        <v>180</v>
+      </c>
+      <c r="C102" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>423</v>
-      </c>
-      <c r="B105" t="s">
-        <v>183</v>
-      </c>
-      <c r="C105" t="s">
-        <v>184</v>
-      </c>
-      <c r="E105" t="s">
-        <v>14</v>
-      </c>
-      <c r="F105" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>153</v>
+        <v>423</v>
       </c>
       <c r="B106" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C106" t="s">
-        <v>186</v>
+        <v>184</v>
+      </c>
+      <c r="E106" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>427</v>
+        <v>153</v>
       </c>
       <c r="B107" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C107" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>9</v>
+        <v>427</v>
       </c>
       <c r="B108" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C108" t="s">
-        <v>190</v>
-      </c>
-      <c r="I108" t="s">
-        <v>474</v>
+        <v>188</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B109" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C109" t="s">
-        <v>192</v>
-      </c>
-      <c r="E109" t="s">
-        <v>14</v>
-      </c>
-      <c r="G109" t="s">
-        <v>417</v>
-      </c>
-      <c r="H109" t="s">
-        <v>162</v>
+        <v>190</v>
+      </c>
+      <c r="I109" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="B110" t="s">
+        <v>191</v>
+      </c>
+      <c r="C110" t="s">
+        <v>192</v>
+      </c>
+      <c r="E110" t="s">
+        <v>14</v>
+      </c>
+      <c r="G110" t="s">
+        <v>417</v>
+      </c>
+      <c r="H110" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>9</v>
-      </c>
-      <c r="B111" t="s">
-        <v>193</v>
-      </c>
-      <c r="C111" t="s">
-        <v>194</v>
-      </c>
-      <c r="I111" t="s">
-        <v>475</v>
+        <v>42</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C112" t="s">
-        <v>166</v>
-      </c>
-      <c r="E112" t="s">
-        <v>14</v>
-      </c>
-      <c r="G112" t="s">
-        <v>507</v>
-      </c>
-      <c r="H112" t="s">
-        <v>167</v>
+        <v>194</v>
+      </c>
+      <c r="I112" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>430</v>
+        <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C113" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
       </c>
-      <c r="F113" t="s">
-        <v>18</v>
-      </c>
-      <c r="I113" t="s">
-        <v>476</v>
+      <c r="G113" t="s">
+        <v>507</v>
+      </c>
+      <c r="H113" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>19</v>
+        <v>430</v>
       </c>
       <c r="B114" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C114" t="s">
-        <v>181</v>
+        <v>197</v>
+      </c>
+      <c r="E114" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114" t="s">
+        <v>18</v>
+      </c>
+      <c r="I114" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>42</v>
+        <v>19</v>
+      </c>
+      <c r="B115" t="s">
+        <v>198</v>
+      </c>
+      <c r="C115" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>423</v>
-      </c>
-      <c r="B118" t="s">
-        <v>199</v>
-      </c>
-      <c r="C118" t="s">
-        <v>200</v>
-      </c>
-      <c r="E118" t="s">
-        <v>14</v>
-      </c>
-      <c r="F118" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>153</v>
+        <v>423</v>
       </c>
       <c r="B119" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C119" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="E119" t="s">
+        <v>14</v>
+      </c>
+      <c r="F119" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>432</v>
+        <v>153</v>
       </c>
       <c r="B120" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C120" t="s">
-        <v>204</v>
-      </c>
-      <c r="E120" t="s">
-        <v>14</v>
-      </c>
-      <c r="F120" t="s">
-        <v>18</v>
+        <v>202</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>9</v>
+        <v>432</v>
       </c>
       <c r="B121" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C121" t="s">
-        <v>206</v>
-      </c>
-      <c r="I121" t="s">
-        <v>477</v>
+        <v>204</v>
+      </c>
+      <c r="E121" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C122" t="s">
-        <v>208</v>
-      </c>
-      <c r="E122" t="s">
-        <v>14</v>
-      </c>
-      <c r="G122" t="s">
-        <v>417</v>
-      </c>
-      <c r="H122" t="s">
-        <v>162</v>
+        <v>206</v>
+      </c>
+      <c r="I122" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="B123" t="s">
+        <v>207</v>
+      </c>
+      <c r="C123" t="s">
+        <v>208</v>
+      </c>
+      <c r="E123" t="s">
+        <v>14</v>
+      </c>
+      <c r="G123" t="s">
+        <v>417</v>
+      </c>
+      <c r="H123" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>9</v>
-      </c>
-      <c r="B124" t="s">
-        <v>209</v>
-      </c>
-      <c r="C124" t="s">
-        <v>210</v>
-      </c>
-      <c r="I124" t="s">
-        <v>478</v>
+        <v>42</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C125" t="s">
-        <v>166</v>
-      </c>
-      <c r="E125" t="s">
-        <v>14</v>
-      </c>
-      <c r="G125" t="s">
-        <v>507</v>
-      </c>
-      <c r="H125" t="s">
-        <v>167</v>
+        <v>210</v>
+      </c>
+      <c r="I125" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="B126" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C126" t="s">
-        <v>181</v>
+        <v>166</v>
+      </c>
+      <c r="E126" t="s">
+        <v>14</v>
+      </c>
+      <c r="G126" t="s">
+        <v>507</v>
+      </c>
+      <c r="H126" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>42</v>
+        <v>19</v>
+      </c>
+      <c r="B127" t="s">
+        <v>212</v>
+      </c>
+      <c r="C127" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>423</v>
-      </c>
-      <c r="B130" t="s">
-        <v>213</v>
-      </c>
-      <c r="C130" t="s">
-        <v>214</v>
-      </c>
-      <c r="E130" t="s">
-        <v>14</v>
-      </c>
-      <c r="F130" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>153</v>
+        <v>423</v>
       </c>
       <c r="B131" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C131" t="s">
-        <v>216</v>
+        <v>214</v>
+      </c>
+      <c r="E131" t="s">
+        <v>14</v>
+      </c>
+      <c r="F131" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>434</v>
+        <v>153</v>
       </c>
       <c r="B132" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C132" t="s">
-        <v>218</v>
-      </c>
-      <c r="E132" t="s">
-        <v>14</v>
-      </c>
-      <c r="F132" t="s">
-        <v>18</v>
+        <v>216</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>9</v>
+        <v>434</v>
       </c>
       <c r="B133" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C133" t="s">
-        <v>220</v>
-      </c>
-      <c r="I133" t="s">
-        <v>479</v>
+        <v>218</v>
+      </c>
+      <c r="E133" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B134" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C134" t="s">
-        <v>222</v>
-      </c>
-      <c r="E134" t="s">
-        <v>14</v>
-      </c>
-      <c r="G134" t="s">
-        <v>417</v>
-      </c>
-      <c r="H134" t="s">
-        <v>162</v>
+        <v>220</v>
+      </c>
+      <c r="I134" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="B135" t="s">
+        <v>221</v>
+      </c>
+      <c r="C135" t="s">
+        <v>222</v>
+      </c>
+      <c r="E135" t="s">
+        <v>14</v>
+      </c>
+      <c r="G135" t="s">
+        <v>417</v>
+      </c>
+      <c r="H135" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>9</v>
-      </c>
-      <c r="B136" t="s">
-        <v>223</v>
-      </c>
-      <c r="C136" t="s">
-        <v>224</v>
-      </c>
-      <c r="I136" t="s">
-        <v>480</v>
+        <v>42</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C137" t="s">
-        <v>166</v>
-      </c>
-      <c r="E137" t="s">
-        <v>14</v>
-      </c>
-      <c r="G137" t="s">
-        <v>507</v>
-      </c>
-      <c r="H137" t="s">
-        <v>167</v>
+        <v>224</v>
+      </c>
+      <c r="I137" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="B138" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C138" t="s">
-        <v>181</v>
+        <v>166</v>
+      </c>
+      <c r="E138" t="s">
+        <v>14</v>
+      </c>
+      <c r="G138" t="s">
+        <v>507</v>
+      </c>
+      <c r="H138" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>42</v>
+        <v>19</v>
+      </c>
+      <c r="B139" t="s">
+        <v>226</v>
+      </c>
+      <c r="C139" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>423</v>
-      </c>
-      <c r="B142" t="s">
-        <v>227</v>
-      </c>
-      <c r="C142" t="s">
-        <v>228</v>
-      </c>
-      <c r="E142" t="s">
-        <v>14</v>
-      </c>
-      <c r="F142" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>153</v>
+        <v>423</v>
       </c>
       <c r="B143" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C143" t="s">
-        <v>230</v>
+        <v>228</v>
+      </c>
+      <c r="E143" t="s">
+        <v>14</v>
+      </c>
+      <c r="F143" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>434</v>
+        <v>153</v>
       </c>
       <c r="B144" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C144" t="s">
-        <v>232</v>
-      </c>
-      <c r="E144" t="s">
-        <v>14</v>
-      </c>
-      <c r="F144" t="s">
-        <v>18</v>
+        <v>230</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>9</v>
+        <v>434</v>
       </c>
       <c r="B145" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C145" t="s">
-        <v>234</v>
-      </c>
-      <c r="I145" t="s">
-        <v>481</v>
+        <v>232</v>
+      </c>
+      <c r="E145" t="s">
+        <v>14</v>
+      </c>
+      <c r="F145" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B146" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C146" t="s">
-        <v>236</v>
-      </c>
-      <c r="E146" t="s">
-        <v>14</v>
-      </c>
-      <c r="G146" t="s">
-        <v>417</v>
-      </c>
-      <c r="H146" t="s">
-        <v>162</v>
+        <v>234</v>
+      </c>
+      <c r="I146" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="B147" t="s">
+        <v>235</v>
+      </c>
+      <c r="C147" t="s">
+        <v>236</v>
+      </c>
+      <c r="E147" t="s">
+        <v>14</v>
+      </c>
+      <c r="G147" t="s">
+        <v>417</v>
+      </c>
+      <c r="H147" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>9</v>
-      </c>
-      <c r="B148" t="s">
-        <v>237</v>
-      </c>
-      <c r="C148" t="s">
-        <v>238</v>
-      </c>
-      <c r="I148" t="s">
-        <v>482</v>
+        <v>42</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B149" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C149" t="s">
-        <v>166</v>
-      </c>
-      <c r="E149" t="s">
-        <v>14</v>
-      </c>
-      <c r="G149" t="s">
-        <v>507</v>
-      </c>
-      <c r="H149" t="s">
-        <v>167</v>
+        <v>238</v>
+      </c>
+      <c r="I149" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B150" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C150" t="s">
-        <v>241</v>
+        <v>166</v>
+      </c>
+      <c r="E150" t="s">
+        <v>14</v>
+      </c>
+      <c r="G150" t="s">
+        <v>507</v>
+      </c>
+      <c r="H150" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>454</v>
+        <v>9</v>
       </c>
       <c r="B151" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C151" t="s">
-        <v>243</v>
-      </c>
-      <c r="E151" t="s">
-        <v>14</v>
-      </c>
-      <c r="F151" t="s">
-        <v>18</v>
-      </c>
-      <c r="I151" t="s">
-        <v>483</v>
+        <v>241</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>42</v>
+        <v>454</v>
+      </c>
+      <c r="B152" t="s">
+        <v>242</v>
+      </c>
+      <c r="C152" t="s">
+        <v>243</v>
+      </c>
+      <c r="E152" t="s">
+        <v>14</v>
+      </c>
+      <c r="F152" t="s">
+        <v>18</v>
+      </c>
+      <c r="I152" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>9</v>
-      </c>
-      <c r="B153" t="s">
-        <v>244</v>
-      </c>
-      <c r="C153" t="s">
-        <v>245</v>
-      </c>
-      <c r="I153" t="s">
-        <v>484</v>
+        <v>42</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>438</v>
+        <v>9</v>
       </c>
       <c r="B154" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C154" t="s">
-        <v>247</v>
-      </c>
-      <c r="E154" t="s">
-        <v>14</v>
-      </c>
-      <c r="F154" t="s">
-        <v>18</v>
+        <v>245</v>
+      </c>
+      <c r="I154" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>42</v>
+        <v>438</v>
+      </c>
+      <c r="B155" t="s">
+        <v>246</v>
+      </c>
+      <c r="C155" t="s">
+        <v>247</v>
+      </c>
+      <c r="E155" t="s">
+        <v>14</v>
+      </c>
+      <c r="F155" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>19</v>
-      </c>
-      <c r="B156" t="s">
-        <v>248</v>
-      </c>
-      <c r="C156" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>42</v>
+        <v>19</v>
+      </c>
+      <c r="B157" t="s">
+        <v>248</v>
+      </c>
+      <c r="C157" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>9</v>
-      </c>
-      <c r="B162" t="s">
-        <v>249</v>
-      </c>
-      <c r="C162" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B163" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C163" t="s">
-        <v>252</v>
-      </c>
-      <c r="E163" t="s">
-        <v>14</v>
-      </c>
-      <c r="G163" t="s">
-        <v>507</v>
-      </c>
-      <c r="H163" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>440</v>
+        <v>115</v>
       </c>
       <c r="B164" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C164" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E164" t="s">
         <v>14</v>
       </c>
-      <c r="F164" t="s">
-        <v>18</v>
+      <c r="G164" t="s">
+        <v>507</v>
+      </c>
+      <c r="H164" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>56</v>
+        <v>440</v>
       </c>
       <c r="B165" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C165" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E165" t="s">
         <v>14</v>
       </c>
-      <c r="G165" t="s">
-        <v>417</v>
-      </c>
-      <c r="H165" t="s">
-        <v>258</v>
+      <c r="F165" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
@@ -4187,10 +4217,10 @@
         <v>56</v>
       </c>
       <c r="B166" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C166" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E166" t="s">
         <v>14</v>
@@ -4199,154 +4229,154 @@
         <v>417</v>
       </c>
       <c r="H166" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>455</v>
+        <v>56</v>
       </c>
       <c r="B167" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C167" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E167" t="s">
         <v>14</v>
       </c>
-      <c r="F167" t="s">
-        <v>18</v>
+      <c r="G167" t="s">
+        <v>417</v>
+      </c>
+      <c r="H167" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>56</v>
+        <v>455</v>
       </c>
       <c r="B168" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C168" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E168" t="s">
         <v>14</v>
       </c>
-      <c r="G168" t="s">
-        <v>417</v>
-      </c>
-      <c r="H168" t="s">
-        <v>266</v>
+      <c r="F168" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>416</v>
+        <v>56</v>
       </c>
       <c r="B169" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C169" t="s">
-        <v>93</v>
+        <v>265</v>
       </c>
       <c r="E169" t="s">
         <v>14</v>
       </c>
-      <c r="F169" t="s">
-        <v>94</v>
+      <c r="G169" t="s">
+        <v>417</v>
+      </c>
+      <c r="H169" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="B170" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C170" t="s">
-        <v>269</v>
-      </c>
-      <c r="I170" t="s">
-        <v>485</v>
+        <v>93</v>
+      </c>
+      <c r="E170" t="s">
+        <v>14</v>
+      </c>
+      <c r="F170" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>444</v>
+        <v>9</v>
       </c>
       <c r="B171" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C171" t="s">
-        <v>271</v>
-      </c>
-      <c r="E171" t="s">
-        <v>14</v>
+        <v>269</v>
+      </c>
+      <c r="I171" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>416</v>
+        <v>444</v>
       </c>
       <c r="B172" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C172" t="s">
-        <v>107</v>
+        <v>271</v>
       </c>
       <c r="E172" t="s">
         <v>14</v>
-      </c>
-      <c r="F172" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>153</v>
+        <v>416</v>
       </c>
       <c r="B173" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C173" t="s">
-        <v>274</v>
-      </c>
-      <c r="I173" t="s">
-        <v>486</v>
+        <v>107</v>
+      </c>
+      <c r="E173" t="s">
+        <v>14</v>
+      </c>
+      <c r="F173" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>456</v>
+        <v>153</v>
       </c>
       <c r="B174" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C174" t="s">
-        <v>276</v>
-      </c>
-      <c r="E174" t="s">
-        <v>14</v>
+        <v>274</v>
+      </c>
+      <c r="I174" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>56</v>
+        <v>456</v>
       </c>
       <c r="B175" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C175" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E175" t="s">
         <v>14</v>
-      </c>
-      <c r="G175" t="s">
-        <v>417</v>
-      </c>
-      <c r="H175" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
@@ -4354,10 +4384,10 @@
         <v>56</v>
       </c>
       <c r="B176" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C176" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E176" t="s">
         <v>14</v>
@@ -4366,17 +4396,32 @@
         <v>417</v>
       </c>
       <c r="H176" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>182</v>
+        <v>56</v>
+      </c>
+      <c r="B177" t="s">
+        <v>280</v>
+      </c>
+      <c r="C177" t="s">
+        <v>281</v>
+      </c>
+      <c r="E177" t="s">
+        <v>14</v>
+      </c>
+      <c r="G177" t="s">
+        <v>417</v>
+      </c>
+      <c r="H177" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>42</v>
+        <v>182</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
@@ -4384,32 +4429,20 @@
         <v>42</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A181" t="s">
-        <v>9</v>
-      </c>
-      <c r="B181" t="s">
-        <v>283</v>
-      </c>
-      <c r="C181" t="s">
-        <v>284</v>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>416</v>
+        <v>9</v>
       </c>
       <c r="B182" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C182" t="s">
-        <v>286</v>
-      </c>
-      <c r="E182" t="s">
-        <v>14</v>
-      </c>
-      <c r="F182" t="s">
-        <v>88</v>
+        <v>284</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
@@ -4417,147 +4450,159 @@
         <v>416</v>
       </c>
       <c r="B183" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C183" t="s">
-        <v>93</v>
+        <v>286</v>
       </c>
       <c r="E183" t="s">
         <v>14</v>
       </c>
       <c r="F183" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="B184" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C184" t="s">
-        <v>289</v>
-      </c>
-      <c r="I184" t="s">
-        <v>487</v>
+        <v>93</v>
+      </c>
+      <c r="E184" t="s">
+        <v>14</v>
+      </c>
+      <c r="F184" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B185" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C185" t="s">
-        <v>291</v>
-      </c>
-      <c r="E185" t="s">
-        <v>14</v>
-      </c>
-      <c r="G185" t="s">
-        <v>417</v>
-      </c>
-      <c r="H185" t="s">
-        <v>292</v>
+        <v>289</v>
+      </c>
+      <c r="I185" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>416</v>
+        <v>56</v>
       </c>
       <c r="B186" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C186" t="s">
-        <v>107</v>
+        <v>291</v>
       </c>
       <c r="E186" t="s">
         <v>14</v>
       </c>
-      <c r="F186" t="s">
-        <v>94</v>
+      <c r="G186" t="s">
+        <v>417</v>
+      </c>
+      <c r="H186" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="B187" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C187" t="s">
-        <v>295</v>
-      </c>
-      <c r="I187" t="s">
-        <v>488</v>
+        <v>107</v>
+      </c>
+      <c r="E187" t="s">
+        <v>14</v>
+      </c>
+      <c r="F187" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="B188" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C188" t="s">
-        <v>297</v>
-      </c>
-      <c r="E188" t="s">
-        <v>14</v>
-      </c>
-      <c r="G188" t="s">
-        <v>509</v>
-      </c>
-      <c r="H188" t="s">
-        <v>298</v>
+        <v>295</v>
+      </c>
+      <c r="I188" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="B189" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C189" t="s">
-        <v>300</v>
+        <v>297</v>
+      </c>
+      <c r="E189" t="s">
+        <v>14</v>
+      </c>
+      <c r="G189" t="s">
+        <v>509</v>
+      </c>
+      <c r="H189" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>56</v>
+        <v>153</v>
       </c>
       <c r="B190" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C190" t="s">
-        <v>302</v>
-      </c>
-      <c r="E190" t="s">
-        <v>14</v>
+        <v>300</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B191" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C191" t="s">
-        <v>304</v>
+        <v>302</v>
+      </c>
+      <c r="E191" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>182</v>
+        <v>19</v>
+      </c>
+      <c r="B192" t="s">
+        <v>303</v>
+      </c>
+      <c r="C192" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>42</v>
+        <v>182</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
@@ -4567,6 +4612,11 @@
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
the message about farm coordinates was improved
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -1560,12 +1560,6 @@
     <t>farm_location_lon</t>
   </si>
   <si>
-    <t>Latitud de la finca</t>
-  </si>
-  <si>
-    <t>Longitud de la finca</t>
-  </si>
-  <si>
     <t>number(pulldata('farm','lat', 'farm_key', ${farm_id}))</t>
   </si>
   <si>
@@ -1594,6 +1588,12 @@
   </si>
   <si>
     <t>farm_location</t>
+  </si>
+  <si>
+    <t>Latitud de la finca (coordenadas geograficas [-90,90])</t>
+  </si>
+  <si>
+    <t>Longitud de la finca (coordenadas geograficas [-180,180])</t>
   </si>
 </sst>
 </file>
@@ -2002,8 +2002,8 @@
   <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2112,7 +2112,7 @@
         <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2132,7 +2132,7 @@
         <v>401</v>
       </c>
       <c r="H6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J6" t="s">
         <v>490</v>
@@ -2155,7 +2155,7 @@
         <v>401</v>
       </c>
       <c r="H7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="J7" t="s">
         <v>491</v>
@@ -2348,7 +2348,7 @@
         <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2368,7 +2368,7 @@
         <v>401</v>
       </c>
       <c r="H20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J20" t="s">
         <v>497</v>
@@ -2391,7 +2391,7 @@
         <v>401</v>
       </c>
       <c r="H21" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="J21" t="s">
         <v>498</v>
@@ -2589,22 +2589,22 @@
         <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C34" t="s">
+        <v>521</v>
+      </c>
+      <c r="E34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
+        <v>513</v>
+      </c>
+      <c r="H34" t="s">
+        <v>515</v>
+      </c>
+      <c r="J34" t="s">
         <v>511</v>
-      </c>
-      <c r="E34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" t="s">
-        <v>515</v>
-      </c>
-      <c r="H34" t="s">
-        <v>517</v>
-      </c>
-      <c r="J34" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2615,19 +2615,19 @@
         <v>510</v>
       </c>
       <c r="C35" t="s">
+        <v>522</v>
+      </c>
+      <c r="E35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>514</v>
+      </c>
+      <c r="H35" t="s">
+        <v>516</v>
+      </c>
+      <c r="J35" t="s">
         <v>512</v>
-      </c>
-      <c r="E35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" t="s">
-        <v>516</v>
-      </c>
-      <c r="H35" t="s">
-        <v>518</v>
-      </c>
-      <c r="J35" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
the email field is not mandatory for farmers. fixed the condition for validate regexp in number of document for both farmer and assistant
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="524">
   <si>
     <t>type</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Número de identificación</t>
   </si>
   <si>
-    <t>(regex(., '[0-9]+'))</t>
-  </si>
-  <si>
     <t>assistant_name</t>
   </si>
   <si>
@@ -1594,6 +1591,12 @@
   </si>
   <si>
     <t>Longitud de la finca (coordenadas geograficas [-180,180])</t>
+  </si>
+  <si>
+    <t>(if(${assistant_kind_document}='1',regex(., '[0-9]+'),regex(., '[0-9a-zA-z]+')))</t>
+  </si>
+  <si>
+    <t>(if(${farmer_kind_document}='1',regex(., '[0-9]+'),regex(., '[0-9a-zA-z]+')))</t>
   </si>
 </sst>
 </file>
@@ -2002,8 +2005,8 @@
   <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2020,10 +2023,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D1" t="s">
         <v>394</v>
-      </c>
-      <c r="D1" t="s">
-        <v>395</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2035,7 +2038,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2063,7 +2066,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2077,7 +2080,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2109,10 +2112,10 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>522</v>
       </c>
       <c r="H5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2120,22 +2123,22 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2143,22 +2146,22 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2166,70 +2169,70 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>399</v>
+      </c>
+      <c r="H8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>400</v>
-      </c>
-      <c r="H8" t="s">
-        <v>29</v>
-      </c>
       <c r="J8" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>34</v>
-      </c>
       <c r="J10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -2238,18 +2241,18 @@
         <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -2258,7 +2261,7 @@
         <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2266,16 +2269,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="J13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2283,27 +2286,27 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>488</v>
+      </c>
+      <c r="H14" t="s">
         <v>40</v>
       </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" t="s">
-        <v>489</v>
-      </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
       <c r="J14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2311,18 +2314,18 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -2336,7 +2339,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -2345,10 +2348,10 @@
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>523</v>
       </c>
       <c r="H19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2356,22 +2359,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J20" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2379,22 +2382,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H21" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J21" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2402,33 +2405,33 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>399</v>
+      </c>
+      <c r="H22" t="s">
         <v>28</v>
       </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" t="s">
-        <v>400</v>
-      </c>
-      <c r="H22" t="s">
-        <v>29</v>
-      </c>
       <c r="J22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
@@ -2437,38 +2440,38 @@
         <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
         <v>33</v>
       </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" t="s">
-        <v>34</v>
-      </c>
       <c r="J24" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B25" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
         <v>14</v>
@@ -2477,18 +2480,18 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B26" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
@@ -2497,7 +2500,7 @@
         <v>18</v>
       </c>
       <c r="K26" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -2505,16 +2508,16 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
         <v>14</v>
       </c>
       <c r="J27" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -2522,27 +2525,24 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" t="s">
+        <v>488</v>
+      </c>
+      <c r="H28" t="s">
         <v>40</v>
       </c>
-      <c r="E28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" t="s">
-        <v>489</v>
-      </c>
-      <c r="H28" t="s">
-        <v>41</v>
-      </c>
       <c r="J28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -2550,21 +2550,21 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
         <v>54</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
         <v>56</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>57</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -2572,62 +2572,62 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
         <v>59</v>
       </c>
-      <c r="C33" t="s">
-        <v>60</v>
-      </c>
       <c r="E33" t="s">
         <v>14</v>
       </c>
       <c r="J33" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
+        <v>519</v>
+      </c>
+      <c r="C34" t="s">
         <v>520</v>
       </c>
-      <c r="C34" t="s">
-        <v>521</v>
-      </c>
       <c r="E34" t="s">
         <v>14</v>
       </c>
       <c r="G34" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H34" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J34" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C35" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E35" t="s">
         <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H35" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J35" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2635,24 +2635,24 @@
         <v>19</v>
       </c>
       <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
         <v>63</v>
       </c>
-      <c r="C36" t="s">
-        <v>64</v>
-      </c>
       <c r="J36" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
         <v>65</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
       </c>
       <c r="E37" t="s">
         <v>14</v>
@@ -2661,12 +2661,12 @@
         <v>18</v>
       </c>
       <c r="J37" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -2674,10 +2674,10 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
         <v>67</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
@@ -2685,10 +2685,10 @@
         <v>19</v>
       </c>
       <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
         <v>69</v>
-      </c>
-      <c r="C41" t="s">
-        <v>70</v>
       </c>
       <c r="E41" t="s">
         <v>14</v>
@@ -2696,13 +2696,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
         <v>71</v>
-      </c>
-      <c r="C42" t="s">
-        <v>72</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
@@ -2711,12 +2711,12 @@
         <v>14</v>
       </c>
       <c r="L42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2724,27 +2724,27 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" t="s">
         <v>73</v>
-      </c>
-      <c r="C45" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" t="s">
         <v>75</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
         <v>76</v>
-      </c>
-      <c r="E46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -2752,10 +2752,10 @@
         <v>19</v>
       </c>
       <c r="B47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" t="s">
         <v>78</v>
-      </c>
-      <c r="C47" t="s">
-        <v>79</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
@@ -2764,35 +2764,35 @@
         <v>14</v>
       </c>
       <c r="I47" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
         <v>80</v>
       </c>
-      <c r="C48" t="s">
-        <v>81</v>
-      </c>
       <c r="E48" t="s">
         <v>14</v>
       </c>
       <c r="F48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
         <v>82</v>
-      </c>
-      <c r="C49" t="s">
-        <v>83</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
@@ -2803,70 +2803,70 @@
         <v>19</v>
       </c>
       <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" t="s">
         <v>84</v>
       </c>
-      <c r="C50" t="s">
-        <v>85</v>
-      </c>
       <c r="E50" t="s">
         <v>14</v>
       </c>
       <c r="I50" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
         <v>86</v>
       </c>
-      <c r="C51" t="s">
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" t="s">
         <v>87</v>
-      </c>
-      <c r="E51" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" t="s">
         <v>89</v>
       </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
+        <v>416</v>
+      </c>
+      <c r="H52" t="s">
         <v>90</v>
-      </c>
-      <c r="E52" t="s">
-        <v>14</v>
-      </c>
-      <c r="G52" t="s">
-        <v>417</v>
-      </c>
-      <c r="H52" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B53" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" t="s">
         <v>92</v>
       </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
         <v>93</v>
-      </c>
-      <c r="E53" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -2874,90 +2874,90 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" t="s">
         <v>95</v>
       </c>
-      <c r="C54" t="s">
-        <v>96</v>
-      </c>
       <c r="I54" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" t="s">
         <v>97</v>
       </c>
-      <c r="C55" t="s">
+      <c r="E55" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" t="s">
+        <v>416</v>
+      </c>
+      <c r="H55" t="s">
         <v>98</v>
-      </c>
-      <c r="E55" t="s">
-        <v>14</v>
-      </c>
-      <c r="G55" t="s">
-        <v>417</v>
-      </c>
-      <c r="H55" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" t="s">
         <v>100</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" t="s">
+        <v>416</v>
+      </c>
+      <c r="H56" t="s">
         <v>101</v>
-      </c>
-      <c r="E56" t="s">
-        <v>14</v>
-      </c>
-      <c r="G56" t="s">
-        <v>417</v>
-      </c>
-      <c r="H56" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" t="s">
         <v>103</v>
       </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" t="s">
+        <v>416</v>
+      </c>
+      <c r="H57" t="s">
         <v>104</v>
-      </c>
-      <c r="E57" t="s">
-        <v>14</v>
-      </c>
-      <c r="G57" t="s">
-        <v>417</v>
-      </c>
-      <c r="H57" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B58" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" t="s">
         <v>106</v>
       </c>
-      <c r="C58" t="s">
-        <v>107</v>
-      </c>
       <c r="E58" t="s">
         <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -2965,48 +2965,48 @@
         <v>9</v>
       </c>
       <c r="B59" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" t="s">
         <v>108</v>
       </c>
-      <c r="C59" t="s">
-        <v>109</v>
-      </c>
       <c r="I59" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" t="s">
         <v>110</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>111</v>
       </c>
-      <c r="C60" t="s">
-        <v>112</v>
-      </c>
       <c r="E60" t="s">
         <v>14</v>
       </c>
       <c r="G60" t="s">
+        <v>417</v>
+      </c>
+      <c r="H60" t="s">
         <v>418</v>
-      </c>
-      <c r="H60" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -3014,21 +3014,21 @@
         <v>9</v>
       </c>
       <c r="B65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" t="s">
         <v>113</v>
-      </c>
-      <c r="C65" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>114</v>
+      </c>
+      <c r="B66" t="s">
         <v>115</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>116</v>
-      </c>
-      <c r="C66" t="s">
-        <v>117</v>
       </c>
       <c r="E66" t="s">
         <v>14</v>
@@ -3036,13 +3036,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B67" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" t="s">
         <v>118</v>
-      </c>
-      <c r="C67" t="s">
-        <v>119</v>
       </c>
       <c r="E67" t="s">
         <v>14</v>
@@ -3056,24 +3056,24 @@
         <v>9</v>
       </c>
       <c r="B68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" t="s">
         <v>120</v>
       </c>
-      <c r="C68" t="s">
-        <v>121</v>
-      </c>
       <c r="I68" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B69" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" t="s">
         <v>122</v>
-      </c>
-      <c r="C69" t="s">
-        <v>123</v>
       </c>
       <c r="E69" t="s">
         <v>14</v>
@@ -3081,38 +3081,38 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B70" t="s">
+        <v>123</v>
+      </c>
+      <c r="C70" t="s">
         <v>124</v>
       </c>
-      <c r="C70" t="s">
+      <c r="E70" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" t="s">
+        <v>506</v>
+      </c>
+      <c r="H70" t="s">
         <v>125</v>
-      </c>
-      <c r="E70" t="s">
-        <v>14</v>
-      </c>
-      <c r="G70" t="s">
-        <v>507</v>
-      </c>
-      <c r="H70" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B72" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" t="s">
         <v>127</v>
-      </c>
-      <c r="C72" t="s">
-        <v>128</v>
       </c>
       <c r="D72" t="s">
         <v>17</v>
@@ -3121,27 +3121,27 @@
         <v>14</v>
       </c>
       <c r="G72" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B73" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" t="s">
         <v>130</v>
       </c>
-      <c r="C73" t="s">
-        <v>131</v>
-      </c>
       <c r="E73" t="s">
         <v>14</v>
       </c>
       <c r="F73" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -3149,53 +3149,53 @@
         <v>9</v>
       </c>
       <c r="B74" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" t="s">
         <v>132</v>
       </c>
-      <c r="C74" t="s">
-        <v>133</v>
-      </c>
       <c r="I74" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B75" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" t="s">
         <v>134</v>
       </c>
-      <c r="C75" t="s">
+      <c r="E75" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" t="s">
+        <v>506</v>
+      </c>
+      <c r="H75" t="s">
         <v>135</v>
-      </c>
-      <c r="E75" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" t="s">
-        <v>507</v>
-      </c>
-      <c r="H75" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B76" t="s">
+        <v>136</v>
+      </c>
+      <c r="C76" t="s">
         <v>137</v>
       </c>
-      <c r="C76" t="s">
+      <c r="E76" t="s">
+        <v>14</v>
+      </c>
+      <c r="G76" t="s">
+        <v>507</v>
+      </c>
+      <c r="H76" t="s">
         <v>138</v>
-      </c>
-      <c r="E76" t="s">
-        <v>14</v>
-      </c>
-      <c r="G76" t="s">
-        <v>508</v>
-      </c>
-      <c r="H76" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -3203,10 +3203,10 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
+        <v>139</v>
+      </c>
+      <c r="C77" t="s">
         <v>140</v>
-      </c>
-      <c r="C77" t="s">
-        <v>141</v>
       </c>
       <c r="E77" t="s">
         <v>14</v>
@@ -3214,19 +3214,19 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B78" t="s">
+        <v>141</v>
+      </c>
+      <c r="C78" t="s">
         <v>142</v>
       </c>
-      <c r="C78" t="s">
-        <v>143</v>
-      </c>
       <c r="E78" t="s">
         <v>14</v>
       </c>
       <c r="F78" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -3234,48 +3234,48 @@
         <v>9</v>
       </c>
       <c r="B79" t="s">
+        <v>143</v>
+      </c>
+      <c r="C79" t="s">
         <v>144</v>
       </c>
-      <c r="C79" t="s">
-        <v>145</v>
-      </c>
       <c r="I79" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B80" t="s">
+        <v>145</v>
+      </c>
+      <c r="C80" t="s">
         <v>146</v>
       </c>
-      <c r="C80" t="s">
+      <c r="E80" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" t="s">
+        <v>417</v>
+      </c>
+      <c r="H80" t="s">
         <v>147</v>
-      </c>
-      <c r="E80" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" t="s">
-        <v>418</v>
-      </c>
-      <c r="H80" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -3283,21 +3283,21 @@
         <v>9</v>
       </c>
       <c r="B85" t="s">
+        <v>148</v>
+      </c>
+      <c r="C85" t="s">
         <v>149</v>
-      </c>
-      <c r="C85" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C87" t="s">
         <v>151</v>
-      </c>
-      <c r="C87" t="s">
-        <v>152</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -3308,24 +3308,24 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>152</v>
+      </c>
+      <c r="B88" t="s">
         <v>153</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>154</v>
-      </c>
-      <c r="C88" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B89" t="s">
+        <v>155</v>
+      </c>
+      <c r="C89" t="s">
         <v>156</v>
-      </c>
-      <c r="C89" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -3333,38 +3333,38 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
+        <v>157</v>
+      </c>
+      <c r="C90" t="s">
         <v>158</v>
       </c>
-      <c r="C90" t="s">
-        <v>159</v>
-      </c>
       <c r="I90" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B91" t="s">
+        <v>159</v>
+      </c>
+      <c r="C91" t="s">
         <v>160</v>
       </c>
-      <c r="C91" t="s">
+      <c r="E91" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" t="s">
+        <v>416</v>
+      </c>
+      <c r="H91" t="s">
         <v>161</v>
-      </c>
-      <c r="E91" t="s">
-        <v>14</v>
-      </c>
-      <c r="G91" t="s">
-        <v>417</v>
-      </c>
-      <c r="H91" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -3372,33 +3372,33 @@
         <v>9</v>
       </c>
       <c r="B93" t="s">
+        <v>162</v>
+      </c>
+      <c r="C93" t="s">
         <v>163</v>
       </c>
-      <c r="C93" t="s">
-        <v>164</v>
-      </c>
       <c r="I93" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B94" t="s">
+        <v>164</v>
+      </c>
+      <c r="C94" t="s">
         <v>165</v>
       </c>
-      <c r="C94" t="s">
+      <c r="E94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" t="s">
+        <v>506</v>
+      </c>
+      <c r="H94" t="s">
         <v>166</v>
-      </c>
-      <c r="E94" t="s">
-        <v>14</v>
-      </c>
-      <c r="G94" t="s">
-        <v>507</v>
-      </c>
-      <c r="H94" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -3406,13 +3406,13 @@
         <v>9</v>
       </c>
       <c r="B95" t="s">
+        <v>167</v>
+      </c>
+      <c r="C95" t="s">
         <v>168</v>
       </c>
-      <c r="C95" t="s">
-        <v>169</v>
-      </c>
       <c r="I95" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
@@ -3420,10 +3420,10 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
+        <v>169</v>
+      </c>
+      <c r="C96" t="s">
         <v>170</v>
-      </c>
-      <c r="C96" t="s">
-        <v>171</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
@@ -3431,13 +3431,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B97" t="s">
+        <v>171</v>
+      </c>
+      <c r="C97" t="s">
         <v>172</v>
-      </c>
-      <c r="C97" t="s">
-        <v>173</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
@@ -3445,13 +3445,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B98" t="s">
+        <v>173</v>
+      </c>
+      <c r="C98" t="s">
         <v>174</v>
-      </c>
-      <c r="C98" t="s">
-        <v>175</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -3459,13 +3459,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B99" t="s">
+        <v>175</v>
+      </c>
+      <c r="C99" t="s">
         <v>176</v>
-      </c>
-      <c r="C99" t="s">
-        <v>177</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
@@ -3473,18 +3473,18 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B101" t="s">
+        <v>177</v>
+      </c>
+      <c r="C101" t="s">
         <v>178</v>
-      </c>
-      <c r="C101" t="s">
-        <v>179</v>
       </c>
       <c r="E101" t="s">
         <v>14</v>
@@ -3493,7 +3493,7 @@
         <v>18</v>
       </c>
       <c r="I101" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
@@ -3501,31 +3501,31 @@
         <v>19</v>
       </c>
       <c r="B102" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" t="s">
         <v>180</v>
-      </c>
-      <c r="C102" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B106" t="s">
+        <v>182</v>
+      </c>
+      <c r="C106" t="s">
         <v>183</v>
-      </c>
-      <c r="C106" t="s">
-        <v>184</v>
       </c>
       <c r="E106" t="s">
         <v>14</v>
@@ -3536,24 +3536,24 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B107" t="s">
+        <v>184</v>
+      </c>
+      <c r="C107" t="s">
         <v>185</v>
-      </c>
-      <c r="C107" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B108" t="s">
+        <v>186</v>
+      </c>
+      <c r="C108" t="s">
         <v>187</v>
-      </c>
-      <c r="C108" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
@@ -3561,38 +3561,38 @@
         <v>9</v>
       </c>
       <c r="B109" t="s">
+        <v>188</v>
+      </c>
+      <c r="C109" t="s">
         <v>189</v>
       </c>
-      <c r="C109" t="s">
-        <v>190</v>
-      </c>
       <c r="I109" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B110" t="s">
+        <v>190</v>
+      </c>
+      <c r="C110" t="s">
         <v>191</v>
       </c>
-      <c r="C110" t="s">
-        <v>192</v>
-      </c>
       <c r="E110" t="s">
         <v>14</v>
       </c>
       <c r="G110" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H110" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
@@ -3600,44 +3600,44 @@
         <v>9</v>
       </c>
       <c r="B112" t="s">
+        <v>192</v>
+      </c>
+      <c r="C112" t="s">
         <v>193</v>
       </c>
-      <c r="C112" t="s">
-        <v>194</v>
-      </c>
       <c r="I112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C113" t="s">
+        <v>165</v>
+      </c>
+      <c r="E113" t="s">
+        <v>14</v>
+      </c>
+      <c r="G113" t="s">
+        <v>506</v>
+      </c>
+      <c r="H113" t="s">
         <v>166</v>
-      </c>
-      <c r="E113" t="s">
-        <v>14</v>
-      </c>
-      <c r="G113" t="s">
-        <v>507</v>
-      </c>
-      <c r="H113" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B114" t="s">
+        <v>195</v>
+      </c>
+      <c r="C114" t="s">
         <v>196</v>
-      </c>
-      <c r="C114" t="s">
-        <v>197</v>
       </c>
       <c r="E114" t="s">
         <v>14</v>
@@ -3646,7 +3646,7 @@
         <v>18</v>
       </c>
       <c r="I114" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
@@ -3654,31 +3654,31 @@
         <v>19</v>
       </c>
       <c r="B115" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B119" t="s">
+        <v>198</v>
+      </c>
+      <c r="C119" t="s">
         <v>199</v>
-      </c>
-      <c r="C119" t="s">
-        <v>200</v>
       </c>
       <c r="E119" t="s">
         <v>14</v>
@@ -3689,24 +3689,24 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B120" t="s">
+        <v>200</v>
+      </c>
+      <c r="C120" t="s">
         <v>201</v>
-      </c>
-      <c r="C120" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B121" t="s">
+        <v>202</v>
+      </c>
+      <c r="C121" t="s">
         <v>203</v>
-      </c>
-      <c r="C121" t="s">
-        <v>204</v>
       </c>
       <c r="E121" t="s">
         <v>14</v>
@@ -3720,38 +3720,38 @@
         <v>9</v>
       </c>
       <c r="B122" t="s">
+        <v>204</v>
+      </c>
+      <c r="C122" t="s">
         <v>205</v>
       </c>
-      <c r="C122" t="s">
-        <v>206</v>
-      </c>
       <c r="I122" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B123" t="s">
+        <v>206</v>
+      </c>
+      <c r="C123" t="s">
         <v>207</v>
       </c>
-      <c r="C123" t="s">
-        <v>208</v>
-      </c>
       <c r="E123" t="s">
         <v>14</v>
       </c>
       <c r="G123" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H123" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
@@ -3759,33 +3759,33 @@
         <v>9</v>
       </c>
       <c r="B125" t="s">
+        <v>208</v>
+      </c>
+      <c r="C125" t="s">
         <v>209</v>
       </c>
-      <c r="C125" t="s">
-        <v>210</v>
-      </c>
       <c r="I125" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B126" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C126" t="s">
+        <v>165</v>
+      </c>
+      <c r="E126" t="s">
+        <v>14</v>
+      </c>
+      <c r="G126" t="s">
+        <v>506</v>
+      </c>
+      <c r="H126" t="s">
         <v>166</v>
-      </c>
-      <c r="E126" t="s">
-        <v>14</v>
-      </c>
-      <c r="G126" t="s">
-        <v>507</v>
-      </c>
-      <c r="H126" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -3793,31 +3793,31 @@
         <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C127" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B131" t="s">
+        <v>212</v>
+      </c>
+      <c r="C131" t="s">
         <v>213</v>
-      </c>
-      <c r="C131" t="s">
-        <v>214</v>
       </c>
       <c r="E131" t="s">
         <v>14</v>
@@ -3828,24 +3828,24 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B132" t="s">
+        <v>214</v>
+      </c>
+      <c r="C132" t="s">
         <v>215</v>
-      </c>
-      <c r="C132" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B133" t="s">
+        <v>216</v>
+      </c>
+      <c r="C133" t="s">
         <v>217</v>
-      </c>
-      <c r="C133" t="s">
-        <v>218</v>
       </c>
       <c r="E133" t="s">
         <v>14</v>
@@ -3859,38 +3859,38 @@
         <v>9</v>
       </c>
       <c r="B134" t="s">
+        <v>218</v>
+      </c>
+      <c r="C134" t="s">
         <v>219</v>
       </c>
-      <c r="C134" t="s">
-        <v>220</v>
-      </c>
       <c r="I134" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B135" t="s">
+        <v>220</v>
+      </c>
+      <c r="C135" t="s">
         <v>221</v>
       </c>
-      <c r="C135" t="s">
-        <v>222</v>
-      </c>
       <c r="E135" t="s">
         <v>14</v>
       </c>
       <c r="G135" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H135" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
@@ -3898,33 +3898,33 @@
         <v>9</v>
       </c>
       <c r="B137" t="s">
+        <v>222</v>
+      </c>
+      <c r="C137" t="s">
         <v>223</v>
       </c>
-      <c r="C137" t="s">
-        <v>224</v>
-      </c>
       <c r="I137" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B138" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C138" t="s">
+        <v>165</v>
+      </c>
+      <c r="E138" t="s">
+        <v>14</v>
+      </c>
+      <c r="G138" t="s">
+        <v>506</v>
+      </c>
+      <c r="H138" t="s">
         <v>166</v>
-      </c>
-      <c r="E138" t="s">
-        <v>14</v>
-      </c>
-      <c r="G138" t="s">
-        <v>507</v>
-      </c>
-      <c r="H138" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
@@ -3932,31 +3932,31 @@
         <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C139" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B143" t="s">
+        <v>226</v>
+      </c>
+      <c r="C143" t="s">
         <v>227</v>
-      </c>
-      <c r="C143" t="s">
-        <v>228</v>
       </c>
       <c r="E143" t="s">
         <v>14</v>
@@ -3967,24 +3967,24 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B144" t="s">
+        <v>228</v>
+      </c>
+      <c r="C144" t="s">
         <v>229</v>
-      </c>
-      <c r="C144" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B145" t="s">
+        <v>230</v>
+      </c>
+      <c r="C145" t="s">
         <v>231</v>
-      </c>
-      <c r="C145" t="s">
-        <v>232</v>
       </c>
       <c r="E145" t="s">
         <v>14</v>
@@ -3998,38 +3998,38 @@
         <v>9</v>
       </c>
       <c r="B146" t="s">
+        <v>232</v>
+      </c>
+      <c r="C146" t="s">
         <v>233</v>
       </c>
-      <c r="C146" t="s">
-        <v>234</v>
-      </c>
       <c r="I146" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B147" t="s">
+        <v>234</v>
+      </c>
+      <c r="C147" t="s">
         <v>235</v>
       </c>
-      <c r="C147" t="s">
-        <v>236</v>
-      </c>
       <c r="E147" t="s">
         <v>14</v>
       </c>
       <c r="G147" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H147" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
@@ -4037,33 +4037,33 @@
         <v>9</v>
       </c>
       <c r="B149" t="s">
+        <v>236</v>
+      </c>
+      <c r="C149" t="s">
         <v>237</v>
       </c>
-      <c r="C149" t="s">
-        <v>238</v>
-      </c>
       <c r="I149" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B150" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C150" t="s">
+        <v>165</v>
+      </c>
+      <c r="E150" t="s">
+        <v>14</v>
+      </c>
+      <c r="G150" t="s">
+        <v>506</v>
+      </c>
+      <c r="H150" t="s">
         <v>166</v>
-      </c>
-      <c r="E150" t="s">
-        <v>14</v>
-      </c>
-      <c r="G150" t="s">
-        <v>507</v>
-      </c>
-      <c r="H150" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
@@ -4071,21 +4071,21 @@
         <v>9</v>
       </c>
       <c r="B151" t="s">
+        <v>239</v>
+      </c>
+      <c r="C151" t="s">
         <v>240</v>
-      </c>
-      <c r="C151" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B152" t="s">
+        <v>241</v>
+      </c>
+      <c r="C152" t="s">
         <v>242</v>
-      </c>
-      <c r="C152" t="s">
-        <v>243</v>
       </c>
       <c r="E152" t="s">
         <v>14</v>
@@ -4094,12 +4094,12 @@
         <v>18</v>
       </c>
       <c r="I152" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
@@ -4107,24 +4107,24 @@
         <v>9</v>
       </c>
       <c r="B154" t="s">
+        <v>243</v>
+      </c>
+      <c r="C154" t="s">
         <v>244</v>
       </c>
-      <c r="C154" t="s">
-        <v>245</v>
-      </c>
       <c r="I154" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B155" t="s">
+        <v>245</v>
+      </c>
+      <c r="C155" t="s">
         <v>246</v>
-      </c>
-      <c r="C155" t="s">
-        <v>247</v>
       </c>
       <c r="E155" t="s">
         <v>14</v>
@@ -4135,7 +4135,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
@@ -4143,25 +4143,25 @@
         <v>19</v>
       </c>
       <c r="B157" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C157" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
@@ -4169,41 +4169,41 @@
         <v>9</v>
       </c>
       <c r="B163" t="s">
+        <v>248</v>
+      </c>
+      <c r="C163" t="s">
         <v>249</v>
-      </c>
-      <c r="C163" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B164" t="s">
+        <v>250</v>
+      </c>
+      <c r="C164" t="s">
         <v>251</v>
       </c>
-      <c r="C164" t="s">
+      <c r="E164" t="s">
+        <v>14</v>
+      </c>
+      <c r="G164" t="s">
+        <v>506</v>
+      </c>
+      <c r="H164" t="s">
         <v>252</v>
-      </c>
-      <c r="E164" t="s">
-        <v>14</v>
-      </c>
-      <c r="G164" t="s">
-        <v>507</v>
-      </c>
-      <c r="H164" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B165" t="s">
+        <v>253</v>
+      </c>
+      <c r="C165" t="s">
         <v>254</v>
-      </c>
-      <c r="C165" t="s">
-        <v>255</v>
       </c>
       <c r="E165" t="s">
         <v>14</v>
@@ -4214,53 +4214,53 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B166" t="s">
+        <v>255</v>
+      </c>
+      <c r="C166" t="s">
         <v>256</v>
       </c>
-      <c r="C166" t="s">
+      <c r="E166" t="s">
+        <v>14</v>
+      </c>
+      <c r="G166" t="s">
+        <v>416</v>
+      </c>
+      <c r="H166" t="s">
         <v>257</v>
-      </c>
-      <c r="E166" t="s">
-        <v>14</v>
-      </c>
-      <c r="G166" t="s">
-        <v>417</v>
-      </c>
-      <c r="H166" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B167" t="s">
+        <v>258</v>
+      </c>
+      <c r="C167" t="s">
         <v>259</v>
       </c>
-      <c r="C167" t="s">
+      <c r="E167" t="s">
+        <v>14</v>
+      </c>
+      <c r="G167" t="s">
+        <v>416</v>
+      </c>
+      <c r="H167" t="s">
         <v>260</v>
-      </c>
-      <c r="E167" t="s">
-        <v>14</v>
-      </c>
-      <c r="G167" t="s">
-        <v>417</v>
-      </c>
-      <c r="H167" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B168" t="s">
+        <v>261</v>
+      </c>
+      <c r="C168" t="s">
         <v>262</v>
-      </c>
-      <c r="C168" t="s">
-        <v>263</v>
       </c>
       <c r="E168" t="s">
         <v>14</v>
@@ -4271,39 +4271,39 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B169" t="s">
+        <v>263</v>
+      </c>
+      <c r="C169" t="s">
         <v>264</v>
       </c>
-      <c r="C169" t="s">
+      <c r="E169" t="s">
+        <v>14</v>
+      </c>
+      <c r="G169" t="s">
+        <v>416</v>
+      </c>
+      <c r="H169" t="s">
         <v>265</v>
-      </c>
-      <c r="E169" t="s">
-        <v>14</v>
-      </c>
-      <c r="G169" t="s">
-        <v>417</v>
-      </c>
-      <c r="H169" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B170" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C170" t="s">
+        <v>92</v>
+      </c>
+      <c r="E170" t="s">
+        <v>14</v>
+      </c>
+      <c r="F170" t="s">
         <v>93</v>
-      </c>
-      <c r="E170" t="s">
-        <v>14</v>
-      </c>
-      <c r="F170" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
@@ -4311,24 +4311,24 @@
         <v>9</v>
       </c>
       <c r="B171" t="s">
+        <v>267</v>
+      </c>
+      <c r="C171" t="s">
         <v>268</v>
       </c>
-      <c r="C171" t="s">
-        <v>269</v>
-      </c>
       <c r="I171" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B172" t="s">
+        <v>269</v>
+      </c>
+      <c r="C172" t="s">
         <v>270</v>
-      </c>
-      <c r="C172" t="s">
-        <v>271</v>
       </c>
       <c r="E172" t="s">
         <v>14</v>
@@ -4336,44 +4336,44 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B173" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C173" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E173" t="s">
         <v>14</v>
       </c>
       <c r="F173" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B174" t="s">
+        <v>272</v>
+      </c>
+      <c r="C174" t="s">
         <v>273</v>
       </c>
-      <c r="C174" t="s">
-        <v>274</v>
-      </c>
       <c r="I174" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B175" t="s">
+        <v>274</v>
+      </c>
+      <c r="C175" t="s">
         <v>275</v>
-      </c>
-      <c r="C175" t="s">
-        <v>276</v>
       </c>
       <c r="E175" t="s">
         <v>14</v>
@@ -4381,57 +4381,57 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B176" t="s">
+        <v>276</v>
+      </c>
+      <c r="C176" t="s">
         <v>277</v>
       </c>
-      <c r="C176" t="s">
+      <c r="E176" t="s">
+        <v>14</v>
+      </c>
+      <c r="G176" t="s">
+        <v>416</v>
+      </c>
+      <c r="H176" t="s">
         <v>278</v>
-      </c>
-      <c r="E176" t="s">
-        <v>14</v>
-      </c>
-      <c r="G176" t="s">
-        <v>417</v>
-      </c>
-      <c r="H176" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B177" t="s">
+        <v>279</v>
+      </c>
+      <c r="C177" t="s">
         <v>280</v>
       </c>
-      <c r="C177" t="s">
+      <c r="E177" t="s">
+        <v>14</v>
+      </c>
+      <c r="G177" t="s">
+        <v>416</v>
+      </c>
+      <c r="H177" t="s">
         <v>281</v>
-      </c>
-      <c r="E177" t="s">
-        <v>14</v>
-      </c>
-      <c r="G177" t="s">
-        <v>417</v>
-      </c>
-      <c r="H177" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
@@ -4439,44 +4439,44 @@
         <v>9</v>
       </c>
       <c r="B182" t="s">
+        <v>282</v>
+      </c>
+      <c r="C182" t="s">
         <v>283</v>
-      </c>
-      <c r="C182" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B183" t="s">
+        <v>284</v>
+      </c>
+      <c r="C183" t="s">
         <v>285</v>
       </c>
-      <c r="C183" t="s">
-        <v>286</v>
-      </c>
       <c r="E183" t="s">
         <v>14</v>
       </c>
       <c r="F183" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B184" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C184" t="s">
+        <v>92</v>
+      </c>
+      <c r="E184" t="s">
+        <v>14</v>
+      </c>
+      <c r="F184" t="s">
         <v>93</v>
-      </c>
-      <c r="E184" t="s">
-        <v>14</v>
-      </c>
-      <c r="F184" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
@@ -4484,50 +4484,50 @@
         <v>9</v>
       </c>
       <c r="B185" t="s">
+        <v>287</v>
+      </c>
+      <c r="C185" t="s">
         <v>288</v>
       </c>
-      <c r="C185" t="s">
-        <v>289</v>
-      </c>
       <c r="I185" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B186" t="s">
+        <v>289</v>
+      </c>
+      <c r="C186" t="s">
         <v>290</v>
       </c>
-      <c r="C186" t="s">
+      <c r="E186" t="s">
+        <v>14</v>
+      </c>
+      <c r="G186" t="s">
+        <v>416</v>
+      </c>
+      <c r="H186" t="s">
         <v>291</v>
-      </c>
-      <c r="E186" t="s">
-        <v>14</v>
-      </c>
-      <c r="G186" t="s">
-        <v>417</v>
-      </c>
-      <c r="H186" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B187" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C187" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E187" t="s">
         <v>14</v>
       </c>
       <c r="F187" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
@@ -4535,55 +4535,55 @@
         <v>9</v>
       </c>
       <c r="B188" t="s">
+        <v>293</v>
+      </c>
+      <c r="C188" t="s">
         <v>294</v>
       </c>
-      <c r="C188" t="s">
-        <v>295</v>
-      </c>
       <c r="I188" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B189" t="s">
+        <v>295</v>
+      </c>
+      <c r="C189" t="s">
         <v>296</v>
       </c>
-      <c r="C189" t="s">
+      <c r="E189" t="s">
+        <v>14</v>
+      </c>
+      <c r="G189" t="s">
+        <v>508</v>
+      </c>
+      <c r="H189" t="s">
         <v>297</v>
-      </c>
-      <c r="E189" t="s">
-        <v>14</v>
-      </c>
-      <c r="G189" t="s">
-        <v>509</v>
-      </c>
-      <c r="H189" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B190" t="s">
+        <v>298</v>
+      </c>
+      <c r="C190" t="s">
         <v>299</v>
-      </c>
-      <c r="C190" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B191" t="s">
+        <v>300</v>
+      </c>
+      <c r="C191" t="s">
         <v>301</v>
-      </c>
-      <c r="C191" t="s">
-        <v>302</v>
       </c>
       <c r="E191" t="s">
         <v>14</v>
@@ -4594,30 +4594,30 @@
         <v>19</v>
       </c>
       <c r="B192" t="s">
+        <v>302</v>
+      </c>
+      <c r="C192" t="s">
         <v>303</v>
-      </c>
-      <c r="C192" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -4642,652 +4642,652 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E1" t="s">
         <v>457</v>
-      </c>
-      <c r="E1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" t="s">
         <v>310</v>
-      </c>
-      <c r="C4" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C5" t="s">
         <v>312</v>
-      </c>
-      <c r="C5" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" t="s">
         <v>318</v>
-      </c>
-      <c r="C8" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B9" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" t="s">
         <v>320</v>
-      </c>
-      <c r="C9" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C29" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C32" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C33" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B35" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B36" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C36" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B37" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C37" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C41" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B42" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C42" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B43" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C43" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B44" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C44" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B45" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C45" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B49" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C49" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B50" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C50" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B53" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
       </c>
       <c r="C58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -5295,354 +5295,354 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B61" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C61" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C62" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B63" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C63" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
       </c>
       <c r="C64" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B66" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C66" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B67" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C67" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B68" t="s">
+        <v>326</v>
+      </c>
+      <c r="C68" t="s">
         <v>327</v>
-      </c>
-      <c r="C68" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B69" t="s">
+        <v>328</v>
+      </c>
+      <c r="C69" t="s">
         <v>329</v>
-      </c>
-      <c r="C69" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B70" t="s">
+        <v>330</v>
+      </c>
+      <c r="C70" t="s">
         <v>331</v>
-      </c>
-      <c r="C70" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B71" t="s">
+        <v>332</v>
+      </c>
+      <c r="C71" t="s">
         <v>333</v>
-      </c>
-      <c r="C71" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B72" t="s">
+        <v>334</v>
+      </c>
+      <c r="C72" t="s">
         <v>335</v>
-      </c>
-      <c r="C72" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B73" t="s">
+        <v>336</v>
+      </c>
+      <c r="C73" t="s">
         <v>337</v>
-      </c>
-      <c r="C73" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B74" t="s">
+        <v>338</v>
+      </c>
+      <c r="C74" t="s">
         <v>339</v>
-      </c>
-      <c r="C74" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C76" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B77" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C77" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B78" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C78" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C80" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C82" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B83" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C83" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B84" t="s">
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B86" t="s">
+        <v>375</v>
+      </c>
+      <c r="C86" t="s">
         <v>376</v>
-      </c>
-      <c r="C86" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B87" t="s">
+        <v>377</v>
+      </c>
+      <c r="C87" t="s">
         <v>378</v>
-      </c>
-      <c r="C87" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B88" t="s">
+        <v>379</v>
+      </c>
+      <c r="C88" t="s">
         <v>380</v>
-      </c>
-      <c r="C88" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B89" t="s">
+        <v>381</v>
+      </c>
+      <c r="C89" t="s">
         <v>382</v>
-      </c>
-      <c r="C89" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B90" t="s">
         <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -5660,7 +5660,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -5684,30 +5684,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" t="s">
         <v>384</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>385</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>386</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>387</v>
       </c>
-      <c r="E1" t="s">
-        <v>388</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -5716,7 +5716,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F2" s="1">
         <v>201807</v>

</xml_diff>

<commit_message>
changed the type of fields from integer to decimal
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -2005,8 +2005,8 @@
   <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2885,7 +2885,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
         <v>96</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B56" t="s">
         <v>99</v>
@@ -2925,7 +2925,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B57" t="s">
         <v>102</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
         <v>126</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B97" t="s">
         <v>171</v>
@@ -3445,7 +3445,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B98" t="s">
         <v>173</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B99" t="s">
         <v>175</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B166" t="s">
         <v>255</v>
@@ -4234,7 +4234,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B167" t="s">
         <v>258</v>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B169" t="s">
         <v>263</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B177" t="s">
         <v>279</v>
@@ -4495,7 +4495,7 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B186" t="s">
         <v>289</v>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B191" t="s">
         <v>300</v>

</xml_diff>

<commit_message>
fixed a issue with search preload data in form odk
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$196</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$233</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="572">
   <si>
     <t>type</t>
   </si>
@@ -1584,9 +1584,6 @@
     <t>El apellido debe contener solamente texto y no tener espacios en blanco al final</t>
   </si>
   <si>
-    <t>farm_location</t>
-  </si>
-  <si>
     <t>Latitud de la finca (coordenadas geograficas [-90,90])</t>
   </si>
   <si>
@@ -1597,6 +1594,153 @@
   </si>
   <si>
     <t>(if(${farmer_kind_document}='1',regex(., '[0-9]+'),regex(., '[0-9a-zA-z]+')))</t>
+  </si>
+  <si>
+    <t>farm_location_lat</t>
+  </si>
+  <si>
+    <t>choices_phenological_products</t>
+  </si>
+  <si>
+    <t>select_one choices_phenological_products</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>assistant_found</t>
+  </si>
+  <si>
+    <t>(if(pulldata('people','name', 'document_key', ${assistant_document_number})='','false','true'))</t>
+  </si>
+  <si>
+    <t>assistant_found_group</t>
+  </si>
+  <si>
+    <t>assistant_found_name</t>
+  </si>
+  <si>
+    <t>assistant_found_last_name</t>
+  </si>
+  <si>
+    <t>assistant_found_cellphone</t>
+  </si>
+  <si>
+    <t>(${assistant_found}='true')</t>
+  </si>
+  <si>
+    <t>assistant_group</t>
+  </si>
+  <si>
+    <t>assistant_found_sex</t>
+  </si>
+  <si>
+    <t>assistant_found_country</t>
+  </si>
+  <si>
+    <t>assistant_found_adm1</t>
+  </si>
+  <si>
+    <t>assistant_found_adm2</t>
+  </si>
+  <si>
+    <t>assistant_found_address</t>
+  </si>
+  <si>
+    <t>assistant_found_email</t>
+  </si>
+  <si>
+    <t>(${assistant_found}='false')</t>
+  </si>
+  <si>
+    <t>Asistente técnico en base de datos</t>
+  </si>
+  <si>
+    <t>farmer_found</t>
+  </si>
+  <si>
+    <t>(if(pulldata('people','name', 'document_key', ${farmer_document_number})='','false','true'))</t>
+  </si>
+  <si>
+    <t>farmer_found_group</t>
+  </si>
+  <si>
+    <t>Agricultor en base de datos</t>
+  </si>
+  <si>
+    <t>(${farmer_found}='true')</t>
+  </si>
+  <si>
+    <t>(${farmer_found}='false')</t>
+  </si>
+  <si>
+    <t>farmer_found_name</t>
+  </si>
+  <si>
+    <t>farmer_found_last_name</t>
+  </si>
+  <si>
+    <t>farmer_found_cellphone</t>
+  </si>
+  <si>
+    <t>farmer_found_sex</t>
+  </si>
+  <si>
+    <t>farmer_found_country</t>
+  </si>
+  <si>
+    <t>farmer_found_adm1</t>
+  </si>
+  <si>
+    <t>farmer_found_adm2</t>
+  </si>
+  <si>
+    <t>farmer_found_address</t>
+  </si>
+  <si>
+    <t>farmer_found_email</t>
+  </si>
+  <si>
+    <t>farmer_group</t>
+  </si>
+  <si>
+    <t>country = ${assistant_found_country}</t>
+  </si>
+  <si>
+    <t>country = ${assistant_found_country} and state = ${assistant_found_adm1}</t>
+  </si>
+  <si>
+    <t>country = ${farmer_found_country}</t>
+  </si>
+  <si>
+    <t>country = ${farmer_found_country} and state = ${farmer_found_adm1}</t>
+  </si>
+  <si>
+    <t>farm_found_group</t>
+  </si>
+  <si>
+    <t>(${farm_id}!='')</t>
+  </si>
+  <si>
+    <t>farm_found_name</t>
+  </si>
+  <si>
+    <t>farm_found_location_lat</t>
+  </si>
+  <si>
+    <t>farm_found_location_lon</t>
+  </si>
+  <si>
+    <t>farm_found_address_comments</t>
+  </si>
+  <si>
+    <t>farm_found_owner</t>
+  </si>
+  <si>
+    <t>(${farm_id}='')</t>
+  </si>
+  <si>
+    <t>farm_group</t>
   </si>
 </sst>
 </file>
@@ -2002,11 +2146,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L196"/>
+  <dimension ref="A1:L233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2112,7 +2256,7 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H5" t="s">
         <v>516</v>
@@ -2120,48 +2264,27 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>526</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>400</v>
-      </c>
-      <c r="H6" t="s">
-        <v>517</v>
+        <v>527</v>
       </c>
       <c r="J6" t="s">
-        <v>489</v>
+        <v>528</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>529</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>400</v>
-      </c>
-      <c r="H7" t="s">
-        <v>518</v>
-      </c>
-      <c r="J7" t="s">
-        <v>490</v>
+        <v>542</v>
+      </c>
+      <c r="I7" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2169,169 +2292,195 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>530</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>517</v>
       </c>
       <c r="J8" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>401</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>531</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
+      <c r="G9" t="s">
+        <v>400</v>
+      </c>
+      <c r="H9" t="s">
+        <v>518</v>
+      </c>
       <c r="J9" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>403</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>532</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="s">
-        <v>33</v>
+      <c r="G10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
       </c>
       <c r="J10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>445</v>
+        <v>401</v>
       </c>
       <c r="B11" t="s">
-        <v>405</v>
+        <v>535</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" t="s">
-        <v>458</v>
+      <c r="J11" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>446</v>
+        <v>403</v>
       </c>
       <c r="B12" t="s">
-        <v>406</v>
+        <v>536</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" t="s">
-        <v>460</v>
+      <c r="J12" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>445</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>537</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="J13" t="s">
-        <v>494</v>
+      <c r="K13" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>446</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>538</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
       </c>
-      <c r="G14" t="s">
-        <v>488</v>
-      </c>
-      <c r="H14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" t="s">
-        <v>495</v>
+      <c r="K14" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>539</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>540</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>488</v>
+      </c>
+      <c r="H16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>397</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>534</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -2339,19 +2488,19 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>523</v>
+        <v>400</v>
       </c>
       <c r="H19" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2359,10 +2508,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -2371,10 +2520,7 @@
         <v>400</v>
       </c>
       <c r="H20" t="s">
-        <v>517</v>
-      </c>
-      <c r="J20" t="s">
-        <v>496</v>
+        <v>518</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2382,96 +2528,81 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H21" t="s">
-        <v>518</v>
-      </c>
-      <c r="J21" t="s">
-        <v>497</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>401</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
-      </c>
-      <c r="G22" t="s">
-        <v>399</v>
-      </c>
-      <c r="H22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" t="s">
-        <v>499</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>403</v>
+        <v>445</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>405</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
-      </c>
-      <c r="J24" t="s">
-        <v>500</v>
+        <v>18</v>
+      </c>
+      <c r="K24" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B25" t="s">
-        <v>461</v>
+        <v>406</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E25" t="s">
         <v>14</v>
@@ -2480,27 +2611,21 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>446</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>462</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
-      </c>
-      <c r="F26" t="s">
-        <v>18</v>
-      </c>
-      <c r="K26" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -2508,36 +2633,24 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
         <v>14</v>
       </c>
-      <c r="J27" t="s">
-        <v>501</v>
+      <c r="G27" t="s">
+        <v>488</v>
+      </c>
+      <c r="H27" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" t="s">
-        <v>488</v>
-      </c>
-      <c r="H28" t="s">
-        <v>40</v>
-      </c>
-      <c r="J28" t="s">
-        <v>502</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -2550,883 +2663,983 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>397</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E33" t="s">
         <v>14</v>
       </c>
-      <c r="J33" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>522</v>
+      </c>
+      <c r="H33" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>526</v>
       </c>
       <c r="B34" t="s">
-        <v>519</v>
-      </c>
-      <c r="C34" t="s">
-        <v>520</v>
-      </c>
-      <c r="E34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" t="s">
-        <v>512</v>
-      </c>
-      <c r="H34" t="s">
-        <v>514</v>
+        <v>543</v>
       </c>
       <c r="J34" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>509</v>
+        <v>545</v>
       </c>
       <c r="C35" t="s">
-        <v>521</v>
-      </c>
-      <c r="E35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" t="s">
-        <v>513</v>
-      </c>
-      <c r="H35" t="s">
-        <v>515</v>
-      </c>
-      <c r="J35" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+        <v>546</v>
+      </c>
+      <c r="I35" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>549</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
+        <v>400</v>
+      </c>
+      <c r="H36" t="s">
+        <v>517</v>
       </c>
       <c r="J36" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>409</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>550</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
         <v>14</v>
       </c>
-      <c r="F37" t="s">
-        <v>18</v>
+      <c r="G37" t="s">
+        <v>400</v>
+      </c>
+      <c r="H37" t="s">
+        <v>518</v>
       </c>
       <c r="J37" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>551</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" t="s">
+        <v>399</v>
+      </c>
+      <c r="H38" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>401</v>
+      </c>
+      <c r="B39" t="s">
+        <v>552</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>403</v>
+      </c>
+      <c r="B40" t="s">
+        <v>553</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>445</v>
+      </c>
+      <c r="B41" t="s">
+        <v>554</v>
+      </c>
+      <c r="C41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>446</v>
+      </c>
+      <c r="B42" t="s">
+        <v>555</v>
+      </c>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>556</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>557</v>
+      </c>
+      <c r="C44" t="s">
+        <v>39</v>
+      </c>
+      <c r="G44" t="s">
+        <v>488</v>
+      </c>
+      <c r="H44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J44" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>9</v>
       </c>
-      <c r="B40" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" t="s">
-        <v>14</v>
-      </c>
-      <c r="L42" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>447</v>
-      </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>558</v>
       </c>
       <c r="C46" t="s">
-        <v>75</v>
-      </c>
-      <c r="E46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="I46" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
       </c>
-      <c r="I47" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G47" t="s">
+        <v>400</v>
+      </c>
+      <c r="H47" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>448</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
       </c>
-      <c r="F48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>400</v>
+      </c>
+      <c r="H48" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>449</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>399</v>
+      </c>
+      <c r="H49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>401</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>403</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>445</v>
+      </c>
+      <c r="B52" t="s">
+        <v>461</v>
+      </c>
+      <c r="C52" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" t="s">
+        <v>18</v>
+      </c>
+      <c r="K52" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>446</v>
+      </c>
+      <c r="B53" t="s">
+        <v>462</v>
+      </c>
+      <c r="C53" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="K53" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>19</v>
       </c>
-      <c r="B50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" t="s">
-        <v>84</v>
-      </c>
-      <c r="E50" t="s">
-        <v>14</v>
-      </c>
-      <c r="I50" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>415</v>
-      </c>
-      <c r="B51" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" t="s">
-        <v>86</v>
-      </c>
-      <c r="E51" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" t="s">
-        <v>89</v>
-      </c>
-      <c r="E52" t="s">
-        <v>14</v>
-      </c>
-      <c r="G52" t="s">
-        <v>416</v>
-      </c>
-      <c r="H52" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>415</v>
-      </c>
-      <c r="B53" t="s">
-        <v>91</v>
-      </c>
-      <c r="C53" t="s">
-        <v>92</v>
-      </c>
-      <c r="E53" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>9</v>
-      </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
-      </c>
-      <c r="I54" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="E54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>97</v>
-      </c>
-      <c r="E55" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="G55" t="s">
-        <v>416</v>
+        <v>488</v>
       </c>
       <c r="H55" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>109</v>
-      </c>
-      <c r="B56" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56" t="s">
-        <v>100</v>
-      </c>
-      <c r="E56" t="s">
-        <v>14</v>
-      </c>
-      <c r="G56" t="s">
-        <v>416</v>
-      </c>
-      <c r="H56" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>109</v>
-      </c>
-      <c r="B57" t="s">
-        <v>102</v>
-      </c>
-      <c r="C57" t="s">
-        <v>103</v>
-      </c>
-      <c r="E57" t="s">
-        <v>14</v>
-      </c>
-      <c r="G57" t="s">
-        <v>416</v>
-      </c>
-      <c r="H57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>415</v>
-      </c>
-      <c r="B58" t="s">
-        <v>105</v>
-      </c>
-      <c r="C58" t="s">
-        <v>106</v>
-      </c>
-      <c r="E58" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>108</v>
-      </c>
-      <c r="I59" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" t="s">
+        <v>563</v>
+      </c>
+      <c r="C61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I61" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" t="s">
+        <v>565</v>
+      </c>
+      <c r="C62" t="s">
+        <v>59</v>
+      </c>
+      <c r="E62" t="s">
+        <v>14</v>
+      </c>
+      <c r="J62" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>109</v>
       </c>
-      <c r="B60" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" t="s">
-        <v>417</v>
-      </c>
-      <c r="H60" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B63" t="s">
+        <v>566</v>
+      </c>
+      <c r="C63" t="s">
+        <v>519</v>
+      </c>
+      <c r="E63" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" t="s">
+        <v>512</v>
+      </c>
+      <c r="H63" t="s">
+        <v>514</v>
+      </c>
+      <c r="J63" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" t="s">
+        <v>567</v>
+      </c>
+      <c r="C64" t="s">
+        <v>520</v>
+      </c>
+      <c r="E64" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" t="s">
+        <v>513</v>
+      </c>
+      <c r="H64" t="s">
+        <v>515</v>
+      </c>
+      <c r="J64" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" t="s">
+        <v>568</v>
+      </c>
+      <c r="C65" t="s">
+        <v>63</v>
+      </c>
+      <c r="J65" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>409</v>
+      </c>
+      <c r="B66" t="s">
+        <v>569</v>
+      </c>
+      <c r="C66" t="s">
+        <v>65</v>
+      </c>
+      <c r="E66" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>9</v>
-      </c>
-      <c r="B65" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>114</v>
-      </c>
-      <c r="B66" t="s">
-        <v>115</v>
-      </c>
-      <c r="C66" t="s">
-        <v>116</v>
-      </c>
-      <c r="E66" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>450</v>
-      </c>
-      <c r="B67" t="s">
-        <v>117</v>
-      </c>
-      <c r="C67" t="s">
-        <v>118</v>
-      </c>
-      <c r="E67" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>119</v>
+        <v>571</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="I68" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>451</v>
+        <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="C69" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="E69" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>123</v>
+        <v>523</v>
       </c>
       <c r="C70" t="s">
-        <v>124</v>
+        <v>519</v>
       </c>
       <c r="E70" t="s">
         <v>14</v>
       </c>
       <c r="G70" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="H70" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>109</v>
+      </c>
+      <c r="B71" t="s">
+        <v>509</v>
+      </c>
+      <c r="C71" t="s">
+        <v>520</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" t="s">
+        <v>513</v>
+      </c>
+      <c r="H71" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>409</v>
+      </c>
+      <c r="B73" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" t="s">
+        <v>65</v>
+      </c>
+      <c r="E73" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>109</v>
-      </c>
-      <c r="B72" t="s">
-        <v>126</v>
-      </c>
-      <c r="C72" t="s">
-        <v>127</v>
-      </c>
-      <c r="D72" t="s">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>9</v>
+      </c>
+      <c r="B77" t="s">
+        <v>66</v>
+      </c>
+      <c r="C77" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" t="s">
+        <v>68</v>
+      </c>
+      <c r="C78" t="s">
+        <v>69</v>
+      </c>
+      <c r="E78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>60</v>
+      </c>
+      <c r="B79" t="s">
+        <v>70</v>
+      </c>
+      <c r="C79" t="s">
+        <v>71</v>
+      </c>
+      <c r="D79" t="s">
         <v>17</v>
       </c>
-      <c r="E72" t="s">
-        <v>14</v>
-      </c>
-      <c r="G72" t="s">
-        <v>416</v>
-      </c>
-      <c r="H72" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>415</v>
-      </c>
-      <c r="B73" t="s">
-        <v>129</v>
-      </c>
-      <c r="C73" t="s">
-        <v>130</v>
-      </c>
-      <c r="E73" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" t="s">
-        <v>131</v>
-      </c>
-      <c r="C74" t="s">
-        <v>132</v>
-      </c>
-      <c r="I74" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>114</v>
-      </c>
-      <c r="B75" t="s">
-        <v>133</v>
-      </c>
-      <c r="C75" t="s">
-        <v>134</v>
-      </c>
-      <c r="E75" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" t="s">
-        <v>506</v>
-      </c>
-      <c r="H75" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>114</v>
-      </c>
-      <c r="B76" t="s">
-        <v>136</v>
-      </c>
-      <c r="C76" t="s">
-        <v>137</v>
-      </c>
-      <c r="E76" t="s">
-        <v>14</v>
-      </c>
-      <c r="G76" t="s">
-        <v>507</v>
-      </c>
-      <c r="H76" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>19</v>
-      </c>
-      <c r="B77" t="s">
-        <v>139</v>
-      </c>
-      <c r="C77" t="s">
-        <v>140</v>
-      </c>
-      <c r="E77" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>415</v>
-      </c>
-      <c r="B78" t="s">
-        <v>141</v>
-      </c>
-      <c r="C78" t="s">
-        <v>142</v>
-      </c>
-      <c r="E78" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" t="s">
-        <v>143</v>
-      </c>
-      <c r="C79" t="s">
-        <v>144</v>
-      </c>
-      <c r="I79" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+      <c r="L79" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>109</v>
-      </c>
-      <c r="B80" t="s">
-        <v>145</v>
-      </c>
-      <c r="C80" t="s">
-        <v>146</v>
-      </c>
-      <c r="E80" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" t="s">
-        <v>417</v>
-      </c>
-      <c r="H80" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>9</v>
+      </c>
+      <c r="B82" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>447</v>
+      </c>
+      <c r="B83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C83" t="s">
+        <v>75</v>
+      </c>
+      <c r="E83" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" t="s">
+        <v>77</v>
+      </c>
+      <c r="C84" t="s">
+        <v>78</v>
+      </c>
+      <c r="D84" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>448</v>
       </c>
       <c r="B85" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>149</v>
+        <v>80</v>
+      </c>
+      <c r="E85" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>449</v>
+      </c>
+      <c r="B86" t="s">
+        <v>81</v>
+      </c>
+      <c r="C86" t="s">
+        <v>82</v>
+      </c>
+      <c r="E86" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>422</v>
+        <v>19</v>
       </c>
       <c r="B87" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
       <c r="C87" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
       </c>
-      <c r="F87" t="s">
-        <v>18</v>
+      <c r="I87" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>415</v>
       </c>
       <c r="B88" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
       <c r="C88" t="s">
-        <v>154</v>
+        <v>86</v>
+      </c>
+      <c r="E88" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>424</v>
+        <v>55</v>
       </c>
       <c r="B89" t="s">
-        <v>155</v>
+        <v>88</v>
       </c>
       <c r="C89" t="s">
-        <v>156</v>
+        <v>89</v>
+      </c>
+      <c r="E89" t="s">
+        <v>14</v>
+      </c>
+      <c r="G89" t="s">
+        <v>416</v>
+      </c>
+      <c r="H89" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>415</v>
       </c>
       <c r="B90" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="C90" t="s">
-        <v>158</v>
-      </c>
-      <c r="I90" t="s">
-        <v>471</v>
+        <v>92</v>
+      </c>
+      <c r="E90" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="C91" t="s">
-        <v>160</v>
-      </c>
-      <c r="E91" t="s">
-        <v>14</v>
-      </c>
-      <c r="G91" t="s">
-        <v>416</v>
-      </c>
-      <c r="H91" t="s">
-        <v>161</v>
+        <v>95</v>
+      </c>
+      <c r="I91" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>109</v>
+      </c>
+      <c r="B92" t="s">
+        <v>96</v>
+      </c>
+      <c r="C92" t="s">
+        <v>97</v>
+      </c>
+      <c r="E92" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" t="s">
+        <v>416</v>
+      </c>
+      <c r="H92" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B93" t="s">
-        <v>162</v>
+        <v>99</v>
       </c>
       <c r="C93" t="s">
-        <v>163</v>
-      </c>
-      <c r="I93" t="s">
-        <v>472</v>
+        <v>100</v>
+      </c>
+      <c r="E93" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" t="s">
+        <v>416</v>
+      </c>
+      <c r="H93" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>164</v>
+        <v>102</v>
       </c>
       <c r="C94" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="E94" t="s">
         <v>14</v>
       </c>
       <c r="G94" t="s">
-        <v>506</v>
+        <v>416</v>
       </c>
       <c r="H94" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>415</v>
       </c>
       <c r="B95" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="C95" t="s">
-        <v>168</v>
-      </c>
-      <c r="I95" t="s">
-        <v>471</v>
+        <v>106</v>
+      </c>
+      <c r="E95" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>169</v>
+        <v>107</v>
       </c>
       <c r="C96" t="s">
-        <v>170</v>
-      </c>
-      <c r="E96" t="s">
-        <v>14</v>
+        <v>108</v>
+      </c>
+      <c r="I96" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -3434,41 +3647,29 @@
         <v>109</v>
       </c>
       <c r="B97" t="s">
-        <v>171</v>
+        <v>110</v>
       </c>
       <c r="C97" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
+      </c>
+      <c r="G97" t="s">
+        <v>417</v>
+      </c>
+      <c r="H97" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>109</v>
-      </c>
-      <c r="B98" t="s">
-        <v>173</v>
-      </c>
-      <c r="C98" t="s">
-        <v>174</v>
-      </c>
-      <c r="E98" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>109</v>
-      </c>
-      <c r="B99" t="s">
-        <v>175</v>
-      </c>
-      <c r="C99" t="s">
-        <v>176</v>
-      </c>
-      <c r="E99" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -3476,137 +3677,173 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>452</v>
-      </c>
-      <c r="B101" t="s">
-        <v>177</v>
-      </c>
-      <c r="C101" t="s">
-        <v>178</v>
-      </c>
-      <c r="E101" t="s">
-        <v>14</v>
-      </c>
-      <c r="F101" t="s">
-        <v>18</v>
-      </c>
-      <c r="I101" t="s">
-        <v>472</v>
-      </c>
-    </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B102" t="s">
-        <v>179</v>
+        <v>112</v>
       </c>
       <c r="C102" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>41</v>
+        <v>114</v>
+      </c>
+      <c r="B103" t="s">
+        <v>115</v>
+      </c>
+      <c r="C103" t="s">
+        <v>116</v>
+      </c>
+      <c r="E103" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>181</v>
+        <v>450</v>
+      </c>
+      <c r="B104" t="s">
+        <v>117</v>
+      </c>
+      <c r="C104" t="s">
+        <v>118</v>
+      </c>
+      <c r="E104" t="s">
+        <v>14</v>
+      </c>
+      <c r="F104" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105" t="s">
+        <v>119</v>
+      </c>
+      <c r="C105" t="s">
+        <v>120</v>
+      </c>
+      <c r="I105" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>422</v>
+        <v>451</v>
       </c>
       <c r="B106" t="s">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="C106" t="s">
-        <v>183</v>
+        <v>122</v>
       </c>
       <c r="E106" t="s">
         <v>14</v>
-      </c>
-      <c r="F106" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="B107" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
       <c r="C107" t="s">
-        <v>185</v>
+        <v>124</v>
+      </c>
+      <c r="E107" t="s">
+        <v>14</v>
+      </c>
+      <c r="G107" t="s">
+        <v>506</v>
+      </c>
+      <c r="H107" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>426</v>
-      </c>
-      <c r="B108" t="s">
-        <v>186</v>
-      </c>
-      <c r="C108" t="s">
-        <v>187</v>
+        <v>41</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>188</v>
+        <v>126</v>
       </c>
       <c r="C109" t="s">
-        <v>189</v>
-      </c>
-      <c r="I109" t="s">
-        <v>473</v>
+        <v>127</v>
+      </c>
+      <c r="D109" t="s">
+        <v>17</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+      <c r="G109" t="s">
+        <v>416</v>
+      </c>
+      <c r="H109" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>55</v>
+        <v>415</v>
       </c>
       <c r="B110" t="s">
-        <v>190</v>
+        <v>129</v>
       </c>
       <c r="C110" t="s">
-        <v>191</v>
+        <v>130</v>
       </c>
       <c r="E110" t="s">
         <v>14</v>
       </c>
-      <c r="G110" t="s">
-        <v>416</v>
-      </c>
-      <c r="H110" t="s">
-        <v>161</v>
+      <c r="F110" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>41</v>
+        <v>9</v>
+      </c>
+      <c r="B111" t="s">
+        <v>131</v>
+      </c>
+      <c r="C111" t="s">
+        <v>132</v>
+      </c>
+      <c r="I111" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>192</v>
+        <v>133</v>
       </c>
       <c r="C112" t="s">
-        <v>193</v>
-      </c>
-      <c r="I112" t="s">
-        <v>474</v>
+        <v>134</v>
+      </c>
+      <c r="E112" t="s">
+        <v>14</v>
+      </c>
+      <c r="G112" t="s">
+        <v>506</v>
+      </c>
+      <c r="H112" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
@@ -3614,105 +3851,99 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
       <c r="C113" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
       </c>
       <c r="G113" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="H113" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>429</v>
+        <v>525</v>
       </c>
       <c r="B114" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="C114" t="s">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="E114" t="s">
         <v>14</v>
-      </c>
-      <c r="F114" t="s">
-        <v>18</v>
-      </c>
-      <c r="I114" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>19</v>
+        <v>415</v>
       </c>
       <c r="B115" t="s">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="C115" t="s">
-        <v>180</v>
+        <v>142</v>
+      </c>
+      <c r="E115" t="s">
+        <v>14</v>
+      </c>
+      <c r="F115" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>41</v>
+        <v>9</v>
+      </c>
+      <c r="B116" t="s">
+        <v>143</v>
+      </c>
+      <c r="C116" t="s">
+        <v>144</v>
+      </c>
+      <c r="I116" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>181</v>
+        <v>109</v>
+      </c>
+      <c r="B117" t="s">
+        <v>145</v>
+      </c>
+      <c r="C117" t="s">
+        <v>146</v>
+      </c>
+      <c r="E117" t="s">
+        <v>14</v>
+      </c>
+      <c r="G117" t="s">
+        <v>417</v>
+      </c>
+      <c r="H117" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>422</v>
-      </c>
-      <c r="B119" t="s">
-        <v>198</v>
-      </c>
-      <c r="C119" t="s">
-        <v>199</v>
-      </c>
-      <c r="E119" t="s">
-        <v>14</v>
-      </c>
-      <c r="F119" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>152</v>
-      </c>
-      <c r="B120" t="s">
-        <v>200</v>
-      </c>
-      <c r="C120" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>431</v>
-      </c>
-      <c r="B121" t="s">
-        <v>202</v>
-      </c>
-      <c r="C121" t="s">
-        <v>203</v>
-      </c>
-      <c r="E121" t="s">
-        <v>14</v>
-      </c>
-      <c r="F121" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
@@ -3720,211 +3951,217 @@
         <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>204</v>
+        <v>148</v>
       </c>
       <c r="C122" t="s">
-        <v>205</v>
-      </c>
-      <c r="I122" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>55</v>
-      </c>
-      <c r="B123" t="s">
-        <v>206</v>
-      </c>
-      <c r="C123" t="s">
-        <v>207</v>
-      </c>
-      <c r="E123" t="s">
-        <v>14</v>
-      </c>
-      <c r="G123" t="s">
-        <v>416</v>
-      </c>
-      <c r="H123" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>422</v>
+      </c>
+      <c r="B124" t="s">
+        <v>150</v>
+      </c>
+      <c r="C124" t="s">
+        <v>151</v>
+      </c>
+      <c r="E124" t="s">
+        <v>14</v>
+      </c>
+      <c r="F124" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>9</v>
+        <v>152</v>
       </c>
       <c r="B125" t="s">
-        <v>208</v>
+        <v>153</v>
       </c>
       <c r="C125" t="s">
-        <v>209</v>
-      </c>
-      <c r="I125" t="s">
-        <v>477</v>
+        <v>154</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>114</v>
+        <v>424</v>
       </c>
       <c r="B126" t="s">
-        <v>210</v>
+        <v>155</v>
       </c>
       <c r="C126" t="s">
-        <v>165</v>
-      </c>
-      <c r="E126" t="s">
-        <v>14</v>
-      </c>
-      <c r="G126" t="s">
-        <v>506</v>
-      </c>
-      <c r="H126" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B127" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="C127" t="s">
-        <v>180</v>
+        <v>158</v>
+      </c>
+      <c r="I127" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>41</v>
+        <v>55</v>
+      </c>
+      <c r="B128" t="s">
+        <v>159</v>
+      </c>
+      <c r="C128" t="s">
+        <v>160</v>
+      </c>
+      <c r="E128" t="s">
+        <v>14</v>
+      </c>
+      <c r="G128" t="s">
+        <v>416</v>
+      </c>
+      <c r="H128" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>181</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" t="s">
+        <v>162</v>
+      </c>
+      <c r="C130" t="s">
+        <v>163</v>
+      </c>
+      <c r="I130" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>422</v>
+        <v>114</v>
       </c>
       <c r="B131" t="s">
-        <v>212</v>
+        <v>164</v>
       </c>
       <c r="C131" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="E131" t="s">
         <v>14</v>
       </c>
-      <c r="F131" t="s">
-        <v>18</v>
+      <c r="G131" t="s">
+        <v>506</v>
+      </c>
+      <c r="H131" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="B132" t="s">
-        <v>214</v>
+        <v>167</v>
       </c>
       <c r="C132" t="s">
-        <v>215</v>
+        <v>168</v>
+      </c>
+      <c r="I132" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>433</v>
+        <v>19</v>
       </c>
       <c r="B133" t="s">
-        <v>216</v>
+        <v>169</v>
       </c>
       <c r="C133" t="s">
-        <v>217</v>
+        <v>170</v>
       </c>
       <c r="E133" t="s">
         <v>14</v>
-      </c>
-      <c r="F133" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B134" t="s">
-        <v>218</v>
+        <v>171</v>
       </c>
       <c r="C134" t="s">
-        <v>219</v>
-      </c>
-      <c r="I134" t="s">
-        <v>478</v>
+        <v>172</v>
+      </c>
+      <c r="E134" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B135" t="s">
-        <v>220</v>
+        <v>173</v>
       </c>
       <c r="C135" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="E135" t="s">
         <v>14</v>
-      </c>
-      <c r="G135" t="s">
-        <v>416</v>
-      </c>
-      <c r="H135" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>41</v>
+        <v>109</v>
+      </c>
+      <c r="B136" t="s">
+        <v>175</v>
+      </c>
+      <c r="C136" t="s">
+        <v>176</v>
+      </c>
+      <c r="E136" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>9</v>
-      </c>
-      <c r="B137" t="s">
-        <v>222</v>
-      </c>
-      <c r="C137" t="s">
-        <v>223</v>
-      </c>
-      <c r="I137" t="s">
-        <v>479</v>
+        <v>41</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>114</v>
+        <v>452</v>
       </c>
       <c r="B138" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="C138" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="E138" t="s">
         <v>14</v>
       </c>
-      <c r="G138" t="s">
-        <v>506</v>
-      </c>
-      <c r="H138" t="s">
-        <v>166</v>
+      <c r="F138" t="s">
+        <v>18</v>
+      </c>
+      <c r="I138" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
@@ -3932,7 +4169,7 @@
         <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="C139" t="s">
         <v>180</v>
@@ -3953,10 +4190,10 @@
         <v>422</v>
       </c>
       <c r="B143" t="s">
-        <v>226</v>
+        <v>182</v>
       </c>
       <c r="C143" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="E143" t="s">
         <v>14</v>
@@ -3970,27 +4207,21 @@
         <v>152</v>
       </c>
       <c r="B144" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="C144" t="s">
-        <v>229</v>
+        <v>185</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B145" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="C145" t="s">
-        <v>231</v>
-      </c>
-      <c r="E145" t="s">
-        <v>14</v>
-      </c>
-      <c r="F145" t="s">
-        <v>18</v>
+        <v>187</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
@@ -3998,13 +4229,13 @@
         <v>9</v>
       </c>
       <c r="B146" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
       <c r="C146" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="I146" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
@@ -4012,10 +4243,10 @@
         <v>55</v>
       </c>
       <c r="B147" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="C147" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="E147" t="s">
         <v>14</v>
@@ -4037,13 +4268,13 @@
         <v>9</v>
       </c>
       <c r="B149" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
       <c r="C149" t="s">
-        <v>237</v>
+        <v>193</v>
       </c>
       <c r="I149" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
@@ -4051,7 +4282,7 @@
         <v>114</v>
       </c>
       <c r="B150" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
       <c r="C150" t="s">
         <v>165</v>
@@ -4068,33 +4299,33 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>9</v>
+        <v>429</v>
       </c>
       <c r="B151" t="s">
-        <v>239</v>
+        <v>195</v>
       </c>
       <c r="C151" t="s">
-        <v>240</v>
+        <v>196</v>
+      </c>
+      <c r="E151" t="s">
+        <v>14</v>
+      </c>
+      <c r="F151" t="s">
+        <v>18</v>
+      </c>
+      <c r="I151" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>453</v>
+        <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>241</v>
+        <v>197</v>
       </c>
       <c r="C152" t="s">
-        <v>242</v>
-      </c>
-      <c r="E152" t="s">
-        <v>14</v>
-      </c>
-      <c r="F152" t="s">
-        <v>18</v>
-      </c>
-      <c r="I152" t="s">
-        <v>482</v>
+        <v>180</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
@@ -4104,59 +4335,86 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>9</v>
-      </c>
-      <c r="B154" t="s">
-        <v>243</v>
-      </c>
-      <c r="C154" t="s">
-        <v>244</v>
-      </c>
-      <c r="I154" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>437</v>
-      </c>
-      <c r="B155" t="s">
-        <v>245</v>
-      </c>
-      <c r="C155" t="s">
-        <v>246</v>
-      </c>
-      <c r="E155" t="s">
-        <v>14</v>
-      </c>
-      <c r="F155" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>41</v>
+        <v>422</v>
+      </c>
+      <c r="B156" t="s">
+        <v>198</v>
+      </c>
+      <c r="C156" t="s">
+        <v>199</v>
+      </c>
+      <c r="E156" t="s">
+        <v>14</v>
+      </c>
+      <c r="F156" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="B157" t="s">
-        <v>247</v>
+        <v>200</v>
       </c>
       <c r="C157" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>41</v>
+        <v>431</v>
+      </c>
+      <c r="B158" t="s">
+        <v>202</v>
+      </c>
+      <c r="C158" t="s">
+        <v>203</v>
+      </c>
+      <c r="E158" t="s">
+        <v>14</v>
+      </c>
+      <c r="F158" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>181</v>
+        <v>9</v>
+      </c>
+      <c r="B159" t="s">
+        <v>204</v>
+      </c>
+      <c r="C159" t="s">
+        <v>205</v>
+      </c>
+      <c r="I159" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>55</v>
+      </c>
+      <c r="B160" t="s">
+        <v>206</v>
+      </c>
+      <c r="C160" t="s">
+        <v>207</v>
+      </c>
+      <c r="E160" t="s">
+        <v>14</v>
+      </c>
+      <c r="G160" t="s">
+        <v>416</v>
+      </c>
+      <c r="H160" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
@@ -4164,103 +4422,70 @@
         <v>41</v>
       </c>
     </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>9</v>
+      </c>
+      <c r="B162" t="s">
+        <v>208</v>
+      </c>
+      <c r="C162" t="s">
+        <v>209</v>
+      </c>
+      <c r="I162" t="s">
+        <v>477</v>
+      </c>
+    </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B163" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="C163" t="s">
-        <v>249</v>
+        <v>165</v>
+      </c>
+      <c r="E163" t="s">
+        <v>14</v>
+      </c>
+      <c r="G163" t="s">
+        <v>506</v>
+      </c>
+      <c r="H163" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="B164" t="s">
-        <v>250</v>
+        <v>211</v>
       </c>
       <c r="C164" t="s">
-        <v>251</v>
-      </c>
-      <c r="E164" t="s">
-        <v>14</v>
-      </c>
-      <c r="G164" t="s">
-        <v>506</v>
-      </c>
-      <c r="H164" t="s">
-        <v>252</v>
+        <v>180</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>439</v>
-      </c>
-      <c r="B165" t="s">
-        <v>253</v>
-      </c>
-      <c r="C165" t="s">
-        <v>254</v>
-      </c>
-      <c r="E165" t="s">
-        <v>14</v>
-      </c>
-      <c r="F165" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>109</v>
-      </c>
-      <c r="B166" t="s">
-        <v>255</v>
-      </c>
-      <c r="C166" t="s">
-        <v>256</v>
-      </c>
-      <c r="E166" t="s">
-        <v>14</v>
-      </c>
-      <c r="G166" t="s">
-        <v>416</v>
-      </c>
-      <c r="H166" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
-        <v>109</v>
-      </c>
-      <c r="B167" t="s">
-        <v>258</v>
-      </c>
-      <c r="C167" t="s">
-        <v>259</v>
-      </c>
-      <c r="E167" t="s">
-        <v>14</v>
-      </c>
-      <c r="G167" t="s">
-        <v>416</v>
-      </c>
-      <c r="H167" t="s">
-        <v>260</v>
+        <v>181</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>454</v>
+        <v>422</v>
       </c>
       <c r="B168" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
       <c r="C168" t="s">
-        <v>262</v>
+        <v>213</v>
       </c>
       <c r="E168" t="s">
         <v>14</v>
@@ -4271,39 +4496,30 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="B169" t="s">
-        <v>263</v>
+        <v>214</v>
       </c>
       <c r="C169" t="s">
-        <v>264</v>
-      </c>
-      <c r="E169" t="s">
-        <v>14</v>
-      </c>
-      <c r="G169" t="s">
-        <v>416</v>
-      </c>
-      <c r="H169" t="s">
-        <v>265</v>
+        <v>215</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="B170" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="C170" t="s">
-        <v>92</v>
+        <v>217</v>
       </c>
       <c r="E170" t="s">
         <v>14</v>
       </c>
       <c r="F170" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
@@ -4311,112 +4527,88 @@
         <v>9</v>
       </c>
       <c r="B171" t="s">
-        <v>267</v>
+        <v>218</v>
       </c>
       <c r="C171" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="I171" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>443</v>
+        <v>55</v>
       </c>
       <c r="B172" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
       <c r="C172" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="E172" t="s">
         <v>14</v>
+      </c>
+      <c r="G172" t="s">
+        <v>416</v>
+      </c>
+      <c r="H172" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>415</v>
-      </c>
-      <c r="B173" t="s">
-        <v>271</v>
-      </c>
-      <c r="C173" t="s">
-        <v>106</v>
-      </c>
-      <c r="E173" t="s">
-        <v>14</v>
-      </c>
-      <c r="F173" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="B174" t="s">
-        <v>272</v>
+        <v>222</v>
       </c>
       <c r="C174" t="s">
-        <v>273</v>
+        <v>223</v>
       </c>
       <c r="I174" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>455</v>
+        <v>114</v>
       </c>
       <c r="B175" t="s">
-        <v>274</v>
+        <v>224</v>
       </c>
       <c r="C175" t="s">
-        <v>275</v>
+        <v>165</v>
       </c>
       <c r="E175" t="s">
         <v>14</v>
+      </c>
+      <c r="G175" t="s">
+        <v>506</v>
+      </c>
+      <c r="H175" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="B176" t="s">
-        <v>276</v>
+        <v>225</v>
       </c>
       <c r="C176" t="s">
-        <v>277</v>
-      </c>
-      <c r="E176" t="s">
-        <v>14</v>
-      </c>
-      <c r="G176" t="s">
-        <v>416</v>
-      </c>
-      <c r="H176" t="s">
-        <v>278</v>
+        <v>180</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>109</v>
-      </c>
-      <c r="B177" t="s">
-        <v>279</v>
-      </c>
-      <c r="C177" t="s">
-        <v>280</v>
-      </c>
-      <c r="E177" t="s">
-        <v>14</v>
-      </c>
-      <c r="G177" t="s">
-        <v>416</v>
-      </c>
-      <c r="H177" t="s">
-        <v>281</v>
+        <v>41</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
@@ -4424,110 +4616,122 @@
         <v>181</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
-        <v>41</v>
-      </c>
-    </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>41</v>
+        <v>422</v>
+      </c>
+      <c r="B180" t="s">
+        <v>226</v>
+      </c>
+      <c r="C180" t="s">
+        <v>227</v>
+      </c>
+      <c r="E180" t="s">
+        <v>14</v>
+      </c>
+      <c r="F180" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>152</v>
+      </c>
+      <c r="B181" t="s">
+        <v>228</v>
+      </c>
+      <c r="C181" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>9</v>
+        <v>433</v>
       </c>
       <c r="B182" t="s">
-        <v>282</v>
+        <v>230</v>
       </c>
       <c r="C182" t="s">
-        <v>283</v>
+        <v>231</v>
+      </c>
+      <c r="E182" t="s">
+        <v>14</v>
+      </c>
+      <c r="F182" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>415</v>
+        <v>9</v>
       </c>
       <c r="B183" t="s">
-        <v>284</v>
+        <v>232</v>
       </c>
       <c r="C183" t="s">
-        <v>285</v>
-      </c>
-      <c r="E183" t="s">
-        <v>14</v>
-      </c>
-      <c r="F183" t="s">
-        <v>87</v>
+        <v>233</v>
+      </c>
+      <c r="I183" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>415</v>
+        <v>55</v>
       </c>
       <c r="B184" t="s">
-        <v>286</v>
+        <v>234</v>
       </c>
       <c r="C184" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
       <c r="E184" t="s">
         <v>14</v>
       </c>
-      <c r="F184" t="s">
-        <v>93</v>
+      <c r="G184" t="s">
+        <v>416</v>
+      </c>
+      <c r="H184" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>9</v>
-      </c>
-      <c r="B185" t="s">
-        <v>287</v>
-      </c>
-      <c r="C185" t="s">
-        <v>288</v>
-      </c>
-      <c r="I185" t="s">
-        <v>486</v>
+        <v>41</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="B186" t="s">
-        <v>289</v>
+        <v>236</v>
       </c>
       <c r="C186" t="s">
-        <v>290</v>
-      </c>
-      <c r="E186" t="s">
-        <v>14</v>
-      </c>
-      <c r="G186" t="s">
-        <v>416</v>
-      </c>
-      <c r="H186" t="s">
-        <v>291</v>
+        <v>237</v>
+      </c>
+      <c r="I186" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>415</v>
+        <v>114</v>
       </c>
       <c r="B187" t="s">
-        <v>292</v>
+        <v>238</v>
       </c>
       <c r="C187" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="E187" t="s">
         <v>14</v>
       </c>
-      <c r="F187" t="s">
-        <v>93</v>
+      <c r="G187" t="s">
+        <v>506</v>
+      </c>
+      <c r="H187" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
@@ -4535,88 +4739,552 @@
         <v>9</v>
       </c>
       <c r="B188" t="s">
-        <v>293</v>
+        <v>239</v>
       </c>
       <c r="C188" t="s">
-        <v>294</v>
-      </c>
-      <c r="I188" t="s">
-        <v>487</v>
+        <v>240</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>114</v>
+        <v>453</v>
       </c>
       <c r="B189" t="s">
-        <v>295</v>
+        <v>241</v>
       </c>
       <c r="C189" t="s">
-        <v>296</v>
+        <v>242</v>
       </c>
       <c r="E189" t="s">
         <v>14</v>
       </c>
-      <c r="G189" t="s">
-        <v>508</v>
-      </c>
-      <c r="H189" t="s">
-        <v>297</v>
+      <c r="F189" t="s">
+        <v>18</v>
+      </c>
+      <c r="I189" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>152</v>
-      </c>
-      <c r="B190" t="s">
-        <v>298</v>
-      </c>
-      <c r="C190" t="s">
-        <v>299</v>
+        <v>41</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="B191" t="s">
-        <v>300</v>
+        <v>243</v>
       </c>
       <c r="C191" t="s">
-        <v>301</v>
-      </c>
-      <c r="E191" t="s">
-        <v>14</v>
+        <v>244</v>
+      </c>
+      <c r="I191" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>437</v>
+      </c>
+      <c r="B192" t="s">
+        <v>245</v>
+      </c>
+      <c r="C192" t="s">
+        <v>246</v>
+      </c>
+      <c r="E192" t="s">
+        <v>14</v>
+      </c>
+      <c r="F192" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
         <v>19</v>
       </c>
-      <c r="B192" t="s">
-        <v>302</v>
-      </c>
-      <c r="C192" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A194" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B194" t="s">
+        <v>247</v>
+      </c>
+      <c r="C194" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>9</v>
+      </c>
+      <c r="B200" t="s">
+        <v>248</v>
+      </c>
+      <c r="C200" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>114</v>
+      </c>
+      <c r="B201" t="s">
+        <v>250</v>
+      </c>
+      <c r="C201" t="s">
+        <v>251</v>
+      </c>
+      <c r="E201" t="s">
+        <v>14</v>
+      </c>
+      <c r="G201" t="s">
+        <v>506</v>
+      </c>
+      <c r="H201" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>439</v>
+      </c>
+      <c r="B202" t="s">
+        <v>253</v>
+      </c>
+      <c r="C202" t="s">
+        <v>254</v>
+      </c>
+      <c r="E202" t="s">
+        <v>14</v>
+      </c>
+      <c r="F202" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>109</v>
+      </c>
+      <c r="B203" t="s">
+        <v>255</v>
+      </c>
+      <c r="C203" t="s">
+        <v>256</v>
+      </c>
+      <c r="E203" t="s">
+        <v>14</v>
+      </c>
+      <c r="G203" t="s">
+        <v>416</v>
+      </c>
+      <c r="H203" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>109</v>
+      </c>
+      <c r="B204" t="s">
+        <v>258</v>
+      </c>
+      <c r="C204" t="s">
+        <v>259</v>
+      </c>
+      <c r="E204" t="s">
+        <v>14</v>
+      </c>
+      <c r="G204" t="s">
+        <v>416</v>
+      </c>
+      <c r="H204" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>454</v>
+      </c>
+      <c r="B205" t="s">
+        <v>261</v>
+      </c>
+      <c r="C205" t="s">
+        <v>262</v>
+      </c>
+      <c r="E205" t="s">
+        <v>14</v>
+      </c>
+      <c r="F205" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>109</v>
+      </c>
+      <c r="B206" t="s">
+        <v>263</v>
+      </c>
+      <c r="C206" t="s">
+        <v>264</v>
+      </c>
+      <c r="E206" t="s">
+        <v>14</v>
+      </c>
+      <c r="G206" t="s">
+        <v>416</v>
+      </c>
+      <c r="H206" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>415</v>
+      </c>
+      <c r="B207" t="s">
+        <v>266</v>
+      </c>
+      <c r="C207" t="s">
+        <v>92</v>
+      </c>
+      <c r="E207" t="s">
+        <v>14</v>
+      </c>
+      <c r="F207" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>9</v>
+      </c>
+      <c r="B208" t="s">
+        <v>267</v>
+      </c>
+      <c r="C208" t="s">
+        <v>268</v>
+      </c>
+      <c r="I208" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>443</v>
+      </c>
+      <c r="B209" t="s">
+        <v>269</v>
+      </c>
+      <c r="C209" t="s">
+        <v>270</v>
+      </c>
+      <c r="E209" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>415</v>
+      </c>
+      <c r="B210" t="s">
+        <v>271</v>
+      </c>
+      <c r="C210" t="s">
+        <v>106</v>
+      </c>
+      <c r="E210" t="s">
+        <v>14</v>
+      </c>
+      <c r="F210" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>152</v>
+      </c>
+      <c r="B211" t="s">
+        <v>272</v>
+      </c>
+      <c r="C211" t="s">
+        <v>273</v>
+      </c>
+      <c r="I211" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>455</v>
+      </c>
+      <c r="B212" t="s">
+        <v>274</v>
+      </c>
+      <c r="C212" t="s">
+        <v>275</v>
+      </c>
+      <c r="E212" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>55</v>
+      </c>
+      <c r="B213" t="s">
+        <v>276</v>
+      </c>
+      <c r="C213" t="s">
+        <v>277</v>
+      </c>
+      <c r="E213" t="s">
+        <v>14</v>
+      </c>
+      <c r="G213" t="s">
+        <v>416</v>
+      </c>
+      <c r="H213" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>109</v>
+      </c>
+      <c r="B214" t="s">
+        <v>279</v>
+      </c>
+      <c r="C214" t="s">
+        <v>280</v>
+      </c>
+      <c r="E214" t="s">
+        <v>14</v>
+      </c>
+      <c r="G214" t="s">
+        <v>416</v>
+      </c>
+      <c r="H214" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>9</v>
+      </c>
+      <c r="B219" t="s">
+        <v>282</v>
+      </c>
+      <c r="C219" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>415</v>
+      </c>
+      <c r="B220" t="s">
+        <v>284</v>
+      </c>
+      <c r="C220" t="s">
+        <v>285</v>
+      </c>
+      <c r="E220" t="s">
+        <v>14</v>
+      </c>
+      <c r="F220" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>415</v>
+      </c>
+      <c r="B221" t="s">
+        <v>286</v>
+      </c>
+      <c r="C221" t="s">
+        <v>92</v>
+      </c>
+      <c r="E221" t="s">
+        <v>14</v>
+      </c>
+      <c r="F221" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>9</v>
+      </c>
+      <c r="B222" t="s">
+        <v>287</v>
+      </c>
+      <c r="C222" t="s">
+        <v>288</v>
+      </c>
+      <c r="I222" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>109</v>
+      </c>
+      <c r="B223" t="s">
+        <v>289</v>
+      </c>
+      <c r="C223" t="s">
+        <v>290</v>
+      </c>
+      <c r="E223" t="s">
+        <v>14</v>
+      </c>
+      <c r="G223" t="s">
+        <v>416</v>
+      </c>
+      <c r="H223" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>415</v>
+      </c>
+      <c r="B224" t="s">
+        <v>292</v>
+      </c>
+      <c r="C224" t="s">
+        <v>106</v>
+      </c>
+      <c r="E224" t="s">
+        <v>14</v>
+      </c>
+      <c r="F224" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>9</v>
+      </c>
+      <c r="B225" t="s">
+        <v>293</v>
+      </c>
+      <c r="C225" t="s">
+        <v>294</v>
+      </c>
+      <c r="I225" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>114</v>
+      </c>
+      <c r="B226" t="s">
+        <v>295</v>
+      </c>
+      <c r="C226" t="s">
+        <v>296</v>
+      </c>
+      <c r="E226" t="s">
+        <v>14</v>
+      </c>
+      <c r="G226" t="s">
+        <v>508</v>
+      </c>
+      <c r="H226" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>152</v>
+      </c>
+      <c r="B227" t="s">
+        <v>298</v>
+      </c>
+      <c r="C227" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>109</v>
+      </c>
+      <c r="B228" t="s">
+        <v>300</v>
+      </c>
+      <c r="C228" t="s">
+        <v>301</v>
+      </c>
+      <c r="E228" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>19</v>
+      </c>
+      <c r="B229" t="s">
+        <v>302</v>
+      </c>
+      <c r="C229" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4628,11 +5296,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5642,6 +6310,17 @@
         <v>18</v>
       </c>
       <c r="C90" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>524</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" t="s">
         <v>442</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the field unit for perfomance crop in odk
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$233</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$234</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="583">
   <si>
     <t>type</t>
   </si>
@@ -804,9 +804,6 @@
     <t>harvest_crop_production</t>
   </si>
   <si>
-    <t>Producción del cultivo (ha)</t>
-  </si>
-  <si>
     <t>La producción de cultivo debe ser mayor a 0</t>
   </si>
   <si>
@@ -1741,6 +1738,42 @@
   </si>
   <si>
     <t>farm_group</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>ton</t>
+  </si>
+  <si>
+    <t>qui</t>
+  </si>
+  <si>
+    <t>Quintales</t>
+  </si>
+  <si>
+    <t>Tonelada (ton)</t>
+  </si>
+  <si>
+    <t>Kilogramo (kg)</t>
+  </si>
+  <si>
+    <t>choices_harvest_performance_unit</t>
+  </si>
+  <si>
+    <t>select_one choices_harvest_performance_unit</t>
+  </si>
+  <si>
+    <t>harvest_crop_production_unit</t>
+  </si>
+  <si>
+    <t>Unidad de medida para producción del cultivo</t>
+  </si>
+  <si>
+    <t>Producción del cultivo ( ${harvest_crop_production_unit} )</t>
+  </si>
+  <si>
+    <t>Finca en la base de datos</t>
   </si>
 </sst>
 </file>
@@ -2146,11 +2179,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L233"/>
+  <dimension ref="A1:L234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2167,10 +2200,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" t="s">
         <v>393</v>
-      </c>
-      <c r="D1" t="s">
-        <v>394</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2182,7 +2215,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2210,7 +2243,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2224,7 +2257,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2256,21 +2289,21 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>525</v>
+      </c>
+      <c r="B6" t="s">
         <v>526</v>
       </c>
-      <c r="B6" t="s">
+      <c r="J6" t="s">
         <v>527</v>
-      </c>
-      <c r="J6" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2278,13 +2311,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2292,7 +2325,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -2301,13 +2334,13 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J8" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -2315,7 +2348,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -2324,13 +2357,13 @@
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2338,7 +2371,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -2347,21 +2380,21 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
       </c>
       <c r="J10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B11" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -2370,15 +2403,15 @@
         <v>14</v>
       </c>
       <c r="J11" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
@@ -2387,15 +2420,15 @@
         <v>14</v>
       </c>
       <c r="J12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -2404,15 +2437,15 @@
         <v>14</v>
       </c>
       <c r="K13" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B14" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
@@ -2421,7 +2454,7 @@
         <v>14</v>
       </c>
       <c r="K14" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2429,7 +2462,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
@@ -2438,7 +2471,7 @@
         <v>14</v>
       </c>
       <c r="J15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2446,7 +2479,7 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C16" t="s">
         <v>39</v>
@@ -2455,13 +2488,13 @@
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H16" t="s">
         <v>40</v>
       </c>
       <c r="J16" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2474,13 +2507,13 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="I18" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -2497,10 +2530,10 @@
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2517,10 +2550,10 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2537,7 +2570,7 @@
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H21" t="s">
         <v>28</v>
@@ -2545,7 +2578,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -2559,7 +2592,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
@@ -2576,10 +2609,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B24" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -2591,15 +2624,15 @@
         <v>18</v>
       </c>
       <c r="K24" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B25" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
@@ -2611,7 +2644,7 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -2642,7 +2675,7 @@
         <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H27" t="s">
         <v>40</v>
@@ -2671,7 +2704,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
@@ -2697,21 +2730,21 @@
         <v>14</v>
       </c>
       <c r="G33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B34" t="s">
+        <v>542</v>
+      </c>
+      <c r="J34" t="s">
         <v>543</v>
-      </c>
-      <c r="J34" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -2719,13 +2752,13 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
+        <v>544</v>
+      </c>
+      <c r="C35" t="s">
         <v>545</v>
       </c>
-      <c r="C35" t="s">
+      <c r="I35" t="s">
         <v>546</v>
-      </c>
-      <c r="I35" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -2733,7 +2766,7 @@
         <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -2742,13 +2775,13 @@
         <v>14</v>
       </c>
       <c r="G36" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H36" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J36" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -2756,7 +2789,7 @@
         <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C37" t="s">
         <v>25</v>
@@ -2765,13 +2798,13 @@
         <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H37" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -2779,7 +2812,7 @@
         <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C38" t="s">
         <v>27</v>
@@ -2788,21 +2821,21 @@
         <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H38" t="s">
         <v>28</v>
       </c>
       <c r="J38" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B39" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C39" t="s">
         <v>30</v>
@@ -2811,15 +2844,15 @@
         <v>14</v>
       </c>
       <c r="J39" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B40" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C40" t="s">
         <v>32</v>
@@ -2828,15 +2861,15 @@
         <v>14</v>
       </c>
       <c r="J40" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B41" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
@@ -2845,15 +2878,15 @@
         <v>14</v>
       </c>
       <c r="K41" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B42" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C42" t="s">
         <v>35</v>
@@ -2862,7 +2895,7 @@
         <v>14</v>
       </c>
       <c r="K42" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2870,7 +2903,7 @@
         <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C43" t="s">
         <v>37</v>
@@ -2879,7 +2912,7 @@
         <v>14</v>
       </c>
       <c r="J43" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2887,19 +2920,19 @@
         <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C44" t="s">
         <v>39</v>
       </c>
       <c r="G44" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H44" t="s">
         <v>40</v>
       </c>
       <c r="J44" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2912,13 +2945,13 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C46" t="s">
         <v>43</v>
       </c>
       <c r="I46" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2935,10 +2968,10 @@
         <v>14</v>
       </c>
       <c r="G47" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H47" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -2955,10 +2988,10 @@
         <v>14</v>
       </c>
       <c r="G48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H48" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -2975,7 +3008,7 @@
         <v>14</v>
       </c>
       <c r="G49" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H49" t="s">
         <v>28</v>
@@ -2983,7 +3016,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
@@ -3000,7 +3033,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
@@ -3017,10 +3050,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B52" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C52" t="s">
         <v>34</v>
@@ -3032,15 +3065,15 @@
         <v>18</v>
       </c>
       <c r="K52" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B53" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C53" t="s">
         <v>35</v>
@@ -3052,7 +3085,7 @@
         <v>18</v>
       </c>
       <c r="K53" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
@@ -3080,7 +3113,7 @@
         <v>39</v>
       </c>
       <c r="G55" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H55" t="s">
         <v>40</v>
@@ -3123,13 +3156,13 @@
         <v>9</v>
       </c>
       <c r="B61" t="s">
+        <v>562</v>
+      </c>
+      <c r="C61" t="s">
+        <v>582</v>
+      </c>
+      <c r="I61" t="s">
         <v>563</v>
-      </c>
-      <c r="C61" t="s">
-        <v>54</v>
-      </c>
-      <c r="I61" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
@@ -3137,7 +3170,7 @@
         <v>19</v>
       </c>
       <c r="B62" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C62" t="s">
         <v>59</v>
@@ -3146,7 +3179,7 @@
         <v>14</v>
       </c>
       <c r="J62" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
@@ -3154,22 +3187,22 @@
         <v>109</v>
       </c>
       <c r="B63" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C63" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H63" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="J63" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
@@ -3177,22 +3210,22 @@
         <v>109</v>
       </c>
       <c r="B64" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C64" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E64" t="s">
         <v>14</v>
       </c>
       <c r="G64" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H64" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J64" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -3200,21 +3233,21 @@
         <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C65" t="s">
         <v>63</v>
       </c>
       <c r="J65" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B66" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C66" t="s">
         <v>65</v>
@@ -3223,7 +3256,7 @@
         <v>14</v>
       </c>
       <c r="J66" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -3236,13 +3269,13 @@
         <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C68" t="s">
         <v>54</v>
       </c>
       <c r="I68" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -3264,19 +3297,19 @@
         <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C70" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E70" t="s">
         <v>14</v>
       </c>
       <c r="G70" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H70" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -3284,19 +3317,19 @@
         <v>109</v>
       </c>
       <c r="B71" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C71" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E71" t="s">
         <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H71" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -3312,7 +3345,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B73" t="s">
         <v>64</v>
@@ -3400,7 +3433,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B83" t="s">
         <v>74</v>
@@ -3432,12 +3465,12 @@
         <v>14</v>
       </c>
       <c r="I84" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B85" t="s">
         <v>79</v>
@@ -3454,7 +3487,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B86" t="s">
         <v>81</v>
@@ -3480,12 +3513,12 @@
         <v>14</v>
       </c>
       <c r="I87" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B88" t="s">
         <v>85</v>
@@ -3514,7 +3547,7 @@
         <v>14</v>
       </c>
       <c r="G89" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H89" t="s">
         <v>90</v>
@@ -3522,7 +3555,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B90" t="s">
         <v>91</v>
@@ -3548,7 +3581,7 @@
         <v>95</v>
       </c>
       <c r="I91" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -3565,7 +3598,7 @@
         <v>14</v>
       </c>
       <c r="G92" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H92" t="s">
         <v>98</v>
@@ -3585,7 +3618,7 @@
         <v>14</v>
       </c>
       <c r="G93" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H93" t="s">
         <v>101</v>
@@ -3605,7 +3638,7 @@
         <v>14</v>
       </c>
       <c r="G94" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H94" t="s">
         <v>104</v>
@@ -3613,7 +3646,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B95" t="s">
         <v>105</v>
@@ -3639,7 +3672,7 @@
         <v>108</v>
       </c>
       <c r="I96" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -3656,10 +3689,10 @@
         <v>14</v>
       </c>
       <c r="G97" t="s">
+        <v>416</v>
+      </c>
+      <c r="H97" t="s">
         <v>417</v>
-      </c>
-      <c r="H97" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -3704,7 +3737,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B104" t="s">
         <v>117</v>
@@ -3730,12 +3763,12 @@
         <v>120</v>
       </c>
       <c r="I105" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B106" t="s">
         <v>121</v>
@@ -3761,7 +3794,7 @@
         <v>14</v>
       </c>
       <c r="G107" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H107" t="s">
         <v>125</v>
@@ -3789,7 +3822,7 @@
         <v>14</v>
       </c>
       <c r="G109" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H109" t="s">
         <v>128</v>
@@ -3797,7 +3830,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B110" t="s">
         <v>129</v>
@@ -3823,7 +3856,7 @@
         <v>132</v>
       </c>
       <c r="I111" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
@@ -3840,7 +3873,7 @@
         <v>14</v>
       </c>
       <c r="G112" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H112" t="s">
         <v>135</v>
@@ -3860,7 +3893,7 @@
         <v>14</v>
       </c>
       <c r="G113" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H113" t="s">
         <v>138</v>
@@ -3868,7 +3901,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B114" t="s">
         <v>139</v>
@@ -3882,7 +3915,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B115" t="s">
         <v>141</v>
@@ -3908,7 +3941,7 @@
         <v>144</v>
       </c>
       <c r="I116" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -3925,7 +3958,7 @@
         <v>14</v>
       </c>
       <c r="G117" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H117" t="s">
         <v>147</v>
@@ -3959,7 +3992,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B124" t="s">
         <v>150</v>
@@ -3987,7 +4020,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B126" t="s">
         <v>155</v>
@@ -4007,7 +4040,7 @@
         <v>158</v>
       </c>
       <c r="I127" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
@@ -4024,7 +4057,7 @@
         <v>14</v>
       </c>
       <c r="G128" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H128" t="s">
         <v>161</v>
@@ -4046,7 +4079,7 @@
         <v>163</v>
       </c>
       <c r="I130" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
@@ -4063,7 +4096,7 @@
         <v>14</v>
       </c>
       <c r="G131" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H131" t="s">
         <v>166</v>
@@ -4080,7 +4113,7 @@
         <v>168</v>
       </c>
       <c r="I132" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
@@ -4146,7 +4179,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B138" t="s">
         <v>177</v>
@@ -4161,7 +4194,7 @@
         <v>18</v>
       </c>
       <c r="I138" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
@@ -4187,7 +4220,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B143" t="s">
         <v>182</v>
@@ -4215,7 +4248,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B145" t="s">
         <v>186</v>
@@ -4235,7 +4268,7 @@
         <v>189</v>
       </c>
       <c r="I146" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
@@ -4252,7 +4285,7 @@
         <v>14</v>
       </c>
       <c r="G147" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H147" t="s">
         <v>161</v>
@@ -4274,7 +4307,7 @@
         <v>193</v>
       </c>
       <c r="I149" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
@@ -4291,7 +4324,7 @@
         <v>14</v>
       </c>
       <c r="G150" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H150" t="s">
         <v>166</v>
@@ -4299,7 +4332,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B151" t="s">
         <v>195</v>
@@ -4314,7 +4347,7 @@
         <v>18</v>
       </c>
       <c r="I151" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
@@ -4340,7 +4373,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B156" t="s">
         <v>198</v>
@@ -4368,7 +4401,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B158" t="s">
         <v>202</v>
@@ -4394,7 +4427,7 @@
         <v>205</v>
       </c>
       <c r="I159" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
@@ -4411,7 +4444,7 @@
         <v>14</v>
       </c>
       <c r="G160" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H160" t="s">
         <v>161</v>
@@ -4433,7 +4466,7 @@
         <v>209</v>
       </c>
       <c r="I162" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
@@ -4450,7 +4483,7 @@
         <v>14</v>
       </c>
       <c r="G163" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H163" t="s">
         <v>166</v>
@@ -4479,7 +4512,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B168" t="s">
         <v>212</v>
@@ -4507,7 +4540,7 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B170" t="s">
         <v>216</v>
@@ -4533,7 +4566,7 @@
         <v>219</v>
       </c>
       <c r="I171" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
@@ -4550,7 +4583,7 @@
         <v>14</v>
       </c>
       <c r="G172" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H172" t="s">
         <v>161</v>
@@ -4572,7 +4605,7 @@
         <v>223</v>
       </c>
       <c r="I174" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
@@ -4589,7 +4622,7 @@
         <v>14</v>
       </c>
       <c r="G175" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H175" t="s">
         <v>166</v>
@@ -4618,7 +4651,7 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B180" t="s">
         <v>226</v>
@@ -4646,7 +4679,7 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B182" t="s">
         <v>230</v>
@@ -4672,7 +4705,7 @@
         <v>233</v>
       </c>
       <c r="I183" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
@@ -4689,7 +4722,7 @@
         <v>14</v>
       </c>
       <c r="G184" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H184" t="s">
         <v>161</v>
@@ -4711,7 +4744,7 @@
         <v>237</v>
       </c>
       <c r="I186" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
@@ -4728,7 +4761,7 @@
         <v>14</v>
       </c>
       <c r="G187" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H187" t="s">
         <v>166</v>
@@ -4747,7 +4780,7 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B189" t="s">
         <v>241</v>
@@ -4762,7 +4795,7 @@
         <v>18</v>
       </c>
       <c r="I189" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
@@ -4781,12 +4814,12 @@
         <v>244</v>
       </c>
       <c r="I191" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B192" t="s">
         <v>245</v>
@@ -4801,12 +4834,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>19</v>
       </c>
@@ -4817,22 +4850,22 @@
         <v>180</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>9</v>
       </c>
@@ -4843,7 +4876,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>114</v>
       </c>
@@ -4857,15 +4890,15 @@
         <v>14</v>
       </c>
       <c r="G201" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H201" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B202" t="s">
         <v>253</v>
@@ -4880,7 +4913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>109</v>
       </c>
@@ -4894,207 +4927,219 @@
         <v>14</v>
       </c>
       <c r="G203" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H203" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
+        <v>578</v>
+      </c>
+      <c r="B204" t="s">
+        <v>579</v>
+      </c>
+      <c r="C204" t="s">
+        <v>580</v>
+      </c>
+      <c r="E204" t="s">
+        <v>14</v>
+      </c>
+      <c r="F204" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
         <v>109</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B205" t="s">
         <v>258</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C205" t="s">
+        <v>581</v>
+      </c>
+      <c r="E205" t="s">
+        <v>14</v>
+      </c>
+      <c r="G205" t="s">
+        <v>415</v>
+      </c>
+      <c r="H205" t="s">
         <v>259</v>
       </c>
-      <c r="E204" t="s">
-        <v>14</v>
-      </c>
-      <c r="G204" t="s">
-        <v>416</v>
-      </c>
-      <c r="H204" t="s">
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>453</v>
+      </c>
+      <c r="B206" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A205" t="s">
-        <v>454</v>
-      </c>
-      <c r="B205" t="s">
+      <c r="C206" t="s">
         <v>261</v>
       </c>
-      <c r="C205" t="s">
+      <c r="E206" t="s">
+        <v>14</v>
+      </c>
+      <c r="F206" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>109</v>
+      </c>
+      <c r="B207" t="s">
         <v>262</v>
       </c>
-      <c r="E205" t="s">
-        <v>14</v>
-      </c>
-      <c r="F205" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
-        <v>109</v>
-      </c>
-      <c r="B206" t="s">
+      <c r="C207" t="s">
         <v>263</v>
       </c>
-      <c r="C206" t="s">
+      <c r="E207" t="s">
+        <v>14</v>
+      </c>
+      <c r="G207" t="s">
+        <v>415</v>
+      </c>
+      <c r="H207" t="s">
         <v>264</v>
       </c>
-      <c r="E206" t="s">
-        <v>14</v>
-      </c>
-      <c r="G206" t="s">
-        <v>416</v>
-      </c>
-      <c r="H206" t="s">
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>414</v>
+      </c>
+      <c r="B208" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A207" t="s">
-        <v>415</v>
-      </c>
-      <c r="B207" t="s">
-        <v>266</v>
-      </c>
-      <c r="C207" t="s">
+      <c r="C208" t="s">
         <v>92</v>
       </c>
-      <c r="E207" t="s">
-        <v>14</v>
-      </c>
-      <c r="F207" t="s">
+      <c r="E208" t="s">
+        <v>14</v>
+      </c>
+      <c r="F208" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
-        <v>9</v>
-      </c>
-      <c r="B208" t="s">
-        <v>267</v>
-      </c>
-      <c r="C208" t="s">
-        <v>268</v>
-      </c>
-      <c r="I208" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>443</v>
+        <v>9</v>
       </c>
       <c r="B209" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C209" t="s">
-        <v>270</v>
-      </c>
-      <c r="E209" t="s">
-        <v>14</v>
+        <v>267</v>
+      </c>
+      <c r="I209" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>415</v>
+        <v>442</v>
       </c>
       <c r="B210" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C210" t="s">
-        <v>106</v>
+        <v>269</v>
       </c>
       <c r="E210" t="s">
         <v>14</v>
-      </c>
-      <c r="F210" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>152</v>
+        <v>414</v>
       </c>
       <c r="B211" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C211" t="s">
-        <v>273</v>
-      </c>
-      <c r="I211" t="s">
-        <v>485</v>
+        <v>106</v>
+      </c>
+      <c r="E211" t="s">
+        <v>14</v>
+      </c>
+      <c r="F211" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>455</v>
+        <v>152</v>
       </c>
       <c r="B212" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C212" t="s">
-        <v>275</v>
-      </c>
-      <c r="E212" t="s">
-        <v>14</v>
+        <v>272</v>
+      </c>
+      <c r="I212" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>55</v>
+        <v>454</v>
       </c>
       <c r="B213" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C213" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E213" t="s">
         <v>14</v>
-      </c>
-      <c r="G213" t="s">
-        <v>416</v>
-      </c>
-      <c r="H213" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="B214" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C214" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E214" t="s">
         <v>14</v>
       </c>
       <c r="G214" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H214" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>181</v>
+        <v>109</v>
+      </c>
+      <c r="B215" t="s">
+        <v>278</v>
+      </c>
+      <c r="C215" t="s">
+        <v>279</v>
+      </c>
+      <c r="E215" t="s">
+        <v>14</v>
+      </c>
+      <c r="G215" t="s">
+        <v>415</v>
+      </c>
+      <c r="H215" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
@@ -5102,180 +5147,180 @@
         <v>41</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A219" t="s">
-        <v>9</v>
-      </c>
-      <c r="B219" t="s">
-        <v>282</v>
-      </c>
-      <c r="C219" t="s">
-        <v>283</v>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>415</v>
+        <v>9</v>
       </c>
       <c r="B220" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C220" t="s">
-        <v>285</v>
-      </c>
-      <c r="E220" t="s">
-        <v>14</v>
-      </c>
-      <c r="F220" t="s">
-        <v>87</v>
+        <v>282</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B221" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C221" t="s">
-        <v>92</v>
+        <v>284</v>
       </c>
       <c r="E221" t="s">
         <v>14</v>
       </c>
       <c r="F221" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>9</v>
+        <v>414</v>
       </c>
       <c r="B222" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C222" t="s">
-        <v>288</v>
-      </c>
-      <c r="I222" t="s">
-        <v>486</v>
+        <v>92</v>
+      </c>
+      <c r="E222" t="s">
+        <v>14</v>
+      </c>
+      <c r="F222" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="B223" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C223" t="s">
-        <v>290</v>
-      </c>
-      <c r="E223" t="s">
-        <v>14</v>
-      </c>
-      <c r="G223" t="s">
-        <v>416</v>
-      </c>
-      <c r="H223" t="s">
-        <v>291</v>
+        <v>287</v>
+      </c>
+      <c r="I223" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
+        <v>109</v>
+      </c>
+      <c r="B224" t="s">
+        <v>288</v>
+      </c>
+      <c r="C224" t="s">
+        <v>289</v>
+      </c>
+      <c r="E224" t="s">
+        <v>14</v>
+      </c>
+      <c r="G224" t="s">
         <v>415</v>
       </c>
-      <c r="B224" t="s">
-        <v>292</v>
-      </c>
-      <c r="C224" t="s">
-        <v>106</v>
-      </c>
-      <c r="E224" t="s">
-        <v>14</v>
-      </c>
-      <c r="F224" t="s">
-        <v>93</v>
+      <c r="H224" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>9</v>
+        <v>414</v>
       </c>
       <c r="B225" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C225" t="s">
-        <v>294</v>
-      </c>
-      <c r="I225" t="s">
-        <v>487</v>
+        <v>106</v>
+      </c>
+      <c r="E225" t="s">
+        <v>14</v>
+      </c>
+      <c r="F225" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="B226" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C226" t="s">
-        <v>296</v>
-      </c>
-      <c r="E226" t="s">
-        <v>14</v>
-      </c>
-      <c r="G226" t="s">
-        <v>508</v>
-      </c>
-      <c r="H226" t="s">
-        <v>297</v>
+        <v>293</v>
+      </c>
+      <c r="I226" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="B227" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C227" t="s">
-        <v>299</v>
+        <v>295</v>
+      </c>
+      <c r="E227" t="s">
+        <v>14</v>
+      </c>
+      <c r="G227" t="s">
+        <v>507</v>
+      </c>
+      <c r="H227" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="B228" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C228" t="s">
-        <v>301</v>
-      </c>
-      <c r="E228" t="s">
-        <v>14</v>
+        <v>298</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="B229" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C229" t="s">
-        <v>303</v>
+        <v>300</v>
+      </c>
+      <c r="E229" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>181</v>
+        <v>19</v>
+      </c>
+      <c r="B230" t="s">
+        <v>301</v>
+      </c>
+      <c r="C230" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
@@ -5285,6 +5330,11 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5296,11 +5346,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5310,277 +5360,277 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E1" t="s">
         <v>456</v>
-      </c>
-      <c r="E1" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B3" t="s">
         <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C4" t="s">
         <v>309</v>
-      </c>
-      <c r="C4" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" t="s">
         <v>311</v>
-      </c>
-      <c r="C5" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B7" t="s">
         <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B8" t="s">
+        <v>316</v>
+      </c>
+      <c r="C8" t="s">
         <v>317</v>
-      </c>
-      <c r="C8" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" t="s">
         <v>319</v>
-      </c>
-      <c r="C9" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B10" t="s">
         <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B11" t="s">
         <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B16" t="s">
         <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B21" t="s">
         <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C23" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -5591,354 +5641,354 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B26" t="s">
         <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B28" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C28" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C29" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B31" t="s">
         <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C33" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B34" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B35" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C36" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B37" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C37" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B39" t="s">
         <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B41" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C41" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B42" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C42" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B43" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C43" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B44" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C44" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B45" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C45" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B47" t="s">
         <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B49" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C49" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B50" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C50" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C53" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B55" t="s">
         <v>76</v>
       </c>
       <c r="C55" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B56" t="s">
         <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D57" t="s">
         <v>33</v>
@@ -5946,7 +5996,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -5963,365 +6013,398 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B60" t="s">
         <v>76</v>
       </c>
       <c r="C60" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B61" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B62" t="s">
         <v>76</v>
       </c>
       <c r="C62" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B63" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C63" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
       </c>
       <c r="C64" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B65" t="s">
         <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B66" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C66" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B67" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C67" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B68" t="s">
+        <v>325</v>
+      </c>
+      <c r="C68" t="s">
         <v>326</v>
-      </c>
-      <c r="C68" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B69" t="s">
+        <v>327</v>
+      </c>
+      <c r="C69" t="s">
         <v>328</v>
-      </c>
-      <c r="C69" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B70" t="s">
+        <v>329</v>
+      </c>
+      <c r="C70" t="s">
         <v>330</v>
-      </c>
-      <c r="C70" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B71" t="s">
+        <v>331</v>
+      </c>
+      <c r="C71" t="s">
         <v>332</v>
-      </c>
-      <c r="C71" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B72" t="s">
+        <v>333</v>
+      </c>
+      <c r="C72" t="s">
         <v>334</v>
-      </c>
-      <c r="C72" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B73" t="s">
+        <v>335</v>
+      </c>
+      <c r="C73" t="s">
         <v>336</v>
-      </c>
-      <c r="C73" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B74" t="s">
+        <v>337</v>
+      </c>
+      <c r="C74" t="s">
         <v>338</v>
-      </c>
-      <c r="C74" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B76" t="s">
         <v>76</v>
       </c>
       <c r="C76" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B77" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C77" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B78" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C78" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B80" t="s">
         <v>76</v>
       </c>
       <c r="C80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B82" t="s">
         <v>76</v>
       </c>
       <c r="C82" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B83" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C83" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B84" t="s">
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B86" t="s">
+        <v>374</v>
+      </c>
+      <c r="C86" t="s">
         <v>375</v>
-      </c>
-      <c r="C86" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B87" t="s">
+        <v>376</v>
+      </c>
+      <c r="C87" t="s">
         <v>377</v>
-      </c>
-      <c r="C87" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B88" t="s">
+        <v>378</v>
+      </c>
+      <c r="C88" t="s">
         <v>379</v>
-      </c>
-      <c r="C88" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B89" t="s">
+        <v>380</v>
+      </c>
+      <c r="C89" t="s">
         <v>381</v>
-      </c>
-      <c r="C89" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>441</v>
+        <v>577</v>
       </c>
       <c r="B90" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="C90" t="s">
-        <v>442</v>
+        <v>576</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>524</v>
+        <v>577</v>
       </c>
       <c r="B91" t="s">
+        <v>572</v>
+      </c>
+      <c r="C91" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>577</v>
+      </c>
+      <c r="B92" t="s">
+        <v>573</v>
+      </c>
+      <c r="C92" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>440</v>
+      </c>
+      <c r="B93" t="s">
         <v>18</v>
       </c>
-      <c r="C91" t="s">
-        <v>442</v>
+      <c r="C93" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>523</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -6339,7 +6422,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -6353,7 +6436,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6363,30 +6446,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B1" t="s">
         <v>383</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>384</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>385</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>386</v>
       </c>
-      <c r="E1" t="s">
-        <v>387</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -6395,10 +6478,10 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F2" s="1">
-        <v>201807</v>
+        <v>20180829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the messages with days from planting and harvest date in odk
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$234</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$236</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="588">
   <si>
     <t>type</t>
   </si>
@@ -1774,6 +1774,21 @@
   </si>
   <si>
     <t>Finca en la base de datos</t>
+  </si>
+  <si>
+    <t>harvest_days</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>harvest_days_note</t>
+  </si>
+  <si>
+    <t>decimal-date-time(${harvest_date}) - decimal-date-time(${planting_date})</t>
+  </si>
+  <si>
+    <t>Días desde siembra ${harvest_days}</t>
   </si>
 </sst>
 </file>
@@ -2179,11 +2194,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L234"/>
+  <dimension ref="A1:L236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C204" sqref="C204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4834,12 +4849,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>19</v>
       </c>
@@ -4850,22 +4865,22 @@
         <v>180</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>9</v>
       </c>
@@ -4876,7 +4891,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>114</v>
       </c>
@@ -4896,69 +4911,54 @@
         <v>252</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
+        <v>525</v>
+      </c>
+      <c r="B202" t="s">
+        <v>583</v>
+      </c>
+      <c r="J202" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>584</v>
+      </c>
+      <c r="B203" t="s">
+        <v>585</v>
+      </c>
+      <c r="C203" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
         <v>438</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B204" t="s">
         <v>253</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C204" t="s">
         <v>254</v>
       </c>
-      <c r="E202" t="s">
-        <v>14</v>
-      </c>
-      <c r="F202" t="s">
+      <c r="E204" t="s">
+        <v>14</v>
+      </c>
+      <c r="F204" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A203" t="s">
-        <v>109</v>
-      </c>
-      <c r="B203" t="s">
-        <v>255</v>
-      </c>
-      <c r="C203" t="s">
-        <v>256</v>
-      </c>
-      <c r="E203" t="s">
-        <v>14</v>
-      </c>
-      <c r="G203" t="s">
-        <v>415</v>
-      </c>
-      <c r="H203" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
-        <v>578</v>
-      </c>
-      <c r="B204" t="s">
-        <v>579</v>
-      </c>
-      <c r="C204" t="s">
-        <v>580</v>
-      </c>
-      <c r="E204" t="s">
-        <v>14</v>
-      </c>
-      <c r="F204" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>109</v>
       </c>
       <c r="B205" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C205" t="s">
-        <v>581</v>
+        <v>256</v>
       </c>
       <c r="E205" t="s">
         <v>14</v>
@@ -4967,35 +4967,35 @@
         <v>415</v>
       </c>
       <c r="H205" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>453</v>
+        <v>578</v>
       </c>
       <c r="B206" t="s">
-        <v>260</v>
+        <v>579</v>
       </c>
       <c r="C206" t="s">
-        <v>261</v>
+        <v>580</v>
       </c>
       <c r="E206" t="s">
         <v>14</v>
       </c>
       <c r="F206" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>109</v>
       </c>
       <c r="B207" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C207" t="s">
-        <v>263</v>
+        <v>581</v>
       </c>
       <c r="E207" t="s">
         <v>14</v>
@@ -5004,337 +5004,374 @@
         <v>415</v>
       </c>
       <c r="H207" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>414</v>
+        <v>453</v>
       </c>
       <c r="B208" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C208" t="s">
-        <v>92</v>
+        <v>261</v>
       </c>
       <c r="E208" t="s">
         <v>14</v>
       </c>
       <c r="F208" t="s">
-        <v>93</v>
+        <v>374</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B209" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C209" t="s">
-        <v>267</v>
-      </c>
-      <c r="I209" t="s">
-        <v>483</v>
+        <v>263</v>
+      </c>
+      <c r="E209" t="s">
+        <v>14</v>
+      </c>
+      <c r="G209" t="s">
+        <v>415</v>
+      </c>
+      <c r="H209" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>442</v>
+        <v>414</v>
       </c>
       <c r="B210" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C210" t="s">
-        <v>269</v>
+        <v>92</v>
       </c>
       <c r="E210" t="s">
         <v>14</v>
+      </c>
+      <c r="F210" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>414</v>
+        <v>9</v>
       </c>
       <c r="B211" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C211" t="s">
-        <v>106</v>
-      </c>
-      <c r="E211" t="s">
-        <v>14</v>
-      </c>
-      <c r="F211" t="s">
-        <v>93</v>
+        <v>267</v>
+      </c>
+      <c r="I211" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>152</v>
+        <v>442</v>
       </c>
       <c r="B212" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C212" t="s">
-        <v>272</v>
-      </c>
-      <c r="I212" t="s">
-        <v>484</v>
+        <v>269</v>
+      </c>
+      <c r="E212" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>454</v>
+        <v>414</v>
       </c>
       <c r="B213" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C213" t="s">
-        <v>274</v>
+        <v>106</v>
       </c>
       <c r="E213" t="s">
         <v>14</v>
+      </c>
+      <c r="F213" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="B214" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C214" t="s">
-        <v>276</v>
-      </c>
-      <c r="E214" t="s">
-        <v>14</v>
-      </c>
-      <c r="G214" t="s">
-        <v>415</v>
-      </c>
-      <c r="H214" t="s">
-        <v>277</v>
+        <v>272</v>
+      </c>
+      <c r="I214" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>109</v>
+        <v>454</v>
       </c>
       <c r="B215" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C215" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E215" t="s">
         <v>14</v>
-      </c>
-      <c r="G215" t="s">
-        <v>415</v>
-      </c>
-      <c r="H215" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>181</v>
+        <v>55</v>
+      </c>
+      <c r="B216" t="s">
+        <v>275</v>
+      </c>
+      <c r="C216" t="s">
+        <v>276</v>
+      </c>
+      <c r="E216" t="s">
+        <v>14</v>
+      </c>
+      <c r="G216" t="s">
+        <v>415</v>
+      </c>
+      <c r="H216" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>41</v>
+        <v>109</v>
+      </c>
+      <c r="B217" t="s">
+        <v>278</v>
+      </c>
+      <c r="C217" t="s">
+        <v>279</v>
+      </c>
+      <c r="E217" t="s">
+        <v>14</v>
+      </c>
+      <c r="G217" t="s">
+        <v>415</v>
+      </c>
+      <c r="H217" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>9</v>
-      </c>
-      <c r="B220" t="s">
-        <v>281</v>
-      </c>
-      <c r="C220" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A221" t="s">
-        <v>414</v>
-      </c>
-      <c r="B221" t="s">
-        <v>283</v>
-      </c>
-      <c r="C221" t="s">
-        <v>284</v>
-      </c>
-      <c r="E221" t="s">
-        <v>14</v>
-      </c>
-      <c r="F221" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>414</v>
+        <v>9</v>
       </c>
       <c r="B222" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C222" t="s">
-        <v>92</v>
-      </c>
-      <c r="E222" t="s">
-        <v>14</v>
-      </c>
-      <c r="F222" t="s">
-        <v>93</v>
+        <v>282</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>9</v>
+        <v>414</v>
       </c>
       <c r="B223" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C223" t="s">
-        <v>287</v>
-      </c>
-      <c r="I223" t="s">
-        <v>485</v>
+        <v>284</v>
+      </c>
+      <c r="E223" t="s">
+        <v>14</v>
+      </c>
+      <c r="F223" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>109</v>
+        <v>414</v>
       </c>
       <c r="B224" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C224" t="s">
-        <v>289</v>
+        <v>92</v>
       </c>
       <c r="E224" t="s">
         <v>14</v>
       </c>
-      <c r="G224" t="s">
-        <v>415</v>
-      </c>
-      <c r="H224" t="s">
-        <v>290</v>
+      <c r="F224" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>414</v>
+        <v>9</v>
       </c>
       <c r="B225" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C225" t="s">
-        <v>106</v>
-      </c>
-      <c r="E225" t="s">
-        <v>14</v>
-      </c>
-      <c r="F225" t="s">
-        <v>93</v>
+        <v>287</v>
+      </c>
+      <c r="I225" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B226" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C226" t="s">
-        <v>293</v>
-      </c>
-      <c r="I226" t="s">
-        <v>486</v>
+        <v>289</v>
+      </c>
+      <c r="E226" t="s">
+        <v>14</v>
+      </c>
+      <c r="G226" t="s">
+        <v>415</v>
+      </c>
+      <c r="H226" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>114</v>
+        <v>414</v>
       </c>
       <c r="B227" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C227" t="s">
-        <v>295</v>
+        <v>106</v>
       </c>
       <c r="E227" t="s">
         <v>14</v>
       </c>
-      <c r="G227" t="s">
-        <v>507</v>
-      </c>
-      <c r="H227" t="s">
-        <v>296</v>
+      <c r="F227" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="B228" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C228" t="s">
-        <v>298</v>
+        <v>293</v>
+      </c>
+      <c r="I228" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B229" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C229" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E229" t="s">
         <v>14</v>
+      </c>
+      <c r="G229" t="s">
+        <v>507</v>
+      </c>
+      <c r="H229" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="B230" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C230" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>181</v>
+        <v>109</v>
+      </c>
+      <c r="B231" t="s">
+        <v>299</v>
+      </c>
+      <c r="C231" t="s">
+        <v>300</v>
+      </c>
+      <c r="E231" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>41</v>
+        <v>19</v>
+      </c>
+      <c r="B232" t="s">
+        <v>301</v>
+      </c>
+      <c r="C232" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solved iss40. The new section was moved to phytosanitary section
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$251</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$L$246</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7838" uniqueCount="3081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7804" uniqueCount="3069">
   <si>
     <t>type</t>
   </si>
@@ -9207,45 +9207,12 @@
     <t>Agua</t>
   </si>
   <si>
-    <t>agronomy_practice_weeds_type</t>
-  </si>
-  <si>
-    <t>agronomy_practice_weeds</t>
-  </si>
-  <si>
     <t>Tipo de manejo de malezas</t>
   </si>
   <si>
-    <t>Tipo de información de manejo de malezas</t>
-  </si>
-  <si>
     <t>weeds_type</t>
   </si>
   <si>
-    <t>agronomy_practice_weeds_intermediate</t>
-  </si>
-  <si>
-    <t>weeds_type_count_intermediate</t>
-  </si>
-  <si>
-    <t>agronomy_practice_weeds_advanced</t>
-  </si>
-  <si>
-    <t>weeds_date_advanced</t>
-  </si>
-  <si>
-    <t>weeds_notes_advanced</t>
-  </si>
-  <si>
-    <t>Información avanzada de manejo de malezas</t>
-  </si>
-  <si>
-    <t>Cantidad de veces que realizó este tipo de manejo de malezas</t>
-  </si>
-  <si>
-    <t>Información intermedia de manejo de malezas</t>
-  </si>
-  <si>
     <t>select_one choices_agronomy_practices_weeds_type</t>
   </si>
   <si>
@@ -9264,10 +9231,7 @@
     <t>Se presentó arroz rojo en su lote?</t>
   </si>
   <si>
-    <t>(selected(${agronomy_practice_weeds_type},'2'))</t>
-  </si>
-  <si>
-    <t>(selected(${agronomy_practice_weeds_type},'3'))</t>
+    <t>select_one choices_agronomy_practices_phytosanitary_type</t>
   </si>
 </sst>
 </file>
@@ -9674,11 +9638,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L250"/>
+  <dimension ref="A1:L245"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I188" sqref="I188"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12163,10 +12127,10 @@
         <v>391</v>
       </c>
       <c r="B181" t="s">
-        <v>3060</v>
+        <v>213</v>
       </c>
       <c r="C181" t="s">
-        <v>3063</v>
+        <v>214</v>
       </c>
       <c r="E181" t="s">
         <v>14</v>
@@ -12180,21 +12144,21 @@
         <v>146</v>
       </c>
       <c r="B182" t="s">
-        <v>3061</v>
+        <v>215</v>
       </c>
       <c r="C182" t="s">
-        <v>331</v>
+        <v>216</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>3073</v>
+        <v>3068</v>
       </c>
       <c r="B183" t="s">
-        <v>3064</v>
+        <v>217</v>
       </c>
       <c r="C183" t="s">
-        <v>3062</v>
+        <v>218</v>
       </c>
       <c r="E183" t="s">
         <v>14</v>
@@ -12208,13 +12172,13 @@
         <v>9</v>
       </c>
       <c r="B184" t="s">
-        <v>3065</v>
+        <v>219</v>
       </c>
       <c r="C184" t="s">
-        <v>3072</v>
+        <v>220</v>
       </c>
       <c r="I184" t="s">
-        <v>3079</v>
+        <v>447</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
@@ -12222,10 +12186,10 @@
         <v>53</v>
       </c>
       <c r="B185" t="s">
-        <v>3066</v>
+        <v>221</v>
       </c>
       <c r="C185" t="s">
-        <v>3071</v>
+        <v>222</v>
       </c>
       <c r="E185" t="s">
         <v>14</v>
@@ -12247,13 +12211,13 @@
         <v>9</v>
       </c>
       <c r="B187" t="s">
-        <v>3067</v>
+        <v>223</v>
       </c>
       <c r="C187" t="s">
-        <v>3070</v>
+        <v>224</v>
       </c>
       <c r="I187" t="s">
-        <v>3080</v>
+        <v>448</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
@@ -12261,7 +12225,7 @@
         <v>112</v>
       </c>
       <c r="B188" t="s">
-        <v>3068</v>
+        <v>225</v>
       </c>
       <c r="C188" t="s">
         <v>159</v>
@@ -12278,30 +12242,33 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B189" t="s">
-        <v>3069</v>
+        <v>226</v>
       </c>
       <c r="C189" t="s">
-        <v>174</v>
+        <v>227</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>385</v>
+        <v>421</v>
       </c>
       <c r="B190" t="s">
-        <v>3077</v>
+        <v>228</v>
       </c>
       <c r="C190" t="s">
-        <v>3078</v>
+        <v>229</v>
       </c>
       <c r="E190" t="s">
         <v>14</v>
       </c>
       <c r="F190" t="s">
-        <v>91</v>
+        <v>18</v>
+      </c>
+      <c r="I190" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
@@ -12311,18 +12278,44 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="B192" t="s">
+        <v>230</v>
+      </c>
+      <c r="C192" t="s">
+        <v>231</v>
+      </c>
+      <c r="I192" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>3062</v>
+      </c>
+      <c r="B193" t="s">
+        <v>3061</v>
+      </c>
+      <c r="C193" t="s">
+        <v>3060</v>
+      </c>
+      <c r="E193" t="s">
+        <v>14</v>
+      </c>
+      <c r="F193" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>391</v>
+        <v>406</v>
       </c>
       <c r="B194" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C194" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="E194" t="s">
         <v>14</v>
@@ -12331,571 +12324,502 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>146</v>
+        <v>385</v>
       </c>
       <c r="B195" t="s">
-        <v>215</v>
+        <v>3066</v>
       </c>
       <c r="C195" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3067</v>
+      </c>
+      <c r="E195" t="s">
+        <v>14</v>
+      </c>
+      <c r="F195" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>402</v>
-      </c>
-      <c r="B196" t="s">
-        <v>217</v>
-      </c>
-      <c r="C196" t="s">
-        <v>218</v>
-      </c>
-      <c r="E196" t="s">
-        <v>14</v>
-      </c>
-      <c r="F196" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
-        <v>9</v>
-      </c>
-      <c r="B197" t="s">
-        <v>219</v>
-      </c>
-      <c r="C197" t="s">
-        <v>220</v>
-      </c>
-      <c r="I197" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
-        <v>53</v>
-      </c>
-      <c r="B198" t="s">
-        <v>221</v>
-      </c>
-      <c r="C198" t="s">
-        <v>222</v>
-      </c>
-      <c r="E198" t="s">
-        <v>14</v>
-      </c>
-      <c r="G198" t="s">
-        <v>386</v>
-      </c>
-      <c r="H198" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
-        <v>9</v>
-      </c>
-      <c r="B200" t="s">
-        <v>223</v>
-      </c>
-      <c r="C200" t="s">
-        <v>224</v>
-      </c>
-      <c r="I200" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
-        <v>112</v>
-      </c>
-      <c r="B201" t="s">
-        <v>225</v>
-      </c>
-      <c r="C201" t="s">
-        <v>159</v>
-      </c>
-      <c r="E201" t="s">
-        <v>14</v>
-      </c>
-      <c r="G201" t="s">
-        <v>473</v>
-      </c>
-      <c r="H201" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
-        <v>9</v>
-      </c>
-      <c r="B202" t="s">
-        <v>226</v>
-      </c>
-      <c r="C202" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>421</v>
+        <v>19</v>
       </c>
       <c r="B203" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C203" t="s">
-        <v>229</v>
-      </c>
-      <c r="E203" t="s">
-        <v>14</v>
-      </c>
-      <c r="F203" t="s">
-        <v>18</v>
-      </c>
-      <c r="I203" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>9</v>
-      </c>
-      <c r="B205" t="s">
-        <v>230</v>
-      </c>
-      <c r="C205" t="s">
-        <v>231</v>
-      </c>
-      <c r="I205" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
-        <v>406</v>
-      </c>
-      <c r="B206" t="s">
-        <v>232</v>
-      </c>
-      <c r="C206" t="s">
-        <v>233</v>
-      </c>
-      <c r="E206" t="s">
-        <v>14</v>
-      </c>
-      <c r="F206" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
-        <v>19</v>
-      </c>
-      <c r="B208" t="s">
-        <v>234</v>
-      </c>
-      <c r="C208" t="s">
-        <v>174</v>
-      </c>
-    </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>39</v>
+        <v>9</v>
+      </c>
+      <c r="B209" t="s">
+        <v>235</v>
+      </c>
+      <c r="C209" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>175</v>
+        <v>112</v>
+      </c>
+      <c r="B210" t="s">
+        <v>237</v>
+      </c>
+      <c r="C210" t="s">
+        <v>238</v>
+      </c>
+      <c r="E210" t="s">
+        <v>14</v>
+      </c>
+      <c r="G210" t="s">
+        <v>473</v>
+      </c>
+      <c r="H210" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>491</v>
+      </c>
+      <c r="B211" t="s">
+        <v>549</v>
+      </c>
+      <c r="J211" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>39</v>
+        <v>550</v>
+      </c>
+      <c r="B212" t="s">
+        <v>551</v>
+      </c>
+      <c r="C212" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>408</v>
+      </c>
+      <c r="B213" t="s">
+        <v>240</v>
+      </c>
+      <c r="C213" t="s">
+        <v>241</v>
+      </c>
+      <c r="E213" t="s">
+        <v>14</v>
+      </c>
+      <c r="F213" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="B214" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C214" t="s">
-        <v>236</v>
+        <v>243</v>
+      </c>
+      <c r="E214" t="s">
+        <v>14</v>
+      </c>
+      <c r="G214" t="s">
+        <v>386</v>
+      </c>
+      <c r="H214" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>112</v>
+        <v>544</v>
       </c>
       <c r="B215" t="s">
-        <v>237</v>
+        <v>545</v>
       </c>
       <c r="C215" t="s">
-        <v>238</v>
+        <v>546</v>
       </c>
       <c r="E215" t="s">
         <v>14</v>
       </c>
-      <c r="G215" t="s">
-        <v>473</v>
-      </c>
-      <c r="H215" t="s">
-        <v>239</v>
+      <c r="F215" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>491</v>
+        <v>107</v>
       </c>
       <c r="B216" t="s">
-        <v>549</v>
-      </c>
-      <c r="J216" t="s">
-        <v>552</v>
+        <v>245</v>
+      </c>
+      <c r="C216" t="s">
+        <v>547</v>
+      </c>
+      <c r="E216" t="s">
+        <v>14</v>
+      </c>
+      <c r="G216" t="s">
+        <v>386</v>
+      </c>
+      <c r="H216" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>550</v>
+        <v>422</v>
       </c>
       <c r="B217" t="s">
-        <v>551</v>
+        <v>247</v>
       </c>
       <c r="C217" t="s">
-        <v>553</v>
+        <v>248</v>
+      </c>
+      <c r="E217" t="s">
+        <v>14</v>
+      </c>
+      <c r="F217" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>408</v>
+        <v>107</v>
       </c>
       <c r="B218" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="C218" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="E218" t="s">
         <v>14</v>
       </c>
-      <c r="F218" t="s">
-        <v>18</v>
+      <c r="G218" t="s">
+        <v>386</v>
+      </c>
+      <c r="H218" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>107</v>
+        <v>385</v>
       </c>
       <c r="B219" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="C219" t="s">
-        <v>243</v>
+        <v>90</v>
       </c>
       <c r="E219" t="s">
         <v>14</v>
       </c>
-      <c r="G219" t="s">
-        <v>386</v>
-      </c>
-      <c r="H219" t="s">
-        <v>244</v>
+      <c r="F219" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>544</v>
+        <v>9</v>
       </c>
       <c r="B220" t="s">
-        <v>545</v>
+        <v>253</v>
       </c>
       <c r="C220" t="s">
-        <v>546</v>
-      </c>
-      <c r="E220" t="s">
-        <v>14</v>
-      </c>
-      <c r="F220" t="s">
-        <v>537</v>
+        <v>254</v>
+      </c>
+      <c r="I220" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>107</v>
+        <v>412</v>
       </c>
       <c r="B221" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="C221" t="s">
-        <v>547</v>
+        <v>256</v>
       </c>
       <c r="E221" t="s">
         <v>14</v>
       </c>
-      <c r="G221" t="s">
-        <v>386</v>
-      </c>
-      <c r="H221" t="s">
-        <v>246</v>
-      </c>
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>422</v>
+        <v>385</v>
       </c>
       <c r="B222" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="C222" t="s">
-        <v>248</v>
+        <v>104</v>
       </c>
       <c r="E222" t="s">
         <v>14</v>
       </c>
       <c r="F222" t="s">
-        <v>345</v>
+        <v>91</v>
       </c>
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="B223" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="C223" t="s">
-        <v>250</v>
-      </c>
-      <c r="E223" t="s">
-        <v>14</v>
-      </c>
-      <c r="G223" t="s">
-        <v>386</v>
-      </c>
-      <c r="H223" t="s">
-        <v>251</v>
+        <v>259</v>
+      </c>
+      <c r="I223" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>385</v>
+        <v>423</v>
       </c>
       <c r="B224" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C224" t="s">
-        <v>90</v>
+        <v>261</v>
       </c>
       <c r="E224" t="s">
         <v>14</v>
       </c>
-      <c r="F224" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B225" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="C225" t="s">
-        <v>254</v>
-      </c>
-      <c r="I225" t="s">
-        <v>451</v>
+        <v>263</v>
+      </c>
+      <c r="E225" t="s">
+        <v>14</v>
+      </c>
+      <c r="G225" t="s">
+        <v>386</v>
+      </c>
+      <c r="H225" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>412</v>
+        <v>107</v>
       </c>
       <c r="B226" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C226" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="E226" t="s">
         <v>14</v>
       </c>
+      <c r="G226" t="s">
+        <v>386</v>
+      </c>
+      <c r="H226" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>385</v>
-      </c>
-      <c r="B227" t="s">
-        <v>257</v>
-      </c>
-      <c r="C227" t="s">
-        <v>104</v>
-      </c>
-      <c r="E227" t="s">
-        <v>14</v>
-      </c>
-      <c r="F227" t="s">
-        <v>91</v>
+        <v>175</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>146</v>
-      </c>
-      <c r="B228" t="s">
-        <v>258</v>
-      </c>
-      <c r="C228" t="s">
-        <v>259</v>
-      </c>
-      <c r="I228" t="s">
-        <v>452</v>
+        <v>39</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>423</v>
-      </c>
-      <c r="B229" t="s">
-        <v>260</v>
-      </c>
-      <c r="C229" t="s">
-        <v>261</v>
-      </c>
-      <c r="E229" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A230" t="s">
-        <v>53</v>
-      </c>
-      <c r="B230" t="s">
-        <v>262</v>
-      </c>
-      <c r="C230" t="s">
-        <v>263</v>
-      </c>
-      <c r="E230" t="s">
-        <v>14</v>
-      </c>
-      <c r="G230" t="s">
-        <v>386</v>
-      </c>
-      <c r="H230" t="s">
-        <v>264</v>
+        <v>39</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="B231" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C231" t="s">
-        <v>266</v>
-      </c>
-      <c r="E231" t="s">
-        <v>14</v>
-      </c>
-      <c r="G231" t="s">
-        <v>386</v>
-      </c>
-      <c r="H231" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>175</v>
+        <v>385</v>
+      </c>
+      <c r="B232" t="s">
+        <v>270</v>
+      </c>
+      <c r="C232" t="s">
+        <v>271</v>
+      </c>
+      <c r="E232" t="s">
+        <v>14</v>
+      </c>
+      <c r="F232" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>39</v>
+        <v>385</v>
+      </c>
+      <c r="B233" t="s">
+        <v>272</v>
+      </c>
+      <c r="C233" t="s">
+        <v>90</v>
+      </c>
+      <c r="E233" t="s">
+        <v>14</v>
+      </c>
+      <c r="F233" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>39</v>
+        <v>9</v>
+      </c>
+      <c r="B234" t="s">
+        <v>273</v>
+      </c>
+      <c r="C234" t="s">
+        <v>274</v>
+      </c>
+      <c r="I234" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>107</v>
+      </c>
+      <c r="B235" t="s">
+        <v>275</v>
+      </c>
+      <c r="C235" t="s">
+        <v>276</v>
+      </c>
+      <c r="E235" t="s">
+        <v>14</v>
+      </c>
+      <c r="G235" t="s">
+        <v>386</v>
+      </c>
+      <c r="H235" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>9</v>
+        <v>385</v>
       </c>
       <c r="B236" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="C236" t="s">
-        <v>269</v>
+        <v>104</v>
+      </c>
+      <c r="E236" t="s">
+        <v>14</v>
+      </c>
+      <c r="F236" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>385</v>
+        <v>9</v>
       </c>
       <c r="B237" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="C237" t="s">
-        <v>271</v>
-      </c>
-      <c r="E237" t="s">
-        <v>14</v>
-      </c>
-      <c r="F237" t="s">
-        <v>85</v>
+        <v>280</v>
+      </c>
+      <c r="I237" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>385</v>
+        <v>112</v>
       </c>
       <c r="B238" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="C238" t="s">
-        <v>90</v>
+        <v>282</v>
       </c>
       <c r="E238" t="s">
         <v>14</v>
       </c>
-      <c r="F238" t="s">
-        <v>91</v>
+      <c r="G238" t="s">
+        <v>475</v>
+      </c>
+      <c r="H238" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="B239" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C239" t="s">
-        <v>274</v>
-      </c>
-      <c r="I239" t="s">
-        <v>453</v>
+        <v>285</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
@@ -12903,125 +12827,43 @@
         <v>107</v>
       </c>
       <c r="B240" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="C240" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="E240" t="s">
         <v>14</v>
       </c>
-      <c r="G240" t="s">
-        <v>386</v>
-      </c>
-      <c r="H240" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>385</v>
+        <v>19</v>
       </c>
       <c r="B241" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="C241" t="s">
-        <v>104</v>
-      </c>
-      <c r="E241" t="s">
-        <v>14</v>
-      </c>
-      <c r="F241" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>9</v>
-      </c>
-      <c r="B242" t="s">
-        <v>279</v>
-      </c>
-      <c r="C242" t="s">
-        <v>280</v>
-      </c>
-      <c r="I242" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>112</v>
-      </c>
-      <c r="B243" t="s">
-        <v>281</v>
-      </c>
-      <c r="C243" t="s">
-        <v>282</v>
-      </c>
-      <c r="E243" t="s">
-        <v>14</v>
-      </c>
-      <c r="G243" t="s">
-        <v>475</v>
-      </c>
-      <c r="H243" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>146</v>
-      </c>
-      <c r="B244" t="s">
-        <v>284</v>
-      </c>
-      <c r="C244" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>107</v>
-      </c>
-      <c r="B245" t="s">
-        <v>286</v>
-      </c>
-      <c r="C245" t="s">
-        <v>287</v>
-      </c>
-      <c r="E245" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A246" t="s">
-        <v>19</v>
-      </c>
-      <c r="B246" t="s">
-        <v>288</v>
-      </c>
-      <c r="C246" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A248" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A250" t="s">
         <v>39</v>
       </c>
     </row>
@@ -13036,8 +12878,8 @@
   <dimension ref="A1:E1430"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13746,7 +13588,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>3074</v>
+        <v>3063</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
@@ -13757,24 +13599,24 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>3074</v>
+        <v>3063</v>
       </c>
       <c r="B65" t="s">
         <v>74</v>
       </c>
       <c r="C65" t="s">
-        <v>3075</v>
+        <v>3064</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>3074</v>
+        <v>3063</v>
       </c>
       <c r="B66" t="s">
         <v>300</v>
       </c>
       <c r="C66" t="s">
-        <v>3076</v>
+        <v>3065</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed form to collect data on field about rice
</commit_message>
<xml_diff>
--- a/odk/aeps_production_event.xlsx
+++ b/odk/aeps_production_event.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$M$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$M$168</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9173" uniqueCount="3202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9178" uniqueCount="3203">
   <si>
     <t>type</t>
   </si>
@@ -9630,6 +9630,9 @@
   </si>
   <si>
     <t>La fecha de actividad debe ser inferior a la fecha de siembra or mayor a la fecha de cosecha</t>
+  </si>
+  <si>
+    <t>plot_general</t>
   </si>
 </sst>
 </file>
@@ -10037,11 +10040,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M167"/>
+  <dimension ref="A1:M169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68:D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11242,230 +11245,203 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>2839</v>
+        <v>3202</v>
       </c>
       <c r="C68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D68" t="s">
-        <v>2738</v>
-      </c>
-      <c r="F68" t="s">
-        <v>13</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="C69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D69" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
       <c r="F69" t="s">
         <v>13</v>
       </c>
-      <c r="M69" t="s">
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2840</v>
+      </c>
+      <c r="C70" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2739</v>
+      </c>
+      <c r="F70" t="s">
+        <v>13</v>
+      </c>
+      <c r="M70" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>9</v>
-      </c>
-      <c r="B71" t="s">
-        <v>44</v>
-      </c>
-      <c r="C71" t="s">
-        <v>45</v>
-      </c>
-      <c r="D71" t="s">
-        <v>2740</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>2842</v>
-      </c>
-      <c r="B72" t="s">
-        <v>2742</v>
-      </c>
-      <c r="C72" t="s">
-        <v>46</v>
-      </c>
-      <c r="D72" t="s">
-        <v>2741</v>
-      </c>
-      <c r="F72" t="s">
-        <v>13</v>
-      </c>
-      <c r="G72" t="s">
-        <v>2848</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>2743</v>
+        <v>44</v>
       </c>
       <c r="C73" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D73" t="s">
-        <v>2744</v>
-      </c>
-      <c r="F73" t="s">
-        <v>13</v>
-      </c>
-      <c r="J73" t="s">
-        <v>2854</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>2856</v>
+        <v>2842</v>
       </c>
       <c r="B74" t="s">
-        <v>2841</v>
+        <v>2742</v>
       </c>
       <c r="C74" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D74" t="s">
-        <v>2745</v>
+        <v>2741</v>
       </c>
       <c r="F74" t="s">
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>47</v>
+        <v>2848</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>2857</v>
+        <v>2743</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>2746</v>
+        <v>48</v>
+      </c>
+      <c r="D75" t="s">
+        <v>2744</v>
       </c>
       <c r="F75" t="s">
         <v>13</v>
       </c>
+      <c r="J75" t="s">
+        <v>2854</v>
+      </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>2856</v>
       </c>
       <c r="B76" t="s">
-        <v>2875</v>
+        <v>2841</v>
       </c>
       <c r="C76" t="s">
-        <v>51</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>2747</v>
+        <v>49</v>
+      </c>
+      <c r="D76" t="s">
+        <v>2745</v>
       </c>
       <c r="F76" t="s">
         <v>13</v>
       </c>
-      <c r="J76" t="s">
-        <v>2870</v>
+      <c r="G76" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B77" t="s">
-        <v>2871</v>
+        <v>2857</v>
       </c>
       <c r="C77" t="s">
-        <v>52</v>
-      </c>
-      <c r="D77" t="s">
-        <v>2748</v>
+        <v>50</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>2746</v>
       </c>
       <c r="F77" t="s">
         <v>13</v>
       </c>
-      <c r="G77" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>2872</v>
+        <v>2875</v>
       </c>
       <c r="C78" t="s">
-        <v>54</v>
-      </c>
-      <c r="D78" t="s">
-        <v>2749</v>
+        <v>51</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>2747</v>
       </c>
       <c r="F78" t="s">
         <v>13</v>
       </c>
-      <c r="H78" t="s">
-        <v>184</v>
-      </c>
-      <c r="I78" t="s">
-        <v>55</v>
+      <c r="J78" t="s">
+        <v>2870</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>61</v>
+        <v>183</v>
       </c>
       <c r="B79" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="C79" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D79" t="s">
-        <v>2750</v>
+        <v>2748</v>
       </c>
       <c r="F79" t="s">
         <v>13</v>
       </c>
-      <c r="H79" t="s">
-        <v>184</v>
-      </c>
-      <c r="I79" t="s">
-        <v>58</v>
+      <c r="G79" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B80" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
       <c r="C80" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D80" t="s">
-        <v>2751</v>
+        <v>2749</v>
       </c>
       <c r="F80" t="s">
         <v>13</v>
@@ -11474,80 +11450,89 @@
         <v>184</v>
       </c>
       <c r="I80" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2873</v>
+      </c>
+      <c r="C81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" t="s">
+        <v>2750</v>
+      </c>
+      <c r="F81" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" t="s">
+        <v>184</v>
+      </c>
+      <c r="I81" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>61</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2874</v>
+      </c>
+      <c r="C82" t="s">
+        <v>59</v>
+      </c>
+      <c r="D82" t="s">
+        <v>2751</v>
+      </c>
+      <c r="F82" t="s">
+        <v>13</v>
+      </c>
+      <c r="H82" t="s">
+        <v>184</v>
+      </c>
+      <c r="I82" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>9</v>
-      </c>
-      <c r="B83" t="s">
-        <v>62</v>
-      </c>
-      <c r="C83" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>2886</v>
-      </c>
-      <c r="B84" t="s">
-        <v>2883</v>
-      </c>
-      <c r="C84" t="s">
-        <v>66</v>
-      </c>
-      <c r="D84" t="s">
-        <v>2882</v>
-      </c>
-      <c r="F84" t="s">
-        <v>13</v>
-      </c>
-      <c r="G84" t="s">
-        <v>2887</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>2884</v>
+        <v>62</v>
       </c>
       <c r="C85" t="s">
-        <v>65</v>
-      </c>
-      <c r="D85" t="s">
-        <v>2876</v>
-      </c>
-      <c r="F85" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>34</v>
+        <v>2886</v>
       </c>
       <c r="B86" t="s">
-        <v>2894</v>
+        <v>2883</v>
       </c>
       <c r="C86" t="s">
-        <v>2672</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>2891</v>
+        <v>66</v>
+      </c>
+      <c r="D86" t="s">
+        <v>2882</v>
       </c>
       <c r="F86" t="s">
         <v>13</v>
       </c>
-      <c r="J86" t="s">
-        <v>2895</v>
+      <c r="G86" t="s">
+        <v>2887</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
@@ -11555,48 +11540,36 @@
         <v>64</v>
       </c>
       <c r="B87" t="s">
-        <v>2893</v>
+        <v>2884</v>
       </c>
       <c r="C87" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D87" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="F87" t="s">
         <v>13</v>
       </c>
-      <c r="H87" t="s">
-        <v>2892</v>
-      </c>
-      <c r="I87" t="s">
-        <v>69</v>
-      </c>
-      <c r="J87" t="s">
-        <v>2895</v>
-      </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B88" t="s">
-        <v>2896</v>
+        <v>2894</v>
       </c>
       <c r="C88" t="s">
-        <v>70</v>
-      </c>
-      <c r="D88" t="s">
-        <v>2878</v>
+        <v>2672</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>2891</v>
       </c>
       <c r="F88" t="s">
         <v>13</v>
       </c>
-      <c r="H88" t="s">
-        <v>184</v>
-      </c>
-      <c r="I88" t="s">
-        <v>71</v>
+      <c r="J88" t="s">
+        <v>2895</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -11604,13 +11577,13 @@
         <v>64</v>
       </c>
       <c r="B89" t="s">
-        <v>2897</v>
+        <v>2893</v>
       </c>
       <c r="C89" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D89" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="F89" t="s">
         <v>13</v>
@@ -11619,324 +11592,327 @@
         <v>2892</v>
       </c>
       <c r="I89" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="J89" t="s">
+        <v>2895</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B90" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="C90" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D90" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="F90" t="s">
         <v>13</v>
       </c>
       <c r="H90" t="s">
-        <v>2900</v>
+        <v>184</v>
       </c>
       <c r="I90" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B91" t="s">
-        <v>2899</v>
+        <v>2897</v>
       </c>
       <c r="C91" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D91" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="F91" t="s">
         <v>13</v>
       </c>
       <c r="H91" t="s">
-        <v>185</v>
+        <v>2892</v>
       </c>
       <c r="I91" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>29</v>
+        <v>64</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2898</v>
+      </c>
+      <c r="C92" t="s">
+        <v>74</v>
+      </c>
+      <c r="D92" t="s">
+        <v>2880</v>
+      </c>
+      <c r="F92" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" t="s">
+        <v>2900</v>
+      </c>
+      <c r="I92" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>61</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2899</v>
+      </c>
+      <c r="C93" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" t="s">
+        <v>2881</v>
+      </c>
+      <c r="F93" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" t="s">
+        <v>185</v>
+      </c>
+      <c r="I93" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>3164</v>
-      </c>
-      <c r="B94" t="s">
-        <v>2904</v>
-      </c>
-      <c r="C94" t="s">
-        <v>3199</v>
-      </c>
-      <c r="D94" t="s">
-        <v>2905</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>2907</v>
-      </c>
-      <c r="B95" t="s">
-        <v>2908</v>
-      </c>
-      <c r="C95" t="s">
-        <v>86</v>
-      </c>
-      <c r="D95" t="s">
-        <v>2901</v>
-      </c>
-      <c r="F95" t="s">
-        <v>13</v>
-      </c>
-      <c r="G95" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>64</v>
+        <v>3164</v>
       </c>
       <c r="B96" t="s">
-        <v>2909</v>
+        <v>2904</v>
       </c>
       <c r="C96" t="s">
-        <v>80</v>
+        <v>3199</v>
       </c>
       <c r="D96" t="s">
-        <v>2902</v>
-      </c>
-      <c r="F96" t="s">
-        <v>13</v>
-      </c>
-      <c r="H96" t="s">
-        <v>3200</v>
-      </c>
-      <c r="I96" t="s">
-        <v>3201</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>2907</v>
       </c>
       <c r="B97" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
       <c r="C97" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D97" t="s">
-        <v>2903</v>
+        <v>2901</v>
+      </c>
+      <c r="F97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>3165</v>
+        <v>64</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2909</v>
+      </c>
+      <c r="C98" t="s">
+        <v>80</v>
+      </c>
+      <c r="D98" t="s">
+        <v>2902</v>
+      </c>
+      <c r="F98" t="s">
+        <v>13</v>
+      </c>
+      <c r="H98" t="s">
+        <v>3200</v>
+      </c>
+      <c r="I98" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2910</v>
+      </c>
+      <c r="C99" t="s">
+        <v>83</v>
+      </c>
+      <c r="D99" t="s">
+        <v>2903</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>3164</v>
-      </c>
-      <c r="B100" t="s">
-        <v>2913</v>
-      </c>
-      <c r="C100" t="s">
-        <v>84</v>
-      </c>
-      <c r="D100" t="s">
-        <v>2912</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>2922</v>
-      </c>
-      <c r="B101" t="s">
-        <v>2923</v>
-      </c>
-      <c r="C101" t="s">
-        <v>85</v>
-      </c>
-      <c r="D101" t="s">
-        <v>2911</v>
-      </c>
-      <c r="F101" t="s">
-        <v>13</v>
-      </c>
-      <c r="G101" t="s">
-        <v>16</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>64</v>
+        <v>3164</v>
       </c>
       <c r="B102" t="s">
-        <v>2924</v>
+        <v>2913</v>
       </c>
       <c r="C102" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D102" t="s">
-        <v>2902</v>
-      </c>
-      <c r="F102" t="s">
-        <v>13</v>
-      </c>
-      <c r="H102" t="s">
-        <v>3197</v>
-      </c>
-      <c r="I102" t="s">
-        <v>3198</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>2922</v>
       </c>
       <c r="B103" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="C103" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D103" t="s">
-        <v>2903</v>
+        <v>2911</v>
+      </c>
+      <c r="F103" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>3165</v>
+        <v>64</v>
+      </c>
+      <c r="B104" t="s">
+        <v>2924</v>
+      </c>
+      <c r="C104" t="s">
+        <v>80</v>
+      </c>
+      <c r="D104" t="s">
+        <v>2902</v>
+      </c>
+      <c r="F104" t="s">
+        <v>13</v>
+      </c>
+      <c r="H104" t="s">
+        <v>3197</v>
+      </c>
+      <c r="I104" t="s">
+        <v>3198</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>17</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2925</v>
+      </c>
+      <c r="C105" t="s">
+        <v>83</v>
+      </c>
+      <c r="D105" t="s">
+        <v>2903</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>3164</v>
-      </c>
-      <c r="B106" t="s">
-        <v>2928</v>
-      </c>
-      <c r="C106" t="s">
-        <v>78</v>
-      </c>
-      <c r="D106" t="s">
-        <v>2939</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>2937</v>
-      </c>
-      <c r="B107" t="s">
-        <v>2940</v>
-      </c>
-      <c r="C107" t="s">
-        <v>79</v>
-      </c>
-      <c r="D107" t="s">
-        <v>2926</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>64</v>
+        <v>3164</v>
       </c>
       <c r="B108" t="s">
-        <v>2941</v>
+        <v>2928</v>
       </c>
       <c r="C108" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D108" t="s">
-        <v>2902</v>
-      </c>
-      <c r="F108" t="s">
-        <v>13</v>
-      </c>
-      <c r="H108" t="s">
-        <v>2892</v>
-      </c>
-      <c r="I108" t="s">
-        <v>81</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>2937</v>
       </c>
       <c r="B109" t="s">
-        <v>3187</v>
+        <v>2940</v>
       </c>
       <c r="C109" t="s">
-        <v>3188</v>
+        <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>3189</v>
-      </c>
-      <c r="F109" t="s">
-        <v>13</v>
-      </c>
-      <c r="J109" t="s">
-        <v>2945</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B110" t="s">
-        <v>3186</v>
+        <v>2941</v>
       </c>
       <c r="C110" t="s">
-        <v>3172</v>
+        <v>80</v>
       </c>
       <c r="D110" t="s">
-        <v>3185</v>
+        <v>2902</v>
       </c>
       <c r="F110" t="s">
         <v>13</v>
       </c>
       <c r="H110" t="s">
-        <v>2712</v>
-      </c>
-      <c r="J110" t="s">
-        <v>2945</v>
+        <v>2892</v>
+      </c>
+      <c r="I110" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>2949</v>
+        <v>3187</v>
       </c>
       <c r="C111" t="s">
-        <v>3173</v>
+        <v>3188</v>
       </c>
       <c r="D111" t="s">
-        <v>3169</v>
+        <v>3189</v>
       </c>
       <c r="F111" t="s">
         <v>13</v>
-      </c>
-      <c r="H111" t="s">
-        <v>2712</v>
       </c>
       <c r="J111" t="s">
         <v>2945</v>
@@ -11947,13 +11923,13 @@
         <v>61</v>
       </c>
       <c r="B112" t="s">
-        <v>2950</v>
+        <v>3186</v>
       </c>
       <c r="C112" t="s">
-        <v>3174</v>
+        <v>3172</v>
       </c>
       <c r="D112" t="s">
-        <v>3170</v>
+        <v>3185</v>
       </c>
       <c r="F112" t="s">
         <v>13</v>
@@ -11970,13 +11946,13 @@
         <v>61</v>
       </c>
       <c r="B113" t="s">
-        <v>2951</v>
+        <v>2949</v>
       </c>
       <c r="C113" t="s">
-        <v>3175</v>
+        <v>3173</v>
       </c>
       <c r="D113" t="s">
-        <v>3171</v>
+        <v>3169</v>
       </c>
       <c r="F113" t="s">
         <v>13</v>
@@ -11993,13 +11969,13 @@
         <v>61</v>
       </c>
       <c r="B114" t="s">
-        <v>3179</v>
+        <v>2950</v>
       </c>
       <c r="C114" t="s">
-        <v>3176</v>
+        <v>3174</v>
       </c>
       <c r="D114" t="s">
-        <v>3182</v>
+        <v>3170</v>
       </c>
       <c r="F114" t="s">
         <v>13</v>
@@ -12016,13 +11992,13 @@
         <v>61</v>
       </c>
       <c r="B115" t="s">
-        <v>3180</v>
+        <v>2951</v>
       </c>
       <c r="C115" t="s">
-        <v>3177</v>
+        <v>3175</v>
       </c>
       <c r="D115" t="s">
-        <v>3183</v>
+        <v>3171</v>
       </c>
       <c r="F115" t="s">
         <v>13</v>
@@ -12039,13 +12015,13 @@
         <v>61</v>
       </c>
       <c r="B116" t="s">
-        <v>3181</v>
+        <v>3179</v>
       </c>
       <c r="C116" t="s">
-        <v>3178</v>
+        <v>3176</v>
       </c>
       <c r="D116" t="s">
-        <v>3184</v>
+        <v>3182</v>
       </c>
       <c r="F116" t="s">
         <v>13</v>
@@ -12059,158 +12035,158 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>2952</v>
+        <v>61</v>
       </c>
       <c r="B117" t="s">
-        <v>2948</v>
+        <v>3180</v>
       </c>
       <c r="C117" t="s">
-        <v>82</v>
+        <v>3177</v>
       </c>
       <c r="D117" t="s">
-        <v>2927</v>
+        <v>3183</v>
       </c>
       <c r="F117" t="s">
         <v>13</v>
       </c>
-      <c r="G117" t="s">
-        <v>16</v>
+      <c r="H117" t="s">
+        <v>2712</v>
       </c>
       <c r="J117" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B118" t="s">
-        <v>2946</v>
+        <v>3181</v>
       </c>
       <c r="C118" t="s">
-        <v>83</v>
+        <v>3178</v>
       </c>
       <c r="D118" t="s">
-        <v>2903</v>
+        <v>3184</v>
+      </c>
+      <c r="F118" t="s">
+        <v>13</v>
+      </c>
+      <c r="H118" t="s">
+        <v>2712</v>
+      </c>
+      <c r="J118" t="s">
+        <v>2945</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>3165</v>
+        <v>2952</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2948</v>
+      </c>
+      <c r="C119" t="s">
+        <v>82</v>
+      </c>
+      <c r="D119" t="s">
+        <v>2927</v>
+      </c>
+      <c r="F119" t="s">
+        <v>13</v>
+      </c>
+      <c r="G119" t="s">
+        <v>16</v>
+      </c>
+      <c r="J119" t="s">
+        <v>2947</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A120" s="3"/>
+      <c r="A120" t="s">
+        <v>17</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2946</v>
+      </c>
+      <c r="C120" t="s">
+        <v>83</v>
+      </c>
+      <c r="D120" t="s">
+        <v>2903</v>
+      </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>3164</v>
-      </c>
-      <c r="B121" t="s">
-        <v>2957</v>
-      </c>
-      <c r="C121" t="s">
-        <v>2674</v>
-      </c>
-      <c r="D121" t="s">
-        <v>2958</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>2964</v>
-      </c>
-      <c r="B122" t="s">
-        <v>2959</v>
-      </c>
-      <c r="C122" t="s">
-        <v>2675</v>
-      </c>
-      <c r="D122" t="s">
-        <v>2960</v>
-      </c>
+      <c r="A122" s="3"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>64</v>
+        <v>3164</v>
       </c>
       <c r="B123" t="s">
-        <v>2969</v>
+        <v>2957</v>
       </c>
       <c r="C123" t="s">
-        <v>80</v>
+        <v>2674</v>
       </c>
       <c r="D123" t="s">
-        <v>2902</v>
-      </c>
-      <c r="F123" t="s">
-        <v>13</v>
-      </c>
-      <c r="H123" t="s">
-        <v>2892</v>
-      </c>
-      <c r="I123" t="s">
-        <v>81</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>2976</v>
+        <v>2964</v>
       </c>
       <c r="B124" t="s">
-        <v>3025</v>
+        <v>2959</v>
       </c>
       <c r="C124" t="s">
-        <v>2713</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>2961</v>
-      </c>
-      <c r="F124" t="s">
-        <v>13</v>
-      </c>
-      <c r="G124" t="s">
-        <v>16</v>
-      </c>
-      <c r="J124" t="s">
-        <v>3010</v>
+        <v>2675</v>
+      </c>
+      <c r="D124" t="s">
+        <v>2960</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>3015</v>
+        <v>64</v>
       </c>
       <c r="B125" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="C125" t="s">
-        <v>2687</v>
+        <v>80</v>
       </c>
       <c r="D125" t="s">
-        <v>2962</v>
+        <v>2902</v>
       </c>
       <c r="F125" t="s">
         <v>13</v>
       </c>
-      <c r="G125" t="s">
-        <v>16</v>
-      </c>
-      <c r="J125" t="s">
-        <v>3011</v>
+      <c r="H125" t="s">
+        <v>2892</v>
+      </c>
+      <c r="I125" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>3022</v>
+        <v>2976</v>
       </c>
       <c r="B126" t="s">
-        <v>2984</v>
+        <v>3025</v>
       </c>
       <c r="C126" t="s">
-        <v>2714</v>
-      </c>
-      <c r="D126" t="s">
-        <v>2963</v>
+        <v>2713</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>2961</v>
       </c>
       <c r="F126" t="s">
         <v>13</v>
@@ -12219,163 +12195,163 @@
         <v>16</v>
       </c>
       <c r="J126" t="s">
-        <v>3012</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>3015</v>
       </c>
       <c r="B127" t="s">
-        <v>2991</v>
+        <v>2970</v>
       </c>
       <c r="C127" t="s">
-        <v>83</v>
+        <v>2687</v>
       </c>
       <c r="D127" t="s">
-        <v>2903</v>
+        <v>2962</v>
+      </c>
+      <c r="F127" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" t="s">
+        <v>16</v>
+      </c>
+      <c r="J127" t="s">
+        <v>3011</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>3165</v>
+        <v>3022</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2984</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2714</v>
+      </c>
+      <c r="D128" t="s">
+        <v>2963</v>
+      </c>
+      <c r="F128" t="s">
+        <v>13</v>
+      </c>
+      <c r="G128" t="s">
+        <v>16</v>
+      </c>
+      <c r="J128" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>17</v>
+      </c>
+      <c r="B129" t="s">
+        <v>2991</v>
+      </c>
+      <c r="C129" t="s">
+        <v>83</v>
+      </c>
+      <c r="D129" t="s">
+        <v>2903</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>3164</v>
-      </c>
-      <c r="B130" t="s">
-        <v>3001</v>
-      </c>
-      <c r="C130" t="s">
-        <v>87</v>
-      </c>
-      <c r="D130" t="s">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>3003</v>
-      </c>
-      <c r="B131" t="s">
-        <v>3002</v>
-      </c>
-      <c r="C131" t="s">
-        <v>88</v>
-      </c>
-      <c r="D131" t="s">
-        <v>2992</v>
-      </c>
-      <c r="F131" t="s">
-        <v>13</v>
-      </c>
-      <c r="G131" t="s">
-        <v>16</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>64</v>
+        <v>3164</v>
       </c>
       <c r="B132" t="s">
-        <v>3005</v>
+        <v>3001</v>
       </c>
       <c r="C132" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D132" t="s">
-        <v>2902</v>
-      </c>
-      <c r="F132" t="s">
-        <v>13</v>
-      </c>
-      <c r="H132" t="s">
-        <v>2892</v>
-      </c>
-      <c r="I132" t="s">
-        <v>81</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>3007</v>
+        <v>3003</v>
       </c>
       <c r="B133" t="s">
-        <v>3013</v>
+        <v>3002</v>
       </c>
       <c r="C133" t="s">
-        <v>2697</v>
+        <v>88</v>
       </c>
       <c r="D133" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="F133" t="s">
         <v>13</v>
       </c>
-      <c r="G133" s="2" t="s">
+      <c r="G133" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>3016</v>
+        <v>64</v>
       </c>
       <c r="B134" t="s">
-        <v>3014</v>
+        <v>3005</v>
       </c>
       <c r="C134" t="s">
-        <v>2687</v>
+        <v>80</v>
       </c>
       <c r="D134" t="s">
-        <v>2994</v>
+        <v>2902</v>
       </c>
       <c r="F134" t="s">
         <v>13</v>
       </c>
-      <c r="G134" t="s">
-        <v>16</v>
-      </c>
-      <c r="J134" t="s">
-        <v>3027</v>
+      <c r="H134" t="s">
+        <v>2892</v>
+      </c>
+      <c r="I134" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>3018</v>
+        <v>3007</v>
       </c>
       <c r="B135" t="s">
-        <v>3020</v>
+        <v>3013</v>
       </c>
       <c r="C135" t="s">
-        <v>89</v>
+        <v>2697</v>
       </c>
       <c r="D135" t="s">
-        <v>2995</v>
+        <v>2993</v>
       </c>
       <c r="F135" t="s">
         <v>13</v>
       </c>
-      <c r="G135" t="s">
+      <c r="G135" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J135" t="s">
-        <v>3027</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>3023</v>
+        <v>3016</v>
       </c>
       <c r="B136" t="s">
-        <v>3021</v>
+        <v>3014</v>
       </c>
       <c r="C136" t="s">
-        <v>2699</v>
+        <v>2687</v>
       </c>
       <c r="D136" t="s">
-        <v>2996</v>
+        <v>2994</v>
       </c>
       <c r="F136" t="s">
         <v>13</v>
@@ -12384,21 +12360,21 @@
         <v>16</v>
       </c>
       <c r="J136" t="s">
-        <v>3026</v>
+        <v>3027</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>3029</v>
+        <v>3018</v>
       </c>
       <c r="B137" t="s">
-        <v>3030</v>
+        <v>3020</v>
       </c>
       <c r="C137" t="s">
-        <v>2693</v>
+        <v>89</v>
       </c>
       <c r="D137" t="s">
-        <v>2997</v>
+        <v>2995</v>
       </c>
       <c r="F137" t="s">
         <v>13</v>
@@ -12407,21 +12383,21 @@
         <v>16</v>
       </c>
       <c r="J137" t="s">
-        <v>3028</v>
+        <v>3027</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>3032</v>
+        <v>3023</v>
       </c>
       <c r="B138" t="s">
-        <v>3031</v>
+        <v>3021</v>
       </c>
       <c r="C138" t="s">
-        <v>90</v>
+        <v>2699</v>
       </c>
       <c r="D138" t="s">
-        <v>2998</v>
+        <v>2996</v>
       </c>
       <c r="F138" t="s">
         <v>13</v>
@@ -12430,27 +12406,27 @@
         <v>16</v>
       </c>
       <c r="J138" t="s">
-        <v>3028</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>183</v>
+        <v>3029</v>
       </c>
       <c r="B139" t="s">
-        <v>3037</v>
+        <v>3030</v>
       </c>
       <c r="C139" t="s">
-        <v>2696</v>
+        <v>2693</v>
       </c>
       <c r="D139" t="s">
-        <v>2999</v>
+        <v>2997</v>
       </c>
       <c r="F139" t="s">
         <v>13</v>
       </c>
       <c r="G139" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="J139" t="s">
         <v>3028</v>
@@ -12458,166 +12434,169 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>3032</v>
       </c>
       <c r="B140" t="s">
-        <v>3006</v>
+        <v>3031</v>
       </c>
       <c r="C140" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D140" t="s">
-        <v>2903</v>
+        <v>2998</v>
+      </c>
+      <c r="F140" t="s">
+        <v>13</v>
+      </c>
+      <c r="G140" t="s">
+        <v>16</v>
+      </c>
+      <c r="J140" t="s">
+        <v>3028</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>3165</v>
+        <v>183</v>
+      </c>
+      <c r="B141" t="s">
+        <v>3037</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2696</v>
+      </c>
+      <c r="D141" t="s">
+        <v>2999</v>
+      </c>
+      <c r="F141" t="s">
+        <v>13</v>
+      </c>
+      <c r="G141" t="s">
+        <v>56</v>
+      </c>
+      <c r="J141" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>17</v>
+      </c>
+      <c r="B142" t="s">
+        <v>3006</v>
+      </c>
+      <c r="C142" t="s">
+        <v>83</v>
+      </c>
+      <c r="D142" t="s">
+        <v>2903</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>9</v>
-      </c>
-      <c r="B143" t="s">
-        <v>91</v>
-      </c>
-      <c r="C143" t="s">
-        <v>92</v>
-      </c>
-      <c r="D143" t="s">
-        <v>3040</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>64</v>
-      </c>
-      <c r="B144" t="s">
-        <v>3041</v>
-      </c>
-      <c r="C144" t="s">
-        <v>93</v>
-      </c>
-      <c r="D144" t="s">
-        <v>3039</v>
-      </c>
-      <c r="F144" t="s">
-        <v>13</v>
-      </c>
-      <c r="H144" t="s">
-        <v>2892</v>
-      </c>
-      <c r="I144" t="s">
-        <v>94</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B145" t="s">
-        <v>3042</v>
+        <v>91</v>
       </c>
       <c r="C145" t="s">
-        <v>3043</v>
+        <v>92</v>
       </c>
       <c r="D145" t="s">
-        <v>3044</v>
-      </c>
-      <c r="F145" t="s">
-        <v>13</v>
-      </c>
-      <c r="H145" t="s">
-        <v>185</v>
-      </c>
-      <c r="I145" t="s">
-        <v>186</v>
+        <v>3040</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>196</v>
+        <v>64</v>
       </c>
       <c r="B146" t="s">
-        <v>3046</v>
-      </c>
-      <c r="K146" t="s">
-        <v>3045</v>
+        <v>3041</v>
+      </c>
+      <c r="C146" t="s">
+        <v>93</v>
+      </c>
+      <c r="D146" t="s">
+        <v>3039</v>
+      </c>
+      <c r="F146" t="s">
+        <v>13</v>
+      </c>
+      <c r="H146" t="s">
+        <v>2892</v>
+      </c>
+      <c r="I146" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>206</v>
+        <v>61</v>
       </c>
       <c r="B147" t="s">
-        <v>3085</v>
+        <v>3042</v>
       </c>
       <c r="C147" t="s">
-        <v>3047</v>
+        <v>3043</v>
+      </c>
+      <c r="D147" t="s">
+        <v>3044</v>
+      </c>
+      <c r="F147" t="s">
+        <v>13</v>
+      </c>
+      <c r="H147" t="s">
+        <v>185</v>
+      </c>
+      <c r="I147" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>3050</v>
+        <v>196</v>
       </c>
       <c r="B148" t="s">
-        <v>3048</v>
-      </c>
-      <c r="C148" t="s">
-        <v>95</v>
-      </c>
-      <c r="D148" t="s">
-        <v>3049</v>
-      </c>
-      <c r="F148" t="s">
-        <v>13</v>
-      </c>
-      <c r="G148" t="s">
-        <v>16</v>
+        <v>3046</v>
+      </c>
+      <c r="K148" t="s">
+        <v>3045</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>61</v>
+        <v>206</v>
       </c>
       <c r="B149" t="s">
-        <v>3054</v>
+        <v>3085</v>
       </c>
       <c r="C149" t="s">
-        <v>96</v>
-      </c>
-      <c r="D149" t="s">
-        <v>3053</v>
-      </c>
-      <c r="F149" t="s">
-        <v>13</v>
-      </c>
-      <c r="H149" t="s">
-        <v>184</v>
-      </c>
-      <c r="I149" t="s">
-        <v>97</v>
+        <v>3047</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>3056</v>
+        <v>3050</v>
       </c>
       <c r="B150" t="s">
-        <v>3062</v>
+        <v>3048</v>
       </c>
       <c r="C150" t="s">
-        <v>205</v>
+        <v>95</v>
       </c>
       <c r="D150" t="s">
-        <v>3055</v>
+        <v>3049</v>
       </c>
       <c r="F150" t="s">
         <v>13</v>
       </c>
       <c r="G150" t="s">
-        <v>199</v>
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.3">
@@ -12625,13 +12604,13 @@
         <v>61</v>
       </c>
       <c r="B151" t="s">
-        <v>3059</v>
+        <v>3054</v>
       </c>
       <c r="C151" t="s">
-        <v>3065</v>
+        <v>96</v>
       </c>
       <c r="D151" t="s">
-        <v>3058</v>
+        <v>3053</v>
       </c>
       <c r="F151" t="s">
         <v>13</v>
@@ -12640,27 +12619,27 @@
         <v>184</v>
       </c>
       <c r="I151" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>3069</v>
+        <v>3056</v>
       </c>
       <c r="B152" t="s">
-        <v>3061</v>
+        <v>3062</v>
       </c>
       <c r="C152" t="s">
-        <v>99</v>
+        <v>205</v>
       </c>
       <c r="D152" t="s">
-        <v>3060</v>
+        <v>3055</v>
       </c>
       <c r="F152" t="s">
         <v>13</v>
       </c>
       <c r="G152" t="s">
-        <v>157</v>
+        <v>199</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.3">
@@ -12668,13 +12647,13 @@
         <v>61</v>
       </c>
       <c r="B153" t="s">
-        <v>3063</v>
+        <v>3059</v>
       </c>
       <c r="C153" t="s">
-        <v>3066</v>
+        <v>3065</v>
       </c>
       <c r="D153" t="s">
-        <v>3064</v>
+        <v>3058</v>
       </c>
       <c r="F153" t="s">
         <v>13</v>
@@ -12683,186 +12662,183 @@
         <v>184</v>
       </c>
       <c r="I153" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>3072</v>
+        <v>3069</v>
       </c>
       <c r="B154" t="s">
-        <v>3067</v>
+        <v>3061</v>
       </c>
       <c r="C154" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D154" t="s">
-        <v>3068</v>
+        <v>3060</v>
       </c>
       <c r="F154" t="s">
         <v>13</v>
       </c>
+      <c r="G154" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="B155" t="s">
-        <v>3076</v>
+        <v>3063</v>
       </c>
       <c r="C155" t="s">
-        <v>2701</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>3073</v>
+        <v>3066</v>
+      </c>
+      <c r="D155" t="s">
+        <v>3064</v>
       </c>
       <c r="F155" t="s">
         <v>13</v>
       </c>
-      <c r="G155" t="s">
-        <v>56</v>
+      <c r="H155" t="s">
+        <v>184</v>
+      </c>
+      <c r="I155" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>61</v>
+        <v>3072</v>
       </c>
       <c r="B156" t="s">
-        <v>3077</v>
+        <v>3067</v>
       </c>
       <c r="C156" t="s">
-        <v>2702</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>3074</v>
+        <v>101</v>
+      </c>
+      <c r="D156" t="s">
+        <v>3068</v>
       </c>
       <c r="F156" t="s">
         <v>13</v>
       </c>
-      <c r="J156" t="s">
-        <v>3084</v>
-      </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>3079</v>
+        <v>183</v>
       </c>
       <c r="B157" t="s">
-        <v>3078</v>
+        <v>3076</v>
       </c>
       <c r="C157" t="s">
-        <v>2706</v>
+        <v>2701</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>3075</v>
+        <v>3073</v>
       </c>
       <c r="F157" t="s">
         <v>13</v>
       </c>
-      <c r="J157" t="s">
-        <v>3084</v>
+      <c r="G157" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="B158" t="s">
+        <v>3077</v>
+      </c>
+      <c r="C158" t="s">
+        <v>2702</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>3074</v>
+      </c>
+      <c r="F158" t="s">
+        <v>13</v>
+      </c>
+      <c r="J158" t="s">
+        <v>3084</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>3079</v>
+      </c>
+      <c r="B159" t="s">
+        <v>3078</v>
+      </c>
+      <c r="C159" t="s">
+        <v>2706</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>3075</v>
+      </c>
+      <c r="F159" t="s">
+        <v>13</v>
+      </c>
+      <c r="J159" t="s">
+        <v>3084</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>9</v>
-      </c>
-      <c r="B160" t="s">
-        <v>102</v>
-      </c>
-      <c r="C160" t="s">
-        <v>103</v>
-      </c>
-      <c r="D160" t="s">
-        <v>3088</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>183</v>
-      </c>
-      <c r="B161" t="s">
-        <v>3086</v>
-      </c>
-      <c r="C161" t="s">
-        <v>104</v>
-      </c>
-      <c r="D161" t="s">
-        <v>3094</v>
-      </c>
-      <c r="F161" t="s">
-        <v>13</v>
-      </c>
-      <c r="G161" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>3090</v>
+        <v>9</v>
       </c>
       <c r="B162" t="s">
-        <v>3087</v>
+        <v>102</v>
       </c>
       <c r="C162" t="s">
-        <v>2711</v>
+        <v>103</v>
       </c>
       <c r="D162" t="s">
-        <v>3095</v>
-      </c>
-      <c r="F162" t="s">
-        <v>13</v>
-      </c>
-      <c r="J162" t="s">
-        <v>3089</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
       <c r="B163" t="s">
-        <v>3196</v>
+        <v>3086</v>
       </c>
       <c r="C163" t="s">
-        <v>3190</v>
+        <v>104</v>
       </c>
       <c r="D163" t="s">
-        <v>3191</v>
+        <v>3094</v>
       </c>
       <c r="F163" t="s">
         <v>13</v>
       </c>
-      <c r="H163" t="s">
-        <v>2712</v>
-      </c>
-      <c r="I163" t="s">
-        <v>3195</v>
-      </c>
-      <c r="J163" t="s">
-        <v>3089</v>
+      <c r="G163" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>61</v>
+        <v>3090</v>
       </c>
       <c r="B164" t="s">
-        <v>3194</v>
+        <v>3087</v>
       </c>
       <c r="C164" t="s">
-        <v>3192</v>
+        <v>2711</v>
       </c>
       <c r="D164" t="s">
-        <v>3193</v>
-      </c>
-      <c r="H164" t="s">
-        <v>2712</v>
+        <v>3095</v>
+      </c>
+      <c r="F164" t="s">
+        <v>13</v>
       </c>
       <c r="J164" t="s">
         <v>3089</v>
@@ -12870,11 +12846,57 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="B165" t="s">
+        <v>3196</v>
+      </c>
+      <c r="C165" t="s">
+        <v>3190</v>
+      </c>
+      <c r="D165" t="s">
+        <v>3191</v>
+      </c>
+      <c r="F165" t="s">
+        <v>13</v>
+      </c>
+      <c r="H165" t="s">
+        <v>2712</v>
+      </c>
+      <c r="I165" t="s">
+        <v>3195</v>
+      </c>
+      <c r="J165" t="s">
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>61</v>
+      </c>
+      <c r="B166" t="s">
+        <v>3194</v>
+      </c>
+      <c r="C166" t="s">
+        <v>3192</v>
+      </c>
+      <c r="D166" t="s">
+        <v>3193</v>
+      </c>
+      <c r="H166" t="s">
+        <v>2712</v>
+      </c>
+      <c r="J166" t="s">
+        <v>3089</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
         <v>3165</v>
       </c>
     </row>
@@ -40753,9 +40775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -40797,7 +40819,7 @@
         <v>3163</v>
       </c>
       <c r="F2" s="1">
-        <v>20190225</v>
+        <v>20191118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>